<commit_message>
Changed Residual Anomalies document for BlueLib Android
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310193817/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310193817/Development/Git/Android-ShineLib/Documents/External/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="689" activeTab="5"/>
+    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="689" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -43,10 +43,10 @@
     <definedName name="ListYN" localSheetId="5">#REF!</definedName>
     <definedName name="ListYN" localSheetId="4">#REF!</definedName>
     <definedName name="ListYN">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Anomalies!$A$1:$H$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">Anomalies!$A$1:$G$37</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Document Introduction'!$A$1:$G$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Introduction!$A$1:$M$20</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">'Maturity Grid'!$A$1:$E$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Maturity Grid'!$A$1:$E$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'Revision History'!$A$1:$G$23</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Title Page'!$A$1:$G$19</definedName>
     <definedName name="SORT" localSheetId="5">#REF!</definedName>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="99">
   <si>
     <t>1.1</t>
   </si>
@@ -136,12 +136,6 @@
   </si>
   <si>
     <t>Repository</t>
-  </si>
-  <si>
-    <t>&lt;John Doe&gt;</t>
-  </si>
-  <si>
-    <t>&lt;Product architect&gt;</t>
   </si>
   <si>
     <t>&lt;state document archive&gt;</t>
@@ -181,9 +175,6 @@
     <t xml:space="preserve">Template ID:  </t>
   </si>
   <si>
-    <t>&lt;approver name&gt;</t>
-  </si>
-  <si>
     <t>Term</t>
   </si>
   <si>
@@ -191,15 +182,6 @@
   </si>
   <si>
     <t>Introduction</t>
-  </si>
-  <si>
-    <t>Workaround</t>
-  </si>
-  <si>
-    <t>Impact on device performance</t>
-  </si>
-  <si>
-    <t>To be solved?</t>
   </si>
   <si>
     <t>Severity</t>
@@ -245,40 +227,10 @@
     </r>
   </si>
   <si>
-    <t>Defect id</t>
-  </si>
-  <si>
-    <t>Problem description</t>
-  </si>
-  <si>
     <t>The list of residual anomalies can be found in tab "Anomalies". An overview is shown below.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Conclusion: </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>&lt;no residual anomalies for &lt;(medical device) software name&gt;&gt; .</t>
-    </r>
-  </si>
-  <si>
     <t>BMS-REA-719, v1.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;
-Before submitting a document for approval make sure all changes are accepted/rejected and all comments are deleted.
-This document shall be approved by E signature according local document management system or by signing the table below. 
-In case of E-signature state:  
-Approved by E-signature in local document management system
-&gt;
-</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -373,6 +325,111 @@
     <t>BG-208</t>
   </si>
   <si>
+    <t>BG-22</t>
+  </si>
+  <si>
+    <t>Association with LifeSense BPM can fail unexpectedly on some Android combos</t>
+  </si>
+  <si>
+    <t>BG-158</t>
+  </si>
+  <si>
+    <t>BG-241</t>
+  </si>
+  <si>
+    <t>BG-88</t>
+  </si>
+  <si>
+    <t>Crash , associating when bluetooth turned off</t>
+  </si>
+  <si>
+    <t>BG-246</t>
+  </si>
+  <si>
+    <t>BG-296</t>
+  </si>
+  <si>
+    <t>BG-238</t>
+  </si>
+  <si>
+    <t>Crash during association</t>
+  </si>
+  <si>
+    <t>Thijs Winter</t>
+  </si>
+  <si>
+    <t>Domain leader conenctivity</t>
+  </si>
+  <si>
+    <t>Blocker</t>
+  </si>
+  <si>
+    <t>Critical</t>
+  </si>
+  <si>
+    <t>Major</t>
+  </si>
+  <si>
+    <t>Minor</t>
+  </si>
+  <si>
+    <t>Trivial</t>
+  </si>
+  <si>
+    <t>Blocks development and/or testing work, production could not run.</t>
+  </si>
+  <si>
+    <t>Crashes, loss of data, severe memory leak.</t>
+  </si>
+  <si>
+    <t>Major loss of function.</t>
+  </si>
+  <si>
+    <t>Minor loss of function, or other problem where easy workaround is present.</t>
+  </si>
+  <si>
+    <t>Cosmetic problem like misspelt words or misaligned text.</t>
+  </si>
+  <si>
+    <t>Key</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Created</t>
+  </si>
+  <si>
+    <t>[Android] Random Crash observed while syncing in samsung android device</t>
+  </si>
+  <si>
+    <t>Bug 30721:Moonshine pairing fails</t>
+  </si>
+  <si>
+    <t>BG-95</t>
+  </si>
+  <si>
+    <t>SHNDeviceImpl should actively disconnect when not all expected services are discovered</t>
+  </si>
+  <si>
+    <t>BG-145</t>
+  </si>
+  <si>
+    <t>Regression in association with thermometer</t>
+  </si>
+  <si>
+    <t>Bug 30096:[Android] Sync error observed in dashboard screen.</t>
+  </si>
+  <si>
+    <t>[Moonshine] [Bug#656] Moonshine pairing issues with Android phones</t>
+  </si>
+  <si>
+    <t>[Moonshot] TFS 32433 - Scale pairing issue Nexus [Support only]</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">This list of residual anomalies for </t>
     </r>
@@ -390,8 +447,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> is generated from the defect tracking database. See table below for an explanation of defect severities.
-The tab "Maturity Grid" gives an overview of the amount of residual anomalies per defect severity. The tab "Anomalies" gives an overview of the anomalous behavior and proposed workaround (when available).
+      <t xml:space="preserve"> is generated from the defect tracking database. The defet severity is decided in an analysis session where the defect is judged on the occurrence rate, its effect on application stability, possiblity of data loss, ability to recover from the defect and market share of phone on which the defect occurs. See the table below for the explanation of defect severities.
+The tab "Maturity Grid" gives an overview of the amount of residual anomalies per defect severity. The tab "Anomalies" gives an overview of the anomalous behavior.
 </t>
     </r>
     <r>
@@ -406,95 +463,26 @@
     </r>
   </si>
   <si>
-    <t>Unacceptable defect</t>
-  </si>
-  <si>
-    <t>Device will crash but after restart will continue to function</t>
-  </si>
-  <si>
-    <t>in future release</t>
-  </si>
-  <si>
-    <t>No workaround</t>
-  </si>
-  <si>
-    <t>BG-22</t>
-  </si>
-  <si>
-    <t>Association with LifeSense BPM can fail unexpectedly on some Android combos</t>
-  </si>
-  <si>
-    <t>BG-158</t>
-  </si>
-  <si>
-    <t>BG-283</t>
-  </si>
-  <si>
-    <t>BG-241</t>
-  </si>
-  <si>
-    <t>BG-209</t>
-  </si>
-  <si>
-    <t>Upperarm BPM doesn't sync with app</t>
-  </si>
-  <si>
-    <t>BG-88</t>
-  </si>
-  <si>
-    <t>Crash , associating when bluetooth turned off</t>
-  </si>
-  <si>
-    <t>BG-246</t>
-  </si>
-  <si>
-    <t>Requires multiple retries to get the device working</t>
-  </si>
-  <si>
-    <t>Undesirable Defect</t>
-  </si>
-  <si>
-    <t>BG-296</t>
-  </si>
-  <si>
-    <t>BG-238</t>
-  </si>
-  <si>
-    <t>Crash during association</t>
-  </si>
-  <si>
-    <t>Random Crash observed while syncing in samsung android device</t>
-  </si>
-  <si>
-    <t>Moonshine pairing issues with Android phones</t>
-  </si>
-  <si>
-    <t>Sync error observed in dashboard screen.</t>
-  </si>
-  <si>
-    <t>Moonshine pairing fails</t>
-  </si>
-  <si>
-    <t>Scale pairing issue Nexus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Association with the device is not possible with some phones. </t>
-  </si>
-  <si>
-    <t>Unacceptable Safety Defect</t>
-  </si>
-  <si>
-    <t>Unacceptable Defect</t>
-  </si>
-  <si>
-    <t>Minor Defect</t>
+    <t>Conclusion: The build cannot be released to clients due to 1 critical and 8 major  defects.</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>2016-JUL-14</t>
+  </si>
+  <si>
+    <t>Changed severity classification</t>
+  </si>
+  <si>
+    <t>Review comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="41" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -601,13 +589,6 @@
     </font>
     <font>
       <i/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
@@ -663,12 +644,6 @@
       <b/>
       <sz val="12"/>
       <color indexed="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -742,8 +717,40 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -758,18 +765,42 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="22"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -845,15 +876,149 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
       </left>
       <right/>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color auto="1"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -863,9 +1028,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -911,19 +1076,19 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -935,16 +1100,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -960,7 +1125,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -971,12 +1136,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -985,20 +1144,14 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1007,7 +1160,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1016,46 +1169,30 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="36" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="36" fillId="4" borderId="5" xfId="4" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="22" fontId="1" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1072,19 +1209,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -1096,13 +1233,45 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="35" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="22" fontId="1" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -1332,44 +1501,6 @@
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>488092</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>1727</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Picture 3"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="1958340"/>
-          <a:ext cx="4755292" cy="2341067"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -1445,6 +1576,256 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4097" name="AutoShape 1" descr="https://atlas.natlab.research.philips.com/jira/images/icons/priorities/blocker.svg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="2959100"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4098" name="AutoShape 2" descr="https://atlas.natlab.research.philips.com/jira/images/icons/priorities/critical.svg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="3416300"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4099" name="AutoShape 3" descr="https://atlas.natlab.research.philips.com/jira/images/icons/priorities/major.svg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="3873500"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4100" name="AutoShape 4" descr="https://atlas.natlab.research.philips.com/jira/images/icons/priorities/minor.svg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="4330700"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4101" name="AutoShape 5" descr="https://atlas.natlab.research.philips.com/jira/images/icons/priorities/trivial.svg"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="1409700" y="4787900"/>
+          <a:ext cx="152400" cy="152400"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1980,8 +2361,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="110" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="110" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1997,10 +2378,10 @@
   <sheetData>
     <row r="1" spans="1:7" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>54</v>
-      </c>
-      <c r="B1" s="67" t="s">
-        <v>55</v>
+        <v>44</v>
+      </c>
+      <c r="B1" s="63" t="s">
+        <v>45</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2010,7 +2391,7 @@
     <row r="2" spans="1:7" ht="28" x14ac:dyDescent="0.2">
       <c r="D2" s="4"/>
       <c r="E2" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="33" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2031,13 +2412,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="79" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2047,27 +2426,27 @@
       <c r="C7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="63" t="s">
+      <c r="D7" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="63" t="s">
+      <c r="E7" s="59" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="22"/>
       <c r="G7" s="23"/>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="29" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>25</v>
+      <c r="B8" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8" s="35" t="s">
+        <v>69</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="29" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
@@ -2100,72 +2479,72 @@
       <c r="B12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12" s="80" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="80"/>
+      <c r="C12" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="D12" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="70"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="68" t="s">
-        <v>60</v>
+      <c r="G12" s="64" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="68" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="81" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="81"/>
+      <c r="C13" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="71"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="68" t="s">
-        <v>61</v>
+      <c r="G13" s="64" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B14" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="D14" s="81"/>
-      <c r="E14" s="81"/>
+      <c r="C14" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="D14" s="71"/>
+      <c r="E14" s="71"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>38</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="68" t="s">
-        <v>57</v>
+      <c r="C15" s="64" t="s">
+        <v>47</v>
       </c>
       <c r="D15" s="28" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E15" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="64" t="s">
-        <v>28</v>
-      </c>
-      <c r="G15" s="65" t="s">
-        <v>29</v>
+        <v>43</v>
+      </c>
+      <c r="F15" s="60" t="s">
+        <v>26</v>
+      </c>
+      <c r="G15" s="61" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2190,12 +2569,12 @@
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="D13:E14"/>
   </mergeCells>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="1.2598425196850394" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="72" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.1&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -2213,8 +2592,8 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A12" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView view="pageLayout" topLeftCell="A6" zoomScale="99" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2229,8 +2608,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="67" t="s">
-        <v>55</v>
+      <c r="B1" s="63" t="s">
+        <v>45</v>
       </c>
       <c r="C1" s="6"/>
       <c r="E1" s="6"/>
@@ -2239,7 +2618,7 @@
     <row r="2" spans="2:6" ht="28" x14ac:dyDescent="0.2">
       <c r="C2" s="4"/>
       <c r="D2" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
@@ -2249,7 +2628,7 @@
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B4" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3"/>
     </row>
@@ -2264,11 +2643,11 @@
       <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="88" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="89"/>
-      <c r="F6" s="90"/>
+      <c r="D6" s="78" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="79"/>
+      <c r="F6" s="80"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
@@ -2277,13 +2656,13 @@
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="91" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="91"/>
-      <c r="F7" s="91"/>
-    </row>
-    <row r="8" spans="2:6" ht="198" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="D7" s="81" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+    </row>
+    <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
         <v>4</v>
       </c>
@@ -2291,19 +2670,19 @@
         <v>5</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="E8" s="59" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="66" t="s">
+      <c r="F8" s="62" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="33"/>
-      <c r="C9" s="69" t="s">
-        <v>65</v>
+      <c r="C9" s="65" t="s">
+        <v>55</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -2330,69 +2709,69 @@
       <c r="C12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="60" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="92" t="s">
+      <c r="D12" s="56" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="82" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="92"/>
+      <c r="F12" s="82"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
-      <c r="D13" s="52" t="s">
-        <v>46</v>
-      </c>
-      <c r="E13" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="83"/>
+      <c r="D13" s="50" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="72" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="73"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
       <c r="C14" s="31"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="85"/>
+      <c r="E14" s="74"/>
+      <c r="F14" s="75"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
       <c r="C15" s="10"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="61"/>
-      <c r="F15" s="62"/>
+      <c r="E15" s="57"/>
+      <c r="F15" s="58"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="77"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="55"/>
+      <c r="A19" s="51"/>
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="55"/>
+      <c r="A20" s="51"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="55"/>
+      <c r="A21" s="51"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="55"/>
+      <c r="A22" s="51"/>
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="55"/>
+      <c r="A23" s="51"/>
       <c r="B23" s="3"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="55"/>
+      <c r="A24" s="51"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="55"/>
+      <c r="A25" s="51"/>
     </row>
     <row r="28" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
@@ -2424,12 +2803,12 @@
     <mergeCell ref="D7:F7"/>
     <mergeCell ref="E12:F12"/>
   </mergeCells>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
   <pageSetup paperSize="9" scale="63" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.1&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -2447,8 +2826,8 @@
   </sheetPr>
   <dimension ref="B1:N179"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2463,8 +2842,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
-        <v>55</v>
+      <c r="B1" s="66" t="s">
+        <v>45</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2490,7 +2869,7 @@
     </row>
     <row r="4" spans="2:14" ht="18" x14ac:dyDescent="0.15">
       <c r="B4" s="5" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
@@ -2522,19 +2901,19 @@
     </row>
     <row r="6" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B6" s="34" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="34" t="s">
+        <v>31</v>
+      </c>
+      <c r="E6" s="34" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="34" t="s">
         <v>34</v>
-      </c>
-      <c r="C6" s="34" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" s="34" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="F6" s="34" t="s">
-        <v>36</v>
       </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
@@ -2546,20 +2925,20 @@
       <c r="N6" s="17"/>
     </row>
     <row r="7" spans="2:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B7" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" s="68" t="s">
+      <c r="B7" s="64" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" s="64" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="D7" s="68" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="68" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" s="68" t="s">
-        <v>66</v>
+      <c r="F7" s="64" t="s">
+        <v>56</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -2571,11 +2950,21 @@
       <c r="N7" s="17"/>
     </row>
     <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
+      <c r="B8" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="64" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>98</v>
+      </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
       <c r="I8" s="17"/>
@@ -5152,12 +5541,12 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.1&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -5172,15 +5561,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AK26"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A13" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView view="pageLayout" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="6" width="9.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="2:37" s="36" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="67" t="s">
-        <v>55</v>
+      <c r="B1" s="63" t="s">
+        <v>45</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="38"/>
@@ -5256,7 +5649,7 @@
     </row>
     <row r="3" spans="2:37" ht="18" x14ac:dyDescent="0.2">
       <c r="B3" s="5" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
@@ -5270,64 +5663,149 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="93" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="94"/>
-      <c r="D4" s="94"/>
-      <c r="E4" s="94"/>
-      <c r="F4" s="94"/>
-      <c r="G4" s="94"/>
-      <c r="H4" s="94"/>
-      <c r="I4" s="94"/>
-      <c r="J4" s="94"/>
-      <c r="K4" s="94"/>
-      <c r="L4" s="94"/>
-    </row>
-    <row r="5" spans="2:37" ht="18.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
+      <c r="B4" s="83" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="84"/>
+      <c r="D4" s="84"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="84"/>
+      <c r="G4" s="84"/>
+      <c r="H4" s="84"/>
+      <c r="I4" s="84"/>
+      <c r="J4" s="84"/>
+      <c r="K4" s="84"/>
+      <c r="L4" s="84"/>
+    </row>
+    <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="48"/>
+      <c r="C5" s="49"/>
+      <c r="D5" s="49"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="49"/>
+      <c r="J5" s="49"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="49"/>
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B6" s="57"/>
+      <c r="B6" s="90" t="s">
+        <v>39</v>
+      </c>
+      <c r="C6" s="91" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="92"/>
+      <c r="I6" s="93"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="M7" s="58"/>
-      <c r="N7" s="58"/>
-      <c r="O7" s="58"/>
-      <c r="P7" s="58"/>
-      <c r="Q7" s="58"/>
+      <c r="B7" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="C7" s="112" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
+      <c r="G7" s="113"/>
+      <c r="H7" s="113"/>
+      <c r="I7" s="114"/>
+      <c r="M7" s="54"/>
+      <c r="N7" s="54"/>
+      <c r="O7" s="54"/>
+      <c r="P7" s="54"/>
+      <c r="Q7" s="54"/>
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="M8" s="58"/>
-      <c r="N8" s="58"/>
-      <c r="O8" s="58"/>
-      <c r="P8" s="58"/>
-      <c r="Q8" s="58"/>
+      <c r="B8" s="95" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="96" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="97"/>
+      <c r="E8" s="97"/>
+      <c r="F8" s="97"/>
+      <c r="G8" s="97"/>
+      <c r="H8" s="97"/>
+      <c r="I8" s="98"/>
+      <c r="M8" s="54"/>
+      <c r="N8" s="54"/>
+      <c r="O8" s="54"/>
+      <c r="P8" s="54"/>
+      <c r="Q8" s="54"/>
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="M9" s="58"/>
-      <c r="N9" s="58"/>
-      <c r="O9" s="58"/>
-      <c r="P9" s="58"/>
-      <c r="Q9" s="58"/>
-    </row>
-    <row r="15" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="E15" t="s">
-        <v>52</v>
-      </c>
+      <c r="B9" s="99" t="s">
+        <v>72</v>
+      </c>
+      <c r="C9" s="100" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="101"/>
+      <c r="E9" s="101"/>
+      <c r="F9" s="101"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+      <c r="I9" s="102"/>
+      <c r="M9" s="54"/>
+      <c r="N9" s="54"/>
+      <c r="O9" s="54"/>
+      <c r="P9" s="54"/>
+      <c r="Q9" s="54"/>
+    </row>
+    <row r="10" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B10" s="103" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="104" t="s">
+        <v>78</v>
+      </c>
+      <c r="D10" s="105"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="106"/>
+    </row>
+    <row r="11" spans="2:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="107" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11" s="108" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" s="109"/>
+      <c r="E11" s="109"/>
+      <c r="F11" s="109"/>
+      <c r="G11" s="109"/>
+      <c r="H11" s="109"/>
+      <c r="I11" s="110"/>
+    </row>
+    <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="C12" s="86"/>
+    </row>
+    <row r="13" spans="2:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="C13" s="86"/>
+    </row>
+    <row r="14" spans="2:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="C14" s="86"/>
+    </row>
+    <row r="15" spans="2:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="C15" s="86"/>
+    </row>
+    <row r="16" spans="2:37" ht="18" x14ac:dyDescent="0.2">
+      <c r="C16" s="86"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="57"/>
+      <c r="B20" s="53"/>
     </row>
     <row r="22" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="42"/>
@@ -5382,15 +5860,20 @@
       <c r="L26" s="43"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="C11:I11"/>
+    <mergeCell ref="C9:I9"/>
     <mergeCell ref="B4:L4"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="C8:I8"/>
   </mergeCells>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="1.2598425196850394" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;F_x000D_Version 0.1&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -5406,10 +5889,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AJ10"/>
+  <dimension ref="B1:AJ11"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6121,82 +6604,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
-        <v>55</v>
+      <c r="B1" s="66" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="95" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="95"/>
+      <c r="B3" s="85" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="85"/>
+      <c r="D3" s="85"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="39"/>
       <c r="C4" s="39"/>
       <c r="D4" s="39"/>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B5" s="73" t="s">
+    <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B5" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" s="47">
+        <v>0</v>
+      </c>
+      <c r="D5" s="39"/>
+    </row>
+    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="87" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" s="47">
+        <v>1</v>
+      </c>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="C7" s="47">
+        <v>8</v>
+      </c>
+      <c r="D7" s="39"/>
+    </row>
+    <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B8" s="87" t="s">
+        <v>73</v>
+      </c>
+      <c r="C8" s="47">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="87" t="s">
+        <v>74</v>
+      </c>
+      <c r="C9" s="50">
+        <v>0</v>
+      </c>
+      <c r="D9" s="41"/>
+    </row>
+    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B10" s="94"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+    </row>
+    <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B11" s="40" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="49">
-        <v>0</v>
-      </c>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B6" s="73" t="s">
-        <v>95</v>
-      </c>
-      <c r="C6" s="49">
-        <v>3</v>
-      </c>
-      <c r="D6" s="39"/>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B7" s="73" t="s">
-        <v>84</v>
-      </c>
-      <c r="C7" s="49">
-        <v>7</v>
-      </c>
-      <c r="D7" s="39"/>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.15">
-      <c r="B8" s="73" t="s">
-        <v>96</v>
-      </c>
-      <c r="C8" s="49">
-        <v>0</v>
-      </c>
-      <c r="D8" s="39"/>
-    </row>
-    <row r="9" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-    </row>
-    <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="C10"/>
-      <c r="D10"/>
+      <c r="C11"/>
+      <c r="D11"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <mergeCells count="1">
     <mergeCell ref="B3:D3"/>
   </mergeCells>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
   <pageSetup paperSize="9" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.1&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -6212,1040 +6704,1014 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AJ29"/>
+  <dimension ref="B1:AI29"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A4" zoomScale="120" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:G7"/>
+    <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="6" style="36" customWidth="1"/>
-    <col min="2" max="2" width="19" style="37" customWidth="1"/>
-    <col min="3" max="3" width="30.6640625" style="37" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" style="38" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" style="38" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="38" customWidth="1"/>
-    <col min="8" max="26" width="3.33203125" style="38" customWidth="1"/>
-    <col min="27" max="27" width="10" style="38" customWidth="1"/>
-    <col min="28" max="36" width="8.83203125" style="38"/>
-    <col min="37" max="237" width="8.83203125" style="36"/>
-    <col min="238" max="238" width="1.5" style="36" customWidth="1"/>
-    <col min="239" max="239" width="1.33203125" style="36" customWidth="1"/>
-    <col min="240" max="240" width="42" style="36" customWidth="1"/>
-    <col min="241" max="241" width="5.5" style="36" customWidth="1"/>
-    <col min="242" max="243" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="244" max="244" width="2.6640625" style="36" customWidth="1"/>
-    <col min="245" max="280" width="3.33203125" style="36" customWidth="1"/>
-    <col min="281" max="281" width="1.6640625" style="36" customWidth="1"/>
-    <col min="282" max="282" width="25.6640625" style="36" customWidth="1"/>
-    <col min="283" max="283" width="31.33203125" style="36" customWidth="1"/>
-    <col min="284" max="493" width="8.83203125" style="36"/>
-    <col min="494" max="494" width="1.5" style="36" customWidth="1"/>
-    <col min="495" max="495" width="1.33203125" style="36" customWidth="1"/>
-    <col min="496" max="496" width="42" style="36" customWidth="1"/>
-    <col min="497" max="497" width="5.5" style="36" customWidth="1"/>
-    <col min="498" max="499" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="500" max="500" width="2.6640625" style="36" customWidth="1"/>
-    <col min="501" max="536" width="3.33203125" style="36" customWidth="1"/>
-    <col min="537" max="537" width="1.6640625" style="36" customWidth="1"/>
-    <col min="538" max="538" width="25.6640625" style="36" customWidth="1"/>
-    <col min="539" max="539" width="31.33203125" style="36" customWidth="1"/>
-    <col min="540" max="749" width="8.83203125" style="36"/>
-    <col min="750" max="750" width="1.5" style="36" customWidth="1"/>
-    <col min="751" max="751" width="1.33203125" style="36" customWidth="1"/>
-    <col min="752" max="752" width="42" style="36" customWidth="1"/>
-    <col min="753" max="753" width="5.5" style="36" customWidth="1"/>
-    <col min="754" max="755" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="756" max="756" width="2.6640625" style="36" customWidth="1"/>
-    <col min="757" max="792" width="3.33203125" style="36" customWidth="1"/>
-    <col min="793" max="793" width="1.6640625" style="36" customWidth="1"/>
-    <col min="794" max="794" width="25.6640625" style="36" customWidth="1"/>
-    <col min="795" max="795" width="31.33203125" style="36" customWidth="1"/>
-    <col min="796" max="1005" width="8.83203125" style="36"/>
-    <col min="1006" max="1006" width="1.5" style="36" customWidth="1"/>
-    <col min="1007" max="1007" width="1.33203125" style="36" customWidth="1"/>
-    <col min="1008" max="1008" width="42" style="36" customWidth="1"/>
-    <col min="1009" max="1009" width="5.5" style="36" customWidth="1"/>
-    <col min="1010" max="1011" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="1012" max="1012" width="2.6640625" style="36" customWidth="1"/>
-    <col min="1013" max="1048" width="3.33203125" style="36" customWidth="1"/>
-    <col min="1049" max="1049" width="1.6640625" style="36" customWidth="1"/>
-    <col min="1050" max="1050" width="25.6640625" style="36" customWidth="1"/>
-    <col min="1051" max="1051" width="31.33203125" style="36" customWidth="1"/>
-    <col min="1052" max="1261" width="8.83203125" style="36"/>
-    <col min="1262" max="1262" width="1.5" style="36" customWidth="1"/>
-    <col min="1263" max="1263" width="1.33203125" style="36" customWidth="1"/>
-    <col min="1264" max="1264" width="42" style="36" customWidth="1"/>
-    <col min="1265" max="1265" width="5.5" style="36" customWidth="1"/>
-    <col min="1266" max="1267" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="1268" max="1268" width="2.6640625" style="36" customWidth="1"/>
-    <col min="1269" max="1304" width="3.33203125" style="36" customWidth="1"/>
-    <col min="1305" max="1305" width="1.6640625" style="36" customWidth="1"/>
-    <col min="1306" max="1306" width="25.6640625" style="36" customWidth="1"/>
-    <col min="1307" max="1307" width="31.33203125" style="36" customWidth="1"/>
-    <col min="1308" max="1517" width="8.83203125" style="36"/>
-    <col min="1518" max="1518" width="1.5" style="36" customWidth="1"/>
-    <col min="1519" max="1519" width="1.33203125" style="36" customWidth="1"/>
-    <col min="1520" max="1520" width="42" style="36" customWidth="1"/>
-    <col min="1521" max="1521" width="5.5" style="36" customWidth="1"/>
-    <col min="1522" max="1523" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="1524" max="1524" width="2.6640625" style="36" customWidth="1"/>
-    <col min="1525" max="1560" width="3.33203125" style="36" customWidth="1"/>
-    <col min="1561" max="1561" width="1.6640625" style="36" customWidth="1"/>
-    <col min="1562" max="1562" width="25.6640625" style="36" customWidth="1"/>
-    <col min="1563" max="1563" width="31.33203125" style="36" customWidth="1"/>
-    <col min="1564" max="1773" width="8.83203125" style="36"/>
-    <col min="1774" max="1774" width="1.5" style="36" customWidth="1"/>
-    <col min="1775" max="1775" width="1.33203125" style="36" customWidth="1"/>
-    <col min="1776" max="1776" width="42" style="36" customWidth="1"/>
-    <col min="1777" max="1777" width="5.5" style="36" customWidth="1"/>
-    <col min="1778" max="1779" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="1780" max="1780" width="2.6640625" style="36" customWidth="1"/>
-    <col min="1781" max="1816" width="3.33203125" style="36" customWidth="1"/>
-    <col min="1817" max="1817" width="1.6640625" style="36" customWidth="1"/>
-    <col min="1818" max="1818" width="25.6640625" style="36" customWidth="1"/>
-    <col min="1819" max="1819" width="31.33203125" style="36" customWidth="1"/>
-    <col min="1820" max="2029" width="8.83203125" style="36"/>
-    <col min="2030" max="2030" width="1.5" style="36" customWidth="1"/>
-    <col min="2031" max="2031" width="1.33203125" style="36" customWidth="1"/>
-    <col min="2032" max="2032" width="42" style="36" customWidth="1"/>
-    <col min="2033" max="2033" width="5.5" style="36" customWidth="1"/>
-    <col min="2034" max="2035" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="2036" max="2036" width="2.6640625" style="36" customWidth="1"/>
-    <col min="2037" max="2072" width="3.33203125" style="36" customWidth="1"/>
-    <col min="2073" max="2073" width="1.6640625" style="36" customWidth="1"/>
-    <col min="2074" max="2074" width="25.6640625" style="36" customWidth="1"/>
-    <col min="2075" max="2075" width="31.33203125" style="36" customWidth="1"/>
-    <col min="2076" max="2285" width="8.83203125" style="36"/>
-    <col min="2286" max="2286" width="1.5" style="36" customWidth="1"/>
-    <col min="2287" max="2287" width="1.33203125" style="36" customWidth="1"/>
-    <col min="2288" max="2288" width="42" style="36" customWidth="1"/>
-    <col min="2289" max="2289" width="5.5" style="36" customWidth="1"/>
-    <col min="2290" max="2291" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="2292" max="2292" width="2.6640625" style="36" customWidth="1"/>
-    <col min="2293" max="2328" width="3.33203125" style="36" customWidth="1"/>
-    <col min="2329" max="2329" width="1.6640625" style="36" customWidth="1"/>
-    <col min="2330" max="2330" width="25.6640625" style="36" customWidth="1"/>
-    <col min="2331" max="2331" width="31.33203125" style="36" customWidth="1"/>
-    <col min="2332" max="2541" width="8.83203125" style="36"/>
-    <col min="2542" max="2542" width="1.5" style="36" customWidth="1"/>
-    <col min="2543" max="2543" width="1.33203125" style="36" customWidth="1"/>
-    <col min="2544" max="2544" width="42" style="36" customWidth="1"/>
-    <col min="2545" max="2545" width="5.5" style="36" customWidth="1"/>
-    <col min="2546" max="2547" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="2548" max="2548" width="2.6640625" style="36" customWidth="1"/>
-    <col min="2549" max="2584" width="3.33203125" style="36" customWidth="1"/>
-    <col min="2585" max="2585" width="1.6640625" style="36" customWidth="1"/>
-    <col min="2586" max="2586" width="25.6640625" style="36" customWidth="1"/>
-    <col min="2587" max="2587" width="31.33203125" style="36" customWidth="1"/>
-    <col min="2588" max="2797" width="8.83203125" style="36"/>
-    <col min="2798" max="2798" width="1.5" style="36" customWidth="1"/>
-    <col min="2799" max="2799" width="1.33203125" style="36" customWidth="1"/>
-    <col min="2800" max="2800" width="42" style="36" customWidth="1"/>
-    <col min="2801" max="2801" width="5.5" style="36" customWidth="1"/>
-    <col min="2802" max="2803" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="2804" max="2804" width="2.6640625" style="36" customWidth="1"/>
-    <col min="2805" max="2840" width="3.33203125" style="36" customWidth="1"/>
-    <col min="2841" max="2841" width="1.6640625" style="36" customWidth="1"/>
-    <col min="2842" max="2842" width="25.6640625" style="36" customWidth="1"/>
-    <col min="2843" max="2843" width="31.33203125" style="36" customWidth="1"/>
-    <col min="2844" max="3053" width="8.83203125" style="36"/>
-    <col min="3054" max="3054" width="1.5" style="36" customWidth="1"/>
-    <col min="3055" max="3055" width="1.33203125" style="36" customWidth="1"/>
-    <col min="3056" max="3056" width="42" style="36" customWidth="1"/>
-    <col min="3057" max="3057" width="5.5" style="36" customWidth="1"/>
-    <col min="3058" max="3059" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="3060" max="3060" width="2.6640625" style="36" customWidth="1"/>
-    <col min="3061" max="3096" width="3.33203125" style="36" customWidth="1"/>
-    <col min="3097" max="3097" width="1.6640625" style="36" customWidth="1"/>
-    <col min="3098" max="3098" width="25.6640625" style="36" customWidth="1"/>
-    <col min="3099" max="3099" width="31.33203125" style="36" customWidth="1"/>
-    <col min="3100" max="3309" width="8.83203125" style="36"/>
-    <col min="3310" max="3310" width="1.5" style="36" customWidth="1"/>
-    <col min="3311" max="3311" width="1.33203125" style="36" customWidth="1"/>
-    <col min="3312" max="3312" width="42" style="36" customWidth="1"/>
-    <col min="3313" max="3313" width="5.5" style="36" customWidth="1"/>
-    <col min="3314" max="3315" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="3316" max="3316" width="2.6640625" style="36" customWidth="1"/>
-    <col min="3317" max="3352" width="3.33203125" style="36" customWidth="1"/>
-    <col min="3353" max="3353" width="1.6640625" style="36" customWidth="1"/>
-    <col min="3354" max="3354" width="25.6640625" style="36" customWidth="1"/>
-    <col min="3355" max="3355" width="31.33203125" style="36" customWidth="1"/>
-    <col min="3356" max="3565" width="8.83203125" style="36"/>
-    <col min="3566" max="3566" width="1.5" style="36" customWidth="1"/>
-    <col min="3567" max="3567" width="1.33203125" style="36" customWidth="1"/>
-    <col min="3568" max="3568" width="42" style="36" customWidth="1"/>
-    <col min="3569" max="3569" width="5.5" style="36" customWidth="1"/>
-    <col min="3570" max="3571" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="3572" max="3572" width="2.6640625" style="36" customWidth="1"/>
-    <col min="3573" max="3608" width="3.33203125" style="36" customWidth="1"/>
-    <col min="3609" max="3609" width="1.6640625" style="36" customWidth="1"/>
-    <col min="3610" max="3610" width="25.6640625" style="36" customWidth="1"/>
-    <col min="3611" max="3611" width="31.33203125" style="36" customWidth="1"/>
-    <col min="3612" max="3821" width="8.83203125" style="36"/>
-    <col min="3822" max="3822" width="1.5" style="36" customWidth="1"/>
-    <col min="3823" max="3823" width="1.33203125" style="36" customWidth="1"/>
-    <col min="3824" max="3824" width="42" style="36" customWidth="1"/>
-    <col min="3825" max="3825" width="5.5" style="36" customWidth="1"/>
-    <col min="3826" max="3827" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="3828" max="3828" width="2.6640625" style="36" customWidth="1"/>
-    <col min="3829" max="3864" width="3.33203125" style="36" customWidth="1"/>
-    <col min="3865" max="3865" width="1.6640625" style="36" customWidth="1"/>
-    <col min="3866" max="3866" width="25.6640625" style="36" customWidth="1"/>
-    <col min="3867" max="3867" width="31.33203125" style="36" customWidth="1"/>
-    <col min="3868" max="4077" width="8.83203125" style="36"/>
-    <col min="4078" max="4078" width="1.5" style="36" customWidth="1"/>
-    <col min="4079" max="4079" width="1.33203125" style="36" customWidth="1"/>
-    <col min="4080" max="4080" width="42" style="36" customWidth="1"/>
-    <col min="4081" max="4081" width="5.5" style="36" customWidth="1"/>
-    <col min="4082" max="4083" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="4084" max="4084" width="2.6640625" style="36" customWidth="1"/>
-    <col min="4085" max="4120" width="3.33203125" style="36" customWidth="1"/>
-    <col min="4121" max="4121" width="1.6640625" style="36" customWidth="1"/>
-    <col min="4122" max="4122" width="25.6640625" style="36" customWidth="1"/>
-    <col min="4123" max="4123" width="31.33203125" style="36" customWidth="1"/>
-    <col min="4124" max="4333" width="8.83203125" style="36"/>
-    <col min="4334" max="4334" width="1.5" style="36" customWidth="1"/>
-    <col min="4335" max="4335" width="1.33203125" style="36" customWidth="1"/>
-    <col min="4336" max="4336" width="42" style="36" customWidth="1"/>
-    <col min="4337" max="4337" width="5.5" style="36" customWidth="1"/>
-    <col min="4338" max="4339" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="4340" max="4340" width="2.6640625" style="36" customWidth="1"/>
-    <col min="4341" max="4376" width="3.33203125" style="36" customWidth="1"/>
-    <col min="4377" max="4377" width="1.6640625" style="36" customWidth="1"/>
-    <col min="4378" max="4378" width="25.6640625" style="36" customWidth="1"/>
-    <col min="4379" max="4379" width="31.33203125" style="36" customWidth="1"/>
-    <col min="4380" max="4589" width="8.83203125" style="36"/>
-    <col min="4590" max="4590" width="1.5" style="36" customWidth="1"/>
-    <col min="4591" max="4591" width="1.33203125" style="36" customWidth="1"/>
-    <col min="4592" max="4592" width="42" style="36" customWidth="1"/>
-    <col min="4593" max="4593" width="5.5" style="36" customWidth="1"/>
-    <col min="4594" max="4595" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="4596" max="4596" width="2.6640625" style="36" customWidth="1"/>
-    <col min="4597" max="4632" width="3.33203125" style="36" customWidth="1"/>
-    <col min="4633" max="4633" width="1.6640625" style="36" customWidth="1"/>
-    <col min="4634" max="4634" width="25.6640625" style="36" customWidth="1"/>
-    <col min="4635" max="4635" width="31.33203125" style="36" customWidth="1"/>
-    <col min="4636" max="4845" width="8.83203125" style="36"/>
-    <col min="4846" max="4846" width="1.5" style="36" customWidth="1"/>
-    <col min="4847" max="4847" width="1.33203125" style="36" customWidth="1"/>
-    <col min="4848" max="4848" width="42" style="36" customWidth="1"/>
-    <col min="4849" max="4849" width="5.5" style="36" customWidth="1"/>
-    <col min="4850" max="4851" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="4852" max="4852" width="2.6640625" style="36" customWidth="1"/>
-    <col min="4853" max="4888" width="3.33203125" style="36" customWidth="1"/>
-    <col min="4889" max="4889" width="1.6640625" style="36" customWidth="1"/>
-    <col min="4890" max="4890" width="25.6640625" style="36" customWidth="1"/>
-    <col min="4891" max="4891" width="31.33203125" style="36" customWidth="1"/>
-    <col min="4892" max="5101" width="8.83203125" style="36"/>
-    <col min="5102" max="5102" width="1.5" style="36" customWidth="1"/>
-    <col min="5103" max="5103" width="1.33203125" style="36" customWidth="1"/>
-    <col min="5104" max="5104" width="42" style="36" customWidth="1"/>
-    <col min="5105" max="5105" width="5.5" style="36" customWidth="1"/>
-    <col min="5106" max="5107" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="5108" max="5108" width="2.6640625" style="36" customWidth="1"/>
-    <col min="5109" max="5144" width="3.33203125" style="36" customWidth="1"/>
-    <col min="5145" max="5145" width="1.6640625" style="36" customWidth="1"/>
-    <col min="5146" max="5146" width="25.6640625" style="36" customWidth="1"/>
-    <col min="5147" max="5147" width="31.33203125" style="36" customWidth="1"/>
-    <col min="5148" max="5357" width="8.83203125" style="36"/>
-    <col min="5358" max="5358" width="1.5" style="36" customWidth="1"/>
-    <col min="5359" max="5359" width="1.33203125" style="36" customWidth="1"/>
-    <col min="5360" max="5360" width="42" style="36" customWidth="1"/>
-    <col min="5361" max="5361" width="5.5" style="36" customWidth="1"/>
-    <col min="5362" max="5363" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="5364" max="5364" width="2.6640625" style="36" customWidth="1"/>
-    <col min="5365" max="5400" width="3.33203125" style="36" customWidth="1"/>
-    <col min="5401" max="5401" width="1.6640625" style="36" customWidth="1"/>
-    <col min="5402" max="5402" width="25.6640625" style="36" customWidth="1"/>
-    <col min="5403" max="5403" width="31.33203125" style="36" customWidth="1"/>
-    <col min="5404" max="5613" width="8.83203125" style="36"/>
-    <col min="5614" max="5614" width="1.5" style="36" customWidth="1"/>
-    <col min="5615" max="5615" width="1.33203125" style="36" customWidth="1"/>
-    <col min="5616" max="5616" width="42" style="36" customWidth="1"/>
-    <col min="5617" max="5617" width="5.5" style="36" customWidth="1"/>
-    <col min="5618" max="5619" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="5620" max="5620" width="2.6640625" style="36" customWidth="1"/>
-    <col min="5621" max="5656" width="3.33203125" style="36" customWidth="1"/>
-    <col min="5657" max="5657" width="1.6640625" style="36" customWidth="1"/>
-    <col min="5658" max="5658" width="25.6640625" style="36" customWidth="1"/>
-    <col min="5659" max="5659" width="31.33203125" style="36" customWidth="1"/>
-    <col min="5660" max="5869" width="8.83203125" style="36"/>
-    <col min="5870" max="5870" width="1.5" style="36" customWidth="1"/>
-    <col min="5871" max="5871" width="1.33203125" style="36" customWidth="1"/>
-    <col min="5872" max="5872" width="42" style="36" customWidth="1"/>
-    <col min="5873" max="5873" width="5.5" style="36" customWidth="1"/>
-    <col min="5874" max="5875" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="5876" max="5876" width="2.6640625" style="36" customWidth="1"/>
-    <col min="5877" max="5912" width="3.33203125" style="36" customWidth="1"/>
-    <col min="5913" max="5913" width="1.6640625" style="36" customWidth="1"/>
-    <col min="5914" max="5914" width="25.6640625" style="36" customWidth="1"/>
-    <col min="5915" max="5915" width="31.33203125" style="36" customWidth="1"/>
-    <col min="5916" max="6125" width="8.83203125" style="36"/>
-    <col min="6126" max="6126" width="1.5" style="36" customWidth="1"/>
-    <col min="6127" max="6127" width="1.33203125" style="36" customWidth="1"/>
-    <col min="6128" max="6128" width="42" style="36" customWidth="1"/>
-    <col min="6129" max="6129" width="5.5" style="36" customWidth="1"/>
-    <col min="6130" max="6131" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="6132" max="6132" width="2.6640625" style="36" customWidth="1"/>
-    <col min="6133" max="6168" width="3.33203125" style="36" customWidth="1"/>
-    <col min="6169" max="6169" width="1.6640625" style="36" customWidth="1"/>
-    <col min="6170" max="6170" width="25.6640625" style="36" customWidth="1"/>
-    <col min="6171" max="6171" width="31.33203125" style="36" customWidth="1"/>
-    <col min="6172" max="6381" width="8.83203125" style="36"/>
-    <col min="6382" max="6382" width="1.5" style="36" customWidth="1"/>
-    <col min="6383" max="6383" width="1.33203125" style="36" customWidth="1"/>
-    <col min="6384" max="6384" width="42" style="36" customWidth="1"/>
-    <col min="6385" max="6385" width="5.5" style="36" customWidth="1"/>
-    <col min="6386" max="6387" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="6388" max="6388" width="2.6640625" style="36" customWidth="1"/>
-    <col min="6389" max="6424" width="3.33203125" style="36" customWidth="1"/>
-    <col min="6425" max="6425" width="1.6640625" style="36" customWidth="1"/>
-    <col min="6426" max="6426" width="25.6640625" style="36" customWidth="1"/>
-    <col min="6427" max="6427" width="31.33203125" style="36" customWidth="1"/>
-    <col min="6428" max="6637" width="8.83203125" style="36"/>
-    <col min="6638" max="6638" width="1.5" style="36" customWidth="1"/>
-    <col min="6639" max="6639" width="1.33203125" style="36" customWidth="1"/>
-    <col min="6640" max="6640" width="42" style="36" customWidth="1"/>
-    <col min="6641" max="6641" width="5.5" style="36" customWidth="1"/>
-    <col min="6642" max="6643" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="6644" max="6644" width="2.6640625" style="36" customWidth="1"/>
-    <col min="6645" max="6680" width="3.33203125" style="36" customWidth="1"/>
-    <col min="6681" max="6681" width="1.6640625" style="36" customWidth="1"/>
-    <col min="6682" max="6682" width="25.6640625" style="36" customWidth="1"/>
-    <col min="6683" max="6683" width="31.33203125" style="36" customWidth="1"/>
-    <col min="6684" max="6893" width="8.83203125" style="36"/>
-    <col min="6894" max="6894" width="1.5" style="36" customWidth="1"/>
-    <col min="6895" max="6895" width="1.33203125" style="36" customWidth="1"/>
-    <col min="6896" max="6896" width="42" style="36" customWidth="1"/>
-    <col min="6897" max="6897" width="5.5" style="36" customWidth="1"/>
-    <col min="6898" max="6899" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="6900" max="6900" width="2.6640625" style="36" customWidth="1"/>
-    <col min="6901" max="6936" width="3.33203125" style="36" customWidth="1"/>
-    <col min="6937" max="6937" width="1.6640625" style="36" customWidth="1"/>
-    <col min="6938" max="6938" width="25.6640625" style="36" customWidth="1"/>
-    <col min="6939" max="6939" width="31.33203125" style="36" customWidth="1"/>
-    <col min="6940" max="7149" width="8.83203125" style="36"/>
-    <col min="7150" max="7150" width="1.5" style="36" customWidth="1"/>
-    <col min="7151" max="7151" width="1.33203125" style="36" customWidth="1"/>
-    <col min="7152" max="7152" width="42" style="36" customWidth="1"/>
-    <col min="7153" max="7153" width="5.5" style="36" customWidth="1"/>
-    <col min="7154" max="7155" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="7156" max="7156" width="2.6640625" style="36" customWidth="1"/>
-    <col min="7157" max="7192" width="3.33203125" style="36" customWidth="1"/>
-    <col min="7193" max="7193" width="1.6640625" style="36" customWidth="1"/>
-    <col min="7194" max="7194" width="25.6640625" style="36" customWidth="1"/>
-    <col min="7195" max="7195" width="31.33203125" style="36" customWidth="1"/>
-    <col min="7196" max="7405" width="8.83203125" style="36"/>
-    <col min="7406" max="7406" width="1.5" style="36" customWidth="1"/>
-    <col min="7407" max="7407" width="1.33203125" style="36" customWidth="1"/>
-    <col min="7408" max="7408" width="42" style="36" customWidth="1"/>
-    <col min="7409" max="7409" width="5.5" style="36" customWidth="1"/>
-    <col min="7410" max="7411" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="7412" max="7412" width="2.6640625" style="36" customWidth="1"/>
-    <col min="7413" max="7448" width="3.33203125" style="36" customWidth="1"/>
-    <col min="7449" max="7449" width="1.6640625" style="36" customWidth="1"/>
-    <col min="7450" max="7450" width="25.6640625" style="36" customWidth="1"/>
-    <col min="7451" max="7451" width="31.33203125" style="36" customWidth="1"/>
-    <col min="7452" max="7661" width="8.83203125" style="36"/>
-    <col min="7662" max="7662" width="1.5" style="36" customWidth="1"/>
-    <col min="7663" max="7663" width="1.33203125" style="36" customWidth="1"/>
-    <col min="7664" max="7664" width="42" style="36" customWidth="1"/>
-    <col min="7665" max="7665" width="5.5" style="36" customWidth="1"/>
-    <col min="7666" max="7667" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="7668" max="7668" width="2.6640625" style="36" customWidth="1"/>
-    <col min="7669" max="7704" width="3.33203125" style="36" customWidth="1"/>
-    <col min="7705" max="7705" width="1.6640625" style="36" customWidth="1"/>
-    <col min="7706" max="7706" width="25.6640625" style="36" customWidth="1"/>
-    <col min="7707" max="7707" width="31.33203125" style="36" customWidth="1"/>
-    <col min="7708" max="7917" width="8.83203125" style="36"/>
-    <col min="7918" max="7918" width="1.5" style="36" customWidth="1"/>
-    <col min="7919" max="7919" width="1.33203125" style="36" customWidth="1"/>
-    <col min="7920" max="7920" width="42" style="36" customWidth="1"/>
-    <col min="7921" max="7921" width="5.5" style="36" customWidth="1"/>
-    <col min="7922" max="7923" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="7924" max="7924" width="2.6640625" style="36" customWidth="1"/>
-    <col min="7925" max="7960" width="3.33203125" style="36" customWidth="1"/>
-    <col min="7961" max="7961" width="1.6640625" style="36" customWidth="1"/>
-    <col min="7962" max="7962" width="25.6640625" style="36" customWidth="1"/>
-    <col min="7963" max="7963" width="31.33203125" style="36" customWidth="1"/>
-    <col min="7964" max="8173" width="8.83203125" style="36"/>
-    <col min="8174" max="8174" width="1.5" style="36" customWidth="1"/>
-    <col min="8175" max="8175" width="1.33203125" style="36" customWidth="1"/>
-    <col min="8176" max="8176" width="42" style="36" customWidth="1"/>
-    <col min="8177" max="8177" width="5.5" style="36" customWidth="1"/>
-    <col min="8178" max="8179" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="8180" max="8180" width="2.6640625" style="36" customWidth="1"/>
-    <col min="8181" max="8216" width="3.33203125" style="36" customWidth="1"/>
-    <col min="8217" max="8217" width="1.6640625" style="36" customWidth="1"/>
-    <col min="8218" max="8218" width="25.6640625" style="36" customWidth="1"/>
-    <col min="8219" max="8219" width="31.33203125" style="36" customWidth="1"/>
-    <col min="8220" max="8429" width="8.83203125" style="36"/>
-    <col min="8430" max="8430" width="1.5" style="36" customWidth="1"/>
-    <col min="8431" max="8431" width="1.33203125" style="36" customWidth="1"/>
-    <col min="8432" max="8432" width="42" style="36" customWidth="1"/>
-    <col min="8433" max="8433" width="5.5" style="36" customWidth="1"/>
-    <col min="8434" max="8435" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="8436" max="8436" width="2.6640625" style="36" customWidth="1"/>
-    <col min="8437" max="8472" width="3.33203125" style="36" customWidth="1"/>
-    <col min="8473" max="8473" width="1.6640625" style="36" customWidth="1"/>
-    <col min="8474" max="8474" width="25.6640625" style="36" customWidth="1"/>
-    <col min="8475" max="8475" width="31.33203125" style="36" customWidth="1"/>
-    <col min="8476" max="8685" width="8.83203125" style="36"/>
-    <col min="8686" max="8686" width="1.5" style="36" customWidth="1"/>
-    <col min="8687" max="8687" width="1.33203125" style="36" customWidth="1"/>
-    <col min="8688" max="8688" width="42" style="36" customWidth="1"/>
-    <col min="8689" max="8689" width="5.5" style="36" customWidth="1"/>
-    <col min="8690" max="8691" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="8692" max="8692" width="2.6640625" style="36" customWidth="1"/>
-    <col min="8693" max="8728" width="3.33203125" style="36" customWidth="1"/>
-    <col min="8729" max="8729" width="1.6640625" style="36" customWidth="1"/>
-    <col min="8730" max="8730" width="25.6640625" style="36" customWidth="1"/>
-    <col min="8731" max="8731" width="31.33203125" style="36" customWidth="1"/>
-    <col min="8732" max="8941" width="8.83203125" style="36"/>
-    <col min="8942" max="8942" width="1.5" style="36" customWidth="1"/>
-    <col min="8943" max="8943" width="1.33203125" style="36" customWidth="1"/>
-    <col min="8944" max="8944" width="42" style="36" customWidth="1"/>
-    <col min="8945" max="8945" width="5.5" style="36" customWidth="1"/>
-    <col min="8946" max="8947" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="8948" max="8948" width="2.6640625" style="36" customWidth="1"/>
-    <col min="8949" max="8984" width="3.33203125" style="36" customWidth="1"/>
-    <col min="8985" max="8985" width="1.6640625" style="36" customWidth="1"/>
-    <col min="8986" max="8986" width="25.6640625" style="36" customWidth="1"/>
-    <col min="8987" max="8987" width="31.33203125" style="36" customWidth="1"/>
-    <col min="8988" max="9197" width="8.83203125" style="36"/>
-    <col min="9198" max="9198" width="1.5" style="36" customWidth="1"/>
-    <col min="9199" max="9199" width="1.33203125" style="36" customWidth="1"/>
-    <col min="9200" max="9200" width="42" style="36" customWidth="1"/>
-    <col min="9201" max="9201" width="5.5" style="36" customWidth="1"/>
-    <col min="9202" max="9203" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="9204" max="9204" width="2.6640625" style="36" customWidth="1"/>
-    <col min="9205" max="9240" width="3.33203125" style="36" customWidth="1"/>
-    <col min="9241" max="9241" width="1.6640625" style="36" customWidth="1"/>
-    <col min="9242" max="9242" width="25.6640625" style="36" customWidth="1"/>
-    <col min="9243" max="9243" width="31.33203125" style="36" customWidth="1"/>
-    <col min="9244" max="9453" width="8.83203125" style="36"/>
-    <col min="9454" max="9454" width="1.5" style="36" customWidth="1"/>
-    <col min="9455" max="9455" width="1.33203125" style="36" customWidth="1"/>
-    <col min="9456" max="9456" width="42" style="36" customWidth="1"/>
-    <col min="9457" max="9457" width="5.5" style="36" customWidth="1"/>
-    <col min="9458" max="9459" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="9460" max="9460" width="2.6640625" style="36" customWidth="1"/>
-    <col min="9461" max="9496" width="3.33203125" style="36" customWidth="1"/>
-    <col min="9497" max="9497" width="1.6640625" style="36" customWidth="1"/>
-    <col min="9498" max="9498" width="25.6640625" style="36" customWidth="1"/>
-    <col min="9499" max="9499" width="31.33203125" style="36" customWidth="1"/>
-    <col min="9500" max="9709" width="8.83203125" style="36"/>
-    <col min="9710" max="9710" width="1.5" style="36" customWidth="1"/>
-    <col min="9711" max="9711" width="1.33203125" style="36" customWidth="1"/>
-    <col min="9712" max="9712" width="42" style="36" customWidth="1"/>
-    <col min="9713" max="9713" width="5.5" style="36" customWidth="1"/>
-    <col min="9714" max="9715" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="9716" max="9716" width="2.6640625" style="36" customWidth="1"/>
-    <col min="9717" max="9752" width="3.33203125" style="36" customWidth="1"/>
-    <col min="9753" max="9753" width="1.6640625" style="36" customWidth="1"/>
-    <col min="9754" max="9754" width="25.6640625" style="36" customWidth="1"/>
-    <col min="9755" max="9755" width="31.33203125" style="36" customWidth="1"/>
-    <col min="9756" max="9965" width="8.83203125" style="36"/>
-    <col min="9966" max="9966" width="1.5" style="36" customWidth="1"/>
-    <col min="9967" max="9967" width="1.33203125" style="36" customWidth="1"/>
-    <col min="9968" max="9968" width="42" style="36" customWidth="1"/>
-    <col min="9969" max="9969" width="5.5" style="36" customWidth="1"/>
-    <col min="9970" max="9971" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="9972" max="9972" width="2.6640625" style="36" customWidth="1"/>
-    <col min="9973" max="10008" width="3.33203125" style="36" customWidth="1"/>
-    <col min="10009" max="10009" width="1.6640625" style="36" customWidth="1"/>
-    <col min="10010" max="10010" width="25.6640625" style="36" customWidth="1"/>
-    <col min="10011" max="10011" width="31.33203125" style="36" customWidth="1"/>
-    <col min="10012" max="10221" width="8.83203125" style="36"/>
-    <col min="10222" max="10222" width="1.5" style="36" customWidth="1"/>
-    <col min="10223" max="10223" width="1.33203125" style="36" customWidth="1"/>
-    <col min="10224" max="10224" width="42" style="36" customWidth="1"/>
-    <col min="10225" max="10225" width="5.5" style="36" customWidth="1"/>
-    <col min="10226" max="10227" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="10228" max="10228" width="2.6640625" style="36" customWidth="1"/>
-    <col min="10229" max="10264" width="3.33203125" style="36" customWidth="1"/>
-    <col min="10265" max="10265" width="1.6640625" style="36" customWidth="1"/>
-    <col min="10266" max="10266" width="25.6640625" style="36" customWidth="1"/>
-    <col min="10267" max="10267" width="31.33203125" style="36" customWidth="1"/>
-    <col min="10268" max="10477" width="8.83203125" style="36"/>
-    <col min="10478" max="10478" width="1.5" style="36" customWidth="1"/>
-    <col min="10479" max="10479" width="1.33203125" style="36" customWidth="1"/>
-    <col min="10480" max="10480" width="42" style="36" customWidth="1"/>
-    <col min="10481" max="10481" width="5.5" style="36" customWidth="1"/>
-    <col min="10482" max="10483" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="10484" max="10484" width="2.6640625" style="36" customWidth="1"/>
-    <col min="10485" max="10520" width="3.33203125" style="36" customWidth="1"/>
-    <col min="10521" max="10521" width="1.6640625" style="36" customWidth="1"/>
-    <col min="10522" max="10522" width="25.6640625" style="36" customWidth="1"/>
-    <col min="10523" max="10523" width="31.33203125" style="36" customWidth="1"/>
-    <col min="10524" max="10733" width="8.83203125" style="36"/>
-    <col min="10734" max="10734" width="1.5" style="36" customWidth="1"/>
-    <col min="10735" max="10735" width="1.33203125" style="36" customWidth="1"/>
-    <col min="10736" max="10736" width="42" style="36" customWidth="1"/>
-    <col min="10737" max="10737" width="5.5" style="36" customWidth="1"/>
-    <col min="10738" max="10739" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="10740" max="10740" width="2.6640625" style="36" customWidth="1"/>
-    <col min="10741" max="10776" width="3.33203125" style="36" customWidth="1"/>
-    <col min="10777" max="10777" width="1.6640625" style="36" customWidth="1"/>
-    <col min="10778" max="10778" width="25.6640625" style="36" customWidth="1"/>
-    <col min="10779" max="10779" width="31.33203125" style="36" customWidth="1"/>
-    <col min="10780" max="10989" width="8.83203125" style="36"/>
-    <col min="10990" max="10990" width="1.5" style="36" customWidth="1"/>
-    <col min="10991" max="10991" width="1.33203125" style="36" customWidth="1"/>
-    <col min="10992" max="10992" width="42" style="36" customWidth="1"/>
-    <col min="10993" max="10993" width="5.5" style="36" customWidth="1"/>
-    <col min="10994" max="10995" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="10996" max="10996" width="2.6640625" style="36" customWidth="1"/>
-    <col min="10997" max="11032" width="3.33203125" style="36" customWidth="1"/>
-    <col min="11033" max="11033" width="1.6640625" style="36" customWidth="1"/>
-    <col min="11034" max="11034" width="25.6640625" style="36" customWidth="1"/>
-    <col min="11035" max="11035" width="31.33203125" style="36" customWidth="1"/>
-    <col min="11036" max="11245" width="8.83203125" style="36"/>
-    <col min="11246" max="11246" width="1.5" style="36" customWidth="1"/>
-    <col min="11247" max="11247" width="1.33203125" style="36" customWidth="1"/>
-    <col min="11248" max="11248" width="42" style="36" customWidth="1"/>
-    <col min="11249" max="11249" width="5.5" style="36" customWidth="1"/>
-    <col min="11250" max="11251" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="11252" max="11252" width="2.6640625" style="36" customWidth="1"/>
-    <col min="11253" max="11288" width="3.33203125" style="36" customWidth="1"/>
-    <col min="11289" max="11289" width="1.6640625" style="36" customWidth="1"/>
-    <col min="11290" max="11290" width="25.6640625" style="36" customWidth="1"/>
-    <col min="11291" max="11291" width="31.33203125" style="36" customWidth="1"/>
-    <col min="11292" max="11501" width="8.83203125" style="36"/>
-    <col min="11502" max="11502" width="1.5" style="36" customWidth="1"/>
-    <col min="11503" max="11503" width="1.33203125" style="36" customWidth="1"/>
-    <col min="11504" max="11504" width="42" style="36" customWidth="1"/>
-    <col min="11505" max="11505" width="5.5" style="36" customWidth="1"/>
-    <col min="11506" max="11507" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="11508" max="11508" width="2.6640625" style="36" customWidth="1"/>
-    <col min="11509" max="11544" width="3.33203125" style="36" customWidth="1"/>
-    <col min="11545" max="11545" width="1.6640625" style="36" customWidth="1"/>
-    <col min="11546" max="11546" width="25.6640625" style="36" customWidth="1"/>
-    <col min="11547" max="11547" width="31.33203125" style="36" customWidth="1"/>
-    <col min="11548" max="11757" width="8.83203125" style="36"/>
-    <col min="11758" max="11758" width="1.5" style="36" customWidth="1"/>
-    <col min="11759" max="11759" width="1.33203125" style="36" customWidth="1"/>
-    <col min="11760" max="11760" width="42" style="36" customWidth="1"/>
-    <col min="11761" max="11761" width="5.5" style="36" customWidth="1"/>
-    <col min="11762" max="11763" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="11764" max="11764" width="2.6640625" style="36" customWidth="1"/>
-    <col min="11765" max="11800" width="3.33203125" style="36" customWidth="1"/>
-    <col min="11801" max="11801" width="1.6640625" style="36" customWidth="1"/>
-    <col min="11802" max="11802" width="25.6640625" style="36" customWidth="1"/>
-    <col min="11803" max="11803" width="31.33203125" style="36" customWidth="1"/>
-    <col min="11804" max="12013" width="8.83203125" style="36"/>
-    <col min="12014" max="12014" width="1.5" style="36" customWidth="1"/>
-    <col min="12015" max="12015" width="1.33203125" style="36" customWidth="1"/>
-    <col min="12016" max="12016" width="42" style="36" customWidth="1"/>
-    <col min="12017" max="12017" width="5.5" style="36" customWidth="1"/>
-    <col min="12018" max="12019" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="12020" max="12020" width="2.6640625" style="36" customWidth="1"/>
-    <col min="12021" max="12056" width="3.33203125" style="36" customWidth="1"/>
-    <col min="12057" max="12057" width="1.6640625" style="36" customWidth="1"/>
-    <col min="12058" max="12058" width="25.6640625" style="36" customWidth="1"/>
-    <col min="12059" max="12059" width="31.33203125" style="36" customWidth="1"/>
-    <col min="12060" max="12269" width="8.83203125" style="36"/>
-    <col min="12270" max="12270" width="1.5" style="36" customWidth="1"/>
-    <col min="12271" max="12271" width="1.33203125" style="36" customWidth="1"/>
-    <col min="12272" max="12272" width="42" style="36" customWidth="1"/>
-    <col min="12273" max="12273" width="5.5" style="36" customWidth="1"/>
-    <col min="12274" max="12275" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="12276" max="12276" width="2.6640625" style="36" customWidth="1"/>
-    <col min="12277" max="12312" width="3.33203125" style="36" customWidth="1"/>
-    <col min="12313" max="12313" width="1.6640625" style="36" customWidth="1"/>
-    <col min="12314" max="12314" width="25.6640625" style="36" customWidth="1"/>
-    <col min="12315" max="12315" width="31.33203125" style="36" customWidth="1"/>
-    <col min="12316" max="12525" width="8.83203125" style="36"/>
-    <col min="12526" max="12526" width="1.5" style="36" customWidth="1"/>
-    <col min="12527" max="12527" width="1.33203125" style="36" customWidth="1"/>
-    <col min="12528" max="12528" width="42" style="36" customWidth="1"/>
-    <col min="12529" max="12529" width="5.5" style="36" customWidth="1"/>
-    <col min="12530" max="12531" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="12532" max="12532" width="2.6640625" style="36" customWidth="1"/>
-    <col min="12533" max="12568" width="3.33203125" style="36" customWidth="1"/>
-    <col min="12569" max="12569" width="1.6640625" style="36" customWidth="1"/>
-    <col min="12570" max="12570" width="25.6640625" style="36" customWidth="1"/>
-    <col min="12571" max="12571" width="31.33203125" style="36" customWidth="1"/>
-    <col min="12572" max="12781" width="8.83203125" style="36"/>
-    <col min="12782" max="12782" width="1.5" style="36" customWidth="1"/>
-    <col min="12783" max="12783" width="1.33203125" style="36" customWidth="1"/>
-    <col min="12784" max="12784" width="42" style="36" customWidth="1"/>
-    <col min="12785" max="12785" width="5.5" style="36" customWidth="1"/>
-    <col min="12786" max="12787" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="12788" max="12788" width="2.6640625" style="36" customWidth="1"/>
-    <col min="12789" max="12824" width="3.33203125" style="36" customWidth="1"/>
-    <col min="12825" max="12825" width="1.6640625" style="36" customWidth="1"/>
-    <col min="12826" max="12826" width="25.6640625" style="36" customWidth="1"/>
-    <col min="12827" max="12827" width="31.33203125" style="36" customWidth="1"/>
-    <col min="12828" max="13037" width="8.83203125" style="36"/>
-    <col min="13038" max="13038" width="1.5" style="36" customWidth="1"/>
-    <col min="13039" max="13039" width="1.33203125" style="36" customWidth="1"/>
-    <col min="13040" max="13040" width="42" style="36" customWidth="1"/>
-    <col min="13041" max="13041" width="5.5" style="36" customWidth="1"/>
-    <col min="13042" max="13043" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="13044" max="13044" width="2.6640625" style="36" customWidth="1"/>
-    <col min="13045" max="13080" width="3.33203125" style="36" customWidth="1"/>
-    <col min="13081" max="13081" width="1.6640625" style="36" customWidth="1"/>
-    <col min="13082" max="13082" width="25.6640625" style="36" customWidth="1"/>
-    <col min="13083" max="13083" width="31.33203125" style="36" customWidth="1"/>
-    <col min="13084" max="13293" width="8.83203125" style="36"/>
-    <col min="13294" max="13294" width="1.5" style="36" customWidth="1"/>
-    <col min="13295" max="13295" width="1.33203125" style="36" customWidth="1"/>
-    <col min="13296" max="13296" width="42" style="36" customWidth="1"/>
-    <col min="13297" max="13297" width="5.5" style="36" customWidth="1"/>
-    <col min="13298" max="13299" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="13300" max="13300" width="2.6640625" style="36" customWidth="1"/>
-    <col min="13301" max="13336" width="3.33203125" style="36" customWidth="1"/>
-    <col min="13337" max="13337" width="1.6640625" style="36" customWidth="1"/>
-    <col min="13338" max="13338" width="25.6640625" style="36" customWidth="1"/>
-    <col min="13339" max="13339" width="31.33203125" style="36" customWidth="1"/>
-    <col min="13340" max="13549" width="8.83203125" style="36"/>
-    <col min="13550" max="13550" width="1.5" style="36" customWidth="1"/>
-    <col min="13551" max="13551" width="1.33203125" style="36" customWidth="1"/>
-    <col min="13552" max="13552" width="42" style="36" customWidth="1"/>
-    <col min="13553" max="13553" width="5.5" style="36" customWidth="1"/>
-    <col min="13554" max="13555" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="13556" max="13556" width="2.6640625" style="36" customWidth="1"/>
-    <col min="13557" max="13592" width="3.33203125" style="36" customWidth="1"/>
-    <col min="13593" max="13593" width="1.6640625" style="36" customWidth="1"/>
-    <col min="13594" max="13594" width="25.6640625" style="36" customWidth="1"/>
-    <col min="13595" max="13595" width="31.33203125" style="36" customWidth="1"/>
-    <col min="13596" max="13805" width="8.83203125" style="36"/>
-    <col min="13806" max="13806" width="1.5" style="36" customWidth="1"/>
-    <col min="13807" max="13807" width="1.33203125" style="36" customWidth="1"/>
-    <col min="13808" max="13808" width="42" style="36" customWidth="1"/>
-    <col min="13809" max="13809" width="5.5" style="36" customWidth="1"/>
-    <col min="13810" max="13811" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="13812" max="13812" width="2.6640625" style="36" customWidth="1"/>
-    <col min="13813" max="13848" width="3.33203125" style="36" customWidth="1"/>
-    <col min="13849" max="13849" width="1.6640625" style="36" customWidth="1"/>
-    <col min="13850" max="13850" width="25.6640625" style="36" customWidth="1"/>
-    <col min="13851" max="13851" width="31.33203125" style="36" customWidth="1"/>
-    <col min="13852" max="14061" width="8.83203125" style="36"/>
-    <col min="14062" max="14062" width="1.5" style="36" customWidth="1"/>
-    <col min="14063" max="14063" width="1.33203125" style="36" customWidth="1"/>
-    <col min="14064" max="14064" width="42" style="36" customWidth="1"/>
-    <col min="14065" max="14065" width="5.5" style="36" customWidth="1"/>
-    <col min="14066" max="14067" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="14068" max="14068" width="2.6640625" style="36" customWidth="1"/>
-    <col min="14069" max="14104" width="3.33203125" style="36" customWidth="1"/>
-    <col min="14105" max="14105" width="1.6640625" style="36" customWidth="1"/>
-    <col min="14106" max="14106" width="25.6640625" style="36" customWidth="1"/>
-    <col min="14107" max="14107" width="31.33203125" style="36" customWidth="1"/>
-    <col min="14108" max="14317" width="8.83203125" style="36"/>
-    <col min="14318" max="14318" width="1.5" style="36" customWidth="1"/>
-    <col min="14319" max="14319" width="1.33203125" style="36" customWidth="1"/>
-    <col min="14320" max="14320" width="42" style="36" customWidth="1"/>
-    <col min="14321" max="14321" width="5.5" style="36" customWidth="1"/>
-    <col min="14322" max="14323" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="14324" max="14324" width="2.6640625" style="36" customWidth="1"/>
-    <col min="14325" max="14360" width="3.33203125" style="36" customWidth="1"/>
-    <col min="14361" max="14361" width="1.6640625" style="36" customWidth="1"/>
-    <col min="14362" max="14362" width="25.6640625" style="36" customWidth="1"/>
-    <col min="14363" max="14363" width="31.33203125" style="36" customWidth="1"/>
-    <col min="14364" max="14573" width="8.83203125" style="36"/>
-    <col min="14574" max="14574" width="1.5" style="36" customWidth="1"/>
-    <col min="14575" max="14575" width="1.33203125" style="36" customWidth="1"/>
-    <col min="14576" max="14576" width="42" style="36" customWidth="1"/>
-    <col min="14577" max="14577" width="5.5" style="36" customWidth="1"/>
-    <col min="14578" max="14579" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="14580" max="14580" width="2.6640625" style="36" customWidth="1"/>
-    <col min="14581" max="14616" width="3.33203125" style="36" customWidth="1"/>
-    <col min="14617" max="14617" width="1.6640625" style="36" customWidth="1"/>
-    <col min="14618" max="14618" width="25.6640625" style="36" customWidth="1"/>
-    <col min="14619" max="14619" width="31.33203125" style="36" customWidth="1"/>
-    <col min="14620" max="14829" width="8.83203125" style="36"/>
-    <col min="14830" max="14830" width="1.5" style="36" customWidth="1"/>
-    <col min="14831" max="14831" width="1.33203125" style="36" customWidth="1"/>
-    <col min="14832" max="14832" width="42" style="36" customWidth="1"/>
-    <col min="14833" max="14833" width="5.5" style="36" customWidth="1"/>
-    <col min="14834" max="14835" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="14836" max="14836" width="2.6640625" style="36" customWidth="1"/>
-    <col min="14837" max="14872" width="3.33203125" style="36" customWidth="1"/>
-    <col min="14873" max="14873" width="1.6640625" style="36" customWidth="1"/>
-    <col min="14874" max="14874" width="25.6640625" style="36" customWidth="1"/>
-    <col min="14875" max="14875" width="31.33203125" style="36" customWidth="1"/>
-    <col min="14876" max="15085" width="8.83203125" style="36"/>
-    <col min="15086" max="15086" width="1.5" style="36" customWidth="1"/>
-    <col min="15087" max="15087" width="1.33203125" style="36" customWidth="1"/>
-    <col min="15088" max="15088" width="42" style="36" customWidth="1"/>
-    <col min="15089" max="15089" width="5.5" style="36" customWidth="1"/>
-    <col min="15090" max="15091" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="15092" max="15092" width="2.6640625" style="36" customWidth="1"/>
-    <col min="15093" max="15128" width="3.33203125" style="36" customWidth="1"/>
-    <col min="15129" max="15129" width="1.6640625" style="36" customWidth="1"/>
-    <col min="15130" max="15130" width="25.6640625" style="36" customWidth="1"/>
-    <col min="15131" max="15131" width="31.33203125" style="36" customWidth="1"/>
-    <col min="15132" max="15341" width="8.83203125" style="36"/>
-    <col min="15342" max="15342" width="1.5" style="36" customWidth="1"/>
-    <col min="15343" max="15343" width="1.33203125" style="36" customWidth="1"/>
-    <col min="15344" max="15344" width="42" style="36" customWidth="1"/>
-    <col min="15345" max="15345" width="5.5" style="36" customWidth="1"/>
-    <col min="15346" max="15347" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="15348" max="15348" width="2.6640625" style="36" customWidth="1"/>
-    <col min="15349" max="15384" width="3.33203125" style="36" customWidth="1"/>
-    <col min="15385" max="15385" width="1.6640625" style="36" customWidth="1"/>
-    <col min="15386" max="15386" width="25.6640625" style="36" customWidth="1"/>
-    <col min="15387" max="15387" width="31.33203125" style="36" customWidth="1"/>
-    <col min="15388" max="15597" width="8.83203125" style="36"/>
-    <col min="15598" max="15598" width="1.5" style="36" customWidth="1"/>
-    <col min="15599" max="15599" width="1.33203125" style="36" customWidth="1"/>
-    <col min="15600" max="15600" width="42" style="36" customWidth="1"/>
-    <col min="15601" max="15601" width="5.5" style="36" customWidth="1"/>
-    <col min="15602" max="15603" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="15604" max="15604" width="2.6640625" style="36" customWidth="1"/>
-    <col min="15605" max="15640" width="3.33203125" style="36" customWidth="1"/>
-    <col min="15641" max="15641" width="1.6640625" style="36" customWidth="1"/>
-    <col min="15642" max="15642" width="25.6640625" style="36" customWidth="1"/>
-    <col min="15643" max="15643" width="31.33203125" style="36" customWidth="1"/>
-    <col min="15644" max="15853" width="8.83203125" style="36"/>
-    <col min="15854" max="15854" width="1.5" style="36" customWidth="1"/>
-    <col min="15855" max="15855" width="1.33203125" style="36" customWidth="1"/>
-    <col min="15856" max="15856" width="42" style="36" customWidth="1"/>
-    <col min="15857" max="15857" width="5.5" style="36" customWidth="1"/>
-    <col min="15858" max="15859" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="15860" max="15860" width="2.6640625" style="36" customWidth="1"/>
-    <col min="15861" max="15896" width="3.33203125" style="36" customWidth="1"/>
-    <col min="15897" max="15897" width="1.6640625" style="36" customWidth="1"/>
-    <col min="15898" max="15898" width="25.6640625" style="36" customWidth="1"/>
-    <col min="15899" max="15899" width="31.33203125" style="36" customWidth="1"/>
-    <col min="15900" max="16109" width="8.83203125" style="36"/>
-    <col min="16110" max="16110" width="1.5" style="36" customWidth="1"/>
-    <col min="16111" max="16111" width="1.33203125" style="36" customWidth="1"/>
-    <col min="16112" max="16112" width="42" style="36" customWidth="1"/>
-    <col min="16113" max="16113" width="5.5" style="36" customWidth="1"/>
-    <col min="16114" max="16115" width="0" style="36" hidden="1" customWidth="1"/>
-    <col min="16116" max="16116" width="2.6640625" style="36" customWidth="1"/>
-    <col min="16117" max="16152" width="3.33203125" style="36" customWidth="1"/>
-    <col min="16153" max="16153" width="1.6640625" style="36" customWidth="1"/>
-    <col min="16154" max="16154" width="25.6640625" style="36" customWidth="1"/>
-    <col min="16155" max="16155" width="31.33203125" style="36" customWidth="1"/>
-    <col min="16156" max="16384" width="8.83203125" style="36"/>
+    <col min="2" max="2" width="7.1640625" style="37" customWidth="1"/>
+    <col min="3" max="3" width="68.5" style="37" customWidth="1"/>
+    <col min="4" max="4" width="8" style="38" customWidth="1"/>
+    <col min="5" max="5" width="14.5" style="38" customWidth="1"/>
+    <col min="6" max="6" width="17.33203125" style="38" customWidth="1"/>
+    <col min="7" max="25" width="3.33203125" style="38" customWidth="1"/>
+    <col min="26" max="26" width="10" style="38" customWidth="1"/>
+    <col min="27" max="35" width="8.83203125" style="38"/>
+    <col min="36" max="236" width="8.83203125" style="36"/>
+    <col min="237" max="237" width="1.5" style="36" customWidth="1"/>
+    <col min="238" max="238" width="1.33203125" style="36" customWidth="1"/>
+    <col min="239" max="239" width="42" style="36" customWidth="1"/>
+    <col min="240" max="240" width="5.5" style="36" customWidth="1"/>
+    <col min="241" max="242" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="243" max="243" width="2.6640625" style="36" customWidth="1"/>
+    <col min="244" max="279" width="3.33203125" style="36" customWidth="1"/>
+    <col min="280" max="280" width="1.6640625" style="36" customWidth="1"/>
+    <col min="281" max="281" width="25.6640625" style="36" customWidth="1"/>
+    <col min="282" max="282" width="31.33203125" style="36" customWidth="1"/>
+    <col min="283" max="492" width="8.83203125" style="36"/>
+    <col min="493" max="493" width="1.5" style="36" customWidth="1"/>
+    <col min="494" max="494" width="1.33203125" style="36" customWidth="1"/>
+    <col min="495" max="495" width="42" style="36" customWidth="1"/>
+    <col min="496" max="496" width="5.5" style="36" customWidth="1"/>
+    <col min="497" max="498" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="499" max="499" width="2.6640625" style="36" customWidth="1"/>
+    <col min="500" max="535" width="3.33203125" style="36" customWidth="1"/>
+    <col min="536" max="536" width="1.6640625" style="36" customWidth="1"/>
+    <col min="537" max="537" width="25.6640625" style="36" customWidth="1"/>
+    <col min="538" max="538" width="31.33203125" style="36" customWidth="1"/>
+    <col min="539" max="748" width="8.83203125" style="36"/>
+    <col min="749" max="749" width="1.5" style="36" customWidth="1"/>
+    <col min="750" max="750" width="1.33203125" style="36" customWidth="1"/>
+    <col min="751" max="751" width="42" style="36" customWidth="1"/>
+    <col min="752" max="752" width="5.5" style="36" customWidth="1"/>
+    <col min="753" max="754" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="755" max="755" width="2.6640625" style="36" customWidth="1"/>
+    <col min="756" max="791" width="3.33203125" style="36" customWidth="1"/>
+    <col min="792" max="792" width="1.6640625" style="36" customWidth="1"/>
+    <col min="793" max="793" width="25.6640625" style="36" customWidth="1"/>
+    <col min="794" max="794" width="31.33203125" style="36" customWidth="1"/>
+    <col min="795" max="1004" width="8.83203125" style="36"/>
+    <col min="1005" max="1005" width="1.5" style="36" customWidth="1"/>
+    <col min="1006" max="1006" width="1.33203125" style="36" customWidth="1"/>
+    <col min="1007" max="1007" width="42" style="36" customWidth="1"/>
+    <col min="1008" max="1008" width="5.5" style="36" customWidth="1"/>
+    <col min="1009" max="1010" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="1011" max="1011" width="2.6640625" style="36" customWidth="1"/>
+    <col min="1012" max="1047" width="3.33203125" style="36" customWidth="1"/>
+    <col min="1048" max="1048" width="1.6640625" style="36" customWidth="1"/>
+    <col min="1049" max="1049" width="25.6640625" style="36" customWidth="1"/>
+    <col min="1050" max="1050" width="31.33203125" style="36" customWidth="1"/>
+    <col min="1051" max="1260" width="8.83203125" style="36"/>
+    <col min="1261" max="1261" width="1.5" style="36" customWidth="1"/>
+    <col min="1262" max="1262" width="1.33203125" style="36" customWidth="1"/>
+    <col min="1263" max="1263" width="42" style="36" customWidth="1"/>
+    <col min="1264" max="1264" width="5.5" style="36" customWidth="1"/>
+    <col min="1265" max="1266" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="1267" max="1267" width="2.6640625" style="36" customWidth="1"/>
+    <col min="1268" max="1303" width="3.33203125" style="36" customWidth="1"/>
+    <col min="1304" max="1304" width="1.6640625" style="36" customWidth="1"/>
+    <col min="1305" max="1305" width="25.6640625" style="36" customWidth="1"/>
+    <col min="1306" max="1306" width="31.33203125" style="36" customWidth="1"/>
+    <col min="1307" max="1516" width="8.83203125" style="36"/>
+    <col min="1517" max="1517" width="1.5" style="36" customWidth="1"/>
+    <col min="1518" max="1518" width="1.33203125" style="36" customWidth="1"/>
+    <col min="1519" max="1519" width="42" style="36" customWidth="1"/>
+    <col min="1520" max="1520" width="5.5" style="36" customWidth="1"/>
+    <col min="1521" max="1522" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="1523" max="1523" width="2.6640625" style="36" customWidth="1"/>
+    <col min="1524" max="1559" width="3.33203125" style="36" customWidth="1"/>
+    <col min="1560" max="1560" width="1.6640625" style="36" customWidth="1"/>
+    <col min="1561" max="1561" width="25.6640625" style="36" customWidth="1"/>
+    <col min="1562" max="1562" width="31.33203125" style="36" customWidth="1"/>
+    <col min="1563" max="1772" width="8.83203125" style="36"/>
+    <col min="1773" max="1773" width="1.5" style="36" customWidth="1"/>
+    <col min="1774" max="1774" width="1.33203125" style="36" customWidth="1"/>
+    <col min="1775" max="1775" width="42" style="36" customWidth="1"/>
+    <col min="1776" max="1776" width="5.5" style="36" customWidth="1"/>
+    <col min="1777" max="1778" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="1779" max="1779" width="2.6640625" style="36" customWidth="1"/>
+    <col min="1780" max="1815" width="3.33203125" style="36" customWidth="1"/>
+    <col min="1816" max="1816" width="1.6640625" style="36" customWidth="1"/>
+    <col min="1817" max="1817" width="25.6640625" style="36" customWidth="1"/>
+    <col min="1818" max="1818" width="31.33203125" style="36" customWidth="1"/>
+    <col min="1819" max="2028" width="8.83203125" style="36"/>
+    <col min="2029" max="2029" width="1.5" style="36" customWidth="1"/>
+    <col min="2030" max="2030" width="1.33203125" style="36" customWidth="1"/>
+    <col min="2031" max="2031" width="42" style="36" customWidth="1"/>
+    <col min="2032" max="2032" width="5.5" style="36" customWidth="1"/>
+    <col min="2033" max="2034" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="2035" max="2035" width="2.6640625" style="36" customWidth="1"/>
+    <col min="2036" max="2071" width="3.33203125" style="36" customWidth="1"/>
+    <col min="2072" max="2072" width="1.6640625" style="36" customWidth="1"/>
+    <col min="2073" max="2073" width="25.6640625" style="36" customWidth="1"/>
+    <col min="2074" max="2074" width="31.33203125" style="36" customWidth="1"/>
+    <col min="2075" max="2284" width="8.83203125" style="36"/>
+    <col min="2285" max="2285" width="1.5" style="36" customWidth="1"/>
+    <col min="2286" max="2286" width="1.33203125" style="36" customWidth="1"/>
+    <col min="2287" max="2287" width="42" style="36" customWidth="1"/>
+    <col min="2288" max="2288" width="5.5" style="36" customWidth="1"/>
+    <col min="2289" max="2290" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="2291" max="2291" width="2.6640625" style="36" customWidth="1"/>
+    <col min="2292" max="2327" width="3.33203125" style="36" customWidth="1"/>
+    <col min="2328" max="2328" width="1.6640625" style="36" customWidth="1"/>
+    <col min="2329" max="2329" width="25.6640625" style="36" customWidth="1"/>
+    <col min="2330" max="2330" width="31.33203125" style="36" customWidth="1"/>
+    <col min="2331" max="2540" width="8.83203125" style="36"/>
+    <col min="2541" max="2541" width="1.5" style="36" customWidth="1"/>
+    <col min="2542" max="2542" width="1.33203125" style="36" customWidth="1"/>
+    <col min="2543" max="2543" width="42" style="36" customWidth="1"/>
+    <col min="2544" max="2544" width="5.5" style="36" customWidth="1"/>
+    <col min="2545" max="2546" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="2547" max="2547" width="2.6640625" style="36" customWidth="1"/>
+    <col min="2548" max="2583" width="3.33203125" style="36" customWidth="1"/>
+    <col min="2584" max="2584" width="1.6640625" style="36" customWidth="1"/>
+    <col min="2585" max="2585" width="25.6640625" style="36" customWidth="1"/>
+    <col min="2586" max="2586" width="31.33203125" style="36" customWidth="1"/>
+    <col min="2587" max="2796" width="8.83203125" style="36"/>
+    <col min="2797" max="2797" width="1.5" style="36" customWidth="1"/>
+    <col min="2798" max="2798" width="1.33203125" style="36" customWidth="1"/>
+    <col min="2799" max="2799" width="42" style="36" customWidth="1"/>
+    <col min="2800" max="2800" width="5.5" style="36" customWidth="1"/>
+    <col min="2801" max="2802" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="2803" max="2803" width="2.6640625" style="36" customWidth="1"/>
+    <col min="2804" max="2839" width="3.33203125" style="36" customWidth="1"/>
+    <col min="2840" max="2840" width="1.6640625" style="36" customWidth="1"/>
+    <col min="2841" max="2841" width="25.6640625" style="36" customWidth="1"/>
+    <col min="2842" max="2842" width="31.33203125" style="36" customWidth="1"/>
+    <col min="2843" max="3052" width="8.83203125" style="36"/>
+    <col min="3053" max="3053" width="1.5" style="36" customWidth="1"/>
+    <col min="3054" max="3054" width="1.33203125" style="36" customWidth="1"/>
+    <col min="3055" max="3055" width="42" style="36" customWidth="1"/>
+    <col min="3056" max="3056" width="5.5" style="36" customWidth="1"/>
+    <col min="3057" max="3058" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="3059" max="3059" width="2.6640625" style="36" customWidth="1"/>
+    <col min="3060" max="3095" width="3.33203125" style="36" customWidth="1"/>
+    <col min="3096" max="3096" width="1.6640625" style="36" customWidth="1"/>
+    <col min="3097" max="3097" width="25.6640625" style="36" customWidth="1"/>
+    <col min="3098" max="3098" width="31.33203125" style="36" customWidth="1"/>
+    <col min="3099" max="3308" width="8.83203125" style="36"/>
+    <col min="3309" max="3309" width="1.5" style="36" customWidth="1"/>
+    <col min="3310" max="3310" width="1.33203125" style="36" customWidth="1"/>
+    <col min="3311" max="3311" width="42" style="36" customWidth="1"/>
+    <col min="3312" max="3312" width="5.5" style="36" customWidth="1"/>
+    <col min="3313" max="3314" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="3315" max="3315" width="2.6640625" style="36" customWidth="1"/>
+    <col min="3316" max="3351" width="3.33203125" style="36" customWidth="1"/>
+    <col min="3352" max="3352" width="1.6640625" style="36" customWidth="1"/>
+    <col min="3353" max="3353" width="25.6640625" style="36" customWidth="1"/>
+    <col min="3354" max="3354" width="31.33203125" style="36" customWidth="1"/>
+    <col min="3355" max="3564" width="8.83203125" style="36"/>
+    <col min="3565" max="3565" width="1.5" style="36" customWidth="1"/>
+    <col min="3566" max="3566" width="1.33203125" style="36" customWidth="1"/>
+    <col min="3567" max="3567" width="42" style="36" customWidth="1"/>
+    <col min="3568" max="3568" width="5.5" style="36" customWidth="1"/>
+    <col min="3569" max="3570" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="3571" max="3571" width="2.6640625" style="36" customWidth="1"/>
+    <col min="3572" max="3607" width="3.33203125" style="36" customWidth="1"/>
+    <col min="3608" max="3608" width="1.6640625" style="36" customWidth="1"/>
+    <col min="3609" max="3609" width="25.6640625" style="36" customWidth="1"/>
+    <col min="3610" max="3610" width="31.33203125" style="36" customWidth="1"/>
+    <col min="3611" max="3820" width="8.83203125" style="36"/>
+    <col min="3821" max="3821" width="1.5" style="36" customWidth="1"/>
+    <col min="3822" max="3822" width="1.33203125" style="36" customWidth="1"/>
+    <col min="3823" max="3823" width="42" style="36" customWidth="1"/>
+    <col min="3824" max="3824" width="5.5" style="36" customWidth="1"/>
+    <col min="3825" max="3826" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="3827" max="3827" width="2.6640625" style="36" customWidth="1"/>
+    <col min="3828" max="3863" width="3.33203125" style="36" customWidth="1"/>
+    <col min="3864" max="3864" width="1.6640625" style="36" customWidth="1"/>
+    <col min="3865" max="3865" width="25.6640625" style="36" customWidth="1"/>
+    <col min="3866" max="3866" width="31.33203125" style="36" customWidth="1"/>
+    <col min="3867" max="4076" width="8.83203125" style="36"/>
+    <col min="4077" max="4077" width="1.5" style="36" customWidth="1"/>
+    <col min="4078" max="4078" width="1.33203125" style="36" customWidth="1"/>
+    <col min="4079" max="4079" width="42" style="36" customWidth="1"/>
+    <col min="4080" max="4080" width="5.5" style="36" customWidth="1"/>
+    <col min="4081" max="4082" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="4083" max="4083" width="2.6640625" style="36" customWidth="1"/>
+    <col min="4084" max="4119" width="3.33203125" style="36" customWidth="1"/>
+    <col min="4120" max="4120" width="1.6640625" style="36" customWidth="1"/>
+    <col min="4121" max="4121" width="25.6640625" style="36" customWidth="1"/>
+    <col min="4122" max="4122" width="31.33203125" style="36" customWidth="1"/>
+    <col min="4123" max="4332" width="8.83203125" style="36"/>
+    <col min="4333" max="4333" width="1.5" style="36" customWidth="1"/>
+    <col min="4334" max="4334" width="1.33203125" style="36" customWidth="1"/>
+    <col min="4335" max="4335" width="42" style="36" customWidth="1"/>
+    <col min="4336" max="4336" width="5.5" style="36" customWidth="1"/>
+    <col min="4337" max="4338" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="4339" max="4339" width="2.6640625" style="36" customWidth="1"/>
+    <col min="4340" max="4375" width="3.33203125" style="36" customWidth="1"/>
+    <col min="4376" max="4376" width="1.6640625" style="36" customWidth="1"/>
+    <col min="4377" max="4377" width="25.6640625" style="36" customWidth="1"/>
+    <col min="4378" max="4378" width="31.33203125" style="36" customWidth="1"/>
+    <col min="4379" max="4588" width="8.83203125" style="36"/>
+    <col min="4589" max="4589" width="1.5" style="36" customWidth="1"/>
+    <col min="4590" max="4590" width="1.33203125" style="36" customWidth="1"/>
+    <col min="4591" max="4591" width="42" style="36" customWidth="1"/>
+    <col min="4592" max="4592" width="5.5" style="36" customWidth="1"/>
+    <col min="4593" max="4594" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="4595" max="4595" width="2.6640625" style="36" customWidth="1"/>
+    <col min="4596" max="4631" width="3.33203125" style="36" customWidth="1"/>
+    <col min="4632" max="4632" width="1.6640625" style="36" customWidth="1"/>
+    <col min="4633" max="4633" width="25.6640625" style="36" customWidth="1"/>
+    <col min="4634" max="4634" width="31.33203125" style="36" customWidth="1"/>
+    <col min="4635" max="4844" width="8.83203125" style="36"/>
+    <col min="4845" max="4845" width="1.5" style="36" customWidth="1"/>
+    <col min="4846" max="4846" width="1.33203125" style="36" customWidth="1"/>
+    <col min="4847" max="4847" width="42" style="36" customWidth="1"/>
+    <col min="4848" max="4848" width="5.5" style="36" customWidth="1"/>
+    <col min="4849" max="4850" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="4851" max="4851" width="2.6640625" style="36" customWidth="1"/>
+    <col min="4852" max="4887" width="3.33203125" style="36" customWidth="1"/>
+    <col min="4888" max="4888" width="1.6640625" style="36" customWidth="1"/>
+    <col min="4889" max="4889" width="25.6640625" style="36" customWidth="1"/>
+    <col min="4890" max="4890" width="31.33203125" style="36" customWidth="1"/>
+    <col min="4891" max="5100" width="8.83203125" style="36"/>
+    <col min="5101" max="5101" width="1.5" style="36" customWidth="1"/>
+    <col min="5102" max="5102" width="1.33203125" style="36" customWidth="1"/>
+    <col min="5103" max="5103" width="42" style="36" customWidth="1"/>
+    <col min="5104" max="5104" width="5.5" style="36" customWidth="1"/>
+    <col min="5105" max="5106" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="5107" max="5107" width="2.6640625" style="36" customWidth="1"/>
+    <col min="5108" max="5143" width="3.33203125" style="36" customWidth="1"/>
+    <col min="5144" max="5144" width="1.6640625" style="36" customWidth="1"/>
+    <col min="5145" max="5145" width="25.6640625" style="36" customWidth="1"/>
+    <col min="5146" max="5146" width="31.33203125" style="36" customWidth="1"/>
+    <col min="5147" max="5356" width="8.83203125" style="36"/>
+    <col min="5357" max="5357" width="1.5" style="36" customWidth="1"/>
+    <col min="5358" max="5358" width="1.33203125" style="36" customWidth="1"/>
+    <col min="5359" max="5359" width="42" style="36" customWidth="1"/>
+    <col min="5360" max="5360" width="5.5" style="36" customWidth="1"/>
+    <col min="5361" max="5362" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="5363" max="5363" width="2.6640625" style="36" customWidth="1"/>
+    <col min="5364" max="5399" width="3.33203125" style="36" customWidth="1"/>
+    <col min="5400" max="5400" width="1.6640625" style="36" customWidth="1"/>
+    <col min="5401" max="5401" width="25.6640625" style="36" customWidth="1"/>
+    <col min="5402" max="5402" width="31.33203125" style="36" customWidth="1"/>
+    <col min="5403" max="5612" width="8.83203125" style="36"/>
+    <col min="5613" max="5613" width="1.5" style="36" customWidth="1"/>
+    <col min="5614" max="5614" width="1.33203125" style="36" customWidth="1"/>
+    <col min="5615" max="5615" width="42" style="36" customWidth="1"/>
+    <col min="5616" max="5616" width="5.5" style="36" customWidth="1"/>
+    <col min="5617" max="5618" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="5619" max="5619" width="2.6640625" style="36" customWidth="1"/>
+    <col min="5620" max="5655" width="3.33203125" style="36" customWidth="1"/>
+    <col min="5656" max="5656" width="1.6640625" style="36" customWidth="1"/>
+    <col min="5657" max="5657" width="25.6640625" style="36" customWidth="1"/>
+    <col min="5658" max="5658" width="31.33203125" style="36" customWidth="1"/>
+    <col min="5659" max="5868" width="8.83203125" style="36"/>
+    <col min="5869" max="5869" width="1.5" style="36" customWidth="1"/>
+    <col min="5870" max="5870" width="1.33203125" style="36" customWidth="1"/>
+    <col min="5871" max="5871" width="42" style="36" customWidth="1"/>
+    <col min="5872" max="5872" width="5.5" style="36" customWidth="1"/>
+    <col min="5873" max="5874" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="5875" max="5875" width="2.6640625" style="36" customWidth="1"/>
+    <col min="5876" max="5911" width="3.33203125" style="36" customWidth="1"/>
+    <col min="5912" max="5912" width="1.6640625" style="36" customWidth="1"/>
+    <col min="5913" max="5913" width="25.6640625" style="36" customWidth="1"/>
+    <col min="5914" max="5914" width="31.33203125" style="36" customWidth="1"/>
+    <col min="5915" max="6124" width="8.83203125" style="36"/>
+    <col min="6125" max="6125" width="1.5" style="36" customWidth="1"/>
+    <col min="6126" max="6126" width="1.33203125" style="36" customWidth="1"/>
+    <col min="6127" max="6127" width="42" style="36" customWidth="1"/>
+    <col min="6128" max="6128" width="5.5" style="36" customWidth="1"/>
+    <col min="6129" max="6130" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="6131" max="6131" width="2.6640625" style="36" customWidth="1"/>
+    <col min="6132" max="6167" width="3.33203125" style="36" customWidth="1"/>
+    <col min="6168" max="6168" width="1.6640625" style="36" customWidth="1"/>
+    <col min="6169" max="6169" width="25.6640625" style="36" customWidth="1"/>
+    <col min="6170" max="6170" width="31.33203125" style="36" customWidth="1"/>
+    <col min="6171" max="6380" width="8.83203125" style="36"/>
+    <col min="6381" max="6381" width="1.5" style="36" customWidth="1"/>
+    <col min="6382" max="6382" width="1.33203125" style="36" customWidth="1"/>
+    <col min="6383" max="6383" width="42" style="36" customWidth="1"/>
+    <col min="6384" max="6384" width="5.5" style="36" customWidth="1"/>
+    <col min="6385" max="6386" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="6387" max="6387" width="2.6640625" style="36" customWidth="1"/>
+    <col min="6388" max="6423" width="3.33203125" style="36" customWidth="1"/>
+    <col min="6424" max="6424" width="1.6640625" style="36" customWidth="1"/>
+    <col min="6425" max="6425" width="25.6640625" style="36" customWidth="1"/>
+    <col min="6426" max="6426" width="31.33203125" style="36" customWidth="1"/>
+    <col min="6427" max="6636" width="8.83203125" style="36"/>
+    <col min="6637" max="6637" width="1.5" style="36" customWidth="1"/>
+    <col min="6638" max="6638" width="1.33203125" style="36" customWidth="1"/>
+    <col min="6639" max="6639" width="42" style="36" customWidth="1"/>
+    <col min="6640" max="6640" width="5.5" style="36" customWidth="1"/>
+    <col min="6641" max="6642" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="6643" max="6643" width="2.6640625" style="36" customWidth="1"/>
+    <col min="6644" max="6679" width="3.33203125" style="36" customWidth="1"/>
+    <col min="6680" max="6680" width="1.6640625" style="36" customWidth="1"/>
+    <col min="6681" max="6681" width="25.6640625" style="36" customWidth="1"/>
+    <col min="6682" max="6682" width="31.33203125" style="36" customWidth="1"/>
+    <col min="6683" max="6892" width="8.83203125" style="36"/>
+    <col min="6893" max="6893" width="1.5" style="36" customWidth="1"/>
+    <col min="6894" max="6894" width="1.33203125" style="36" customWidth="1"/>
+    <col min="6895" max="6895" width="42" style="36" customWidth="1"/>
+    <col min="6896" max="6896" width="5.5" style="36" customWidth="1"/>
+    <col min="6897" max="6898" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="6899" max="6899" width="2.6640625" style="36" customWidth="1"/>
+    <col min="6900" max="6935" width="3.33203125" style="36" customWidth="1"/>
+    <col min="6936" max="6936" width="1.6640625" style="36" customWidth="1"/>
+    <col min="6937" max="6937" width="25.6640625" style="36" customWidth="1"/>
+    <col min="6938" max="6938" width="31.33203125" style="36" customWidth="1"/>
+    <col min="6939" max="7148" width="8.83203125" style="36"/>
+    <col min="7149" max="7149" width="1.5" style="36" customWidth="1"/>
+    <col min="7150" max="7150" width="1.33203125" style="36" customWidth="1"/>
+    <col min="7151" max="7151" width="42" style="36" customWidth="1"/>
+    <col min="7152" max="7152" width="5.5" style="36" customWidth="1"/>
+    <col min="7153" max="7154" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="7155" max="7155" width="2.6640625" style="36" customWidth="1"/>
+    <col min="7156" max="7191" width="3.33203125" style="36" customWidth="1"/>
+    <col min="7192" max="7192" width="1.6640625" style="36" customWidth="1"/>
+    <col min="7193" max="7193" width="25.6640625" style="36" customWidth="1"/>
+    <col min="7194" max="7194" width="31.33203125" style="36" customWidth="1"/>
+    <col min="7195" max="7404" width="8.83203125" style="36"/>
+    <col min="7405" max="7405" width="1.5" style="36" customWidth="1"/>
+    <col min="7406" max="7406" width="1.33203125" style="36" customWidth="1"/>
+    <col min="7407" max="7407" width="42" style="36" customWidth="1"/>
+    <col min="7408" max="7408" width="5.5" style="36" customWidth="1"/>
+    <col min="7409" max="7410" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="7411" max="7411" width="2.6640625" style="36" customWidth="1"/>
+    <col min="7412" max="7447" width="3.33203125" style="36" customWidth="1"/>
+    <col min="7448" max="7448" width="1.6640625" style="36" customWidth="1"/>
+    <col min="7449" max="7449" width="25.6640625" style="36" customWidth="1"/>
+    <col min="7450" max="7450" width="31.33203125" style="36" customWidth="1"/>
+    <col min="7451" max="7660" width="8.83203125" style="36"/>
+    <col min="7661" max="7661" width="1.5" style="36" customWidth="1"/>
+    <col min="7662" max="7662" width="1.33203125" style="36" customWidth="1"/>
+    <col min="7663" max="7663" width="42" style="36" customWidth="1"/>
+    <col min="7664" max="7664" width="5.5" style="36" customWidth="1"/>
+    <col min="7665" max="7666" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="7667" max="7667" width="2.6640625" style="36" customWidth="1"/>
+    <col min="7668" max="7703" width="3.33203125" style="36" customWidth="1"/>
+    <col min="7704" max="7704" width="1.6640625" style="36" customWidth="1"/>
+    <col min="7705" max="7705" width="25.6640625" style="36" customWidth="1"/>
+    <col min="7706" max="7706" width="31.33203125" style="36" customWidth="1"/>
+    <col min="7707" max="7916" width="8.83203125" style="36"/>
+    <col min="7917" max="7917" width="1.5" style="36" customWidth="1"/>
+    <col min="7918" max="7918" width="1.33203125" style="36" customWidth="1"/>
+    <col min="7919" max="7919" width="42" style="36" customWidth="1"/>
+    <col min="7920" max="7920" width="5.5" style="36" customWidth="1"/>
+    <col min="7921" max="7922" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="7923" max="7923" width="2.6640625" style="36" customWidth="1"/>
+    <col min="7924" max="7959" width="3.33203125" style="36" customWidth="1"/>
+    <col min="7960" max="7960" width="1.6640625" style="36" customWidth="1"/>
+    <col min="7961" max="7961" width="25.6640625" style="36" customWidth="1"/>
+    <col min="7962" max="7962" width="31.33203125" style="36" customWidth="1"/>
+    <col min="7963" max="8172" width="8.83203125" style="36"/>
+    <col min="8173" max="8173" width="1.5" style="36" customWidth="1"/>
+    <col min="8174" max="8174" width="1.33203125" style="36" customWidth="1"/>
+    <col min="8175" max="8175" width="42" style="36" customWidth="1"/>
+    <col min="8176" max="8176" width="5.5" style="36" customWidth="1"/>
+    <col min="8177" max="8178" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="8179" max="8179" width="2.6640625" style="36" customWidth="1"/>
+    <col min="8180" max="8215" width="3.33203125" style="36" customWidth="1"/>
+    <col min="8216" max="8216" width="1.6640625" style="36" customWidth="1"/>
+    <col min="8217" max="8217" width="25.6640625" style="36" customWidth="1"/>
+    <col min="8218" max="8218" width="31.33203125" style="36" customWidth="1"/>
+    <col min="8219" max="8428" width="8.83203125" style="36"/>
+    <col min="8429" max="8429" width="1.5" style="36" customWidth="1"/>
+    <col min="8430" max="8430" width="1.33203125" style="36" customWidth="1"/>
+    <col min="8431" max="8431" width="42" style="36" customWidth="1"/>
+    <col min="8432" max="8432" width="5.5" style="36" customWidth="1"/>
+    <col min="8433" max="8434" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="8435" max="8435" width="2.6640625" style="36" customWidth="1"/>
+    <col min="8436" max="8471" width="3.33203125" style="36" customWidth="1"/>
+    <col min="8472" max="8472" width="1.6640625" style="36" customWidth="1"/>
+    <col min="8473" max="8473" width="25.6640625" style="36" customWidth="1"/>
+    <col min="8474" max="8474" width="31.33203125" style="36" customWidth="1"/>
+    <col min="8475" max="8684" width="8.83203125" style="36"/>
+    <col min="8685" max="8685" width="1.5" style="36" customWidth="1"/>
+    <col min="8686" max="8686" width="1.33203125" style="36" customWidth="1"/>
+    <col min="8687" max="8687" width="42" style="36" customWidth="1"/>
+    <col min="8688" max="8688" width="5.5" style="36" customWidth="1"/>
+    <col min="8689" max="8690" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="8691" max="8691" width="2.6640625" style="36" customWidth="1"/>
+    <col min="8692" max="8727" width="3.33203125" style="36" customWidth="1"/>
+    <col min="8728" max="8728" width="1.6640625" style="36" customWidth="1"/>
+    <col min="8729" max="8729" width="25.6640625" style="36" customWidth="1"/>
+    <col min="8730" max="8730" width="31.33203125" style="36" customWidth="1"/>
+    <col min="8731" max="8940" width="8.83203125" style="36"/>
+    <col min="8941" max="8941" width="1.5" style="36" customWidth="1"/>
+    <col min="8942" max="8942" width="1.33203125" style="36" customWidth="1"/>
+    <col min="8943" max="8943" width="42" style="36" customWidth="1"/>
+    <col min="8944" max="8944" width="5.5" style="36" customWidth="1"/>
+    <col min="8945" max="8946" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="8947" max="8947" width="2.6640625" style="36" customWidth="1"/>
+    <col min="8948" max="8983" width="3.33203125" style="36" customWidth="1"/>
+    <col min="8984" max="8984" width="1.6640625" style="36" customWidth="1"/>
+    <col min="8985" max="8985" width="25.6640625" style="36" customWidth="1"/>
+    <col min="8986" max="8986" width="31.33203125" style="36" customWidth="1"/>
+    <col min="8987" max="9196" width="8.83203125" style="36"/>
+    <col min="9197" max="9197" width="1.5" style="36" customWidth="1"/>
+    <col min="9198" max="9198" width="1.33203125" style="36" customWidth="1"/>
+    <col min="9199" max="9199" width="42" style="36" customWidth="1"/>
+    <col min="9200" max="9200" width="5.5" style="36" customWidth="1"/>
+    <col min="9201" max="9202" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="9203" max="9203" width="2.6640625" style="36" customWidth="1"/>
+    <col min="9204" max="9239" width="3.33203125" style="36" customWidth="1"/>
+    <col min="9240" max="9240" width="1.6640625" style="36" customWidth="1"/>
+    <col min="9241" max="9241" width="25.6640625" style="36" customWidth="1"/>
+    <col min="9242" max="9242" width="31.33203125" style="36" customWidth="1"/>
+    <col min="9243" max="9452" width="8.83203125" style="36"/>
+    <col min="9453" max="9453" width="1.5" style="36" customWidth="1"/>
+    <col min="9454" max="9454" width="1.33203125" style="36" customWidth="1"/>
+    <col min="9455" max="9455" width="42" style="36" customWidth="1"/>
+    <col min="9456" max="9456" width="5.5" style="36" customWidth="1"/>
+    <col min="9457" max="9458" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="9459" max="9459" width="2.6640625" style="36" customWidth="1"/>
+    <col min="9460" max="9495" width="3.33203125" style="36" customWidth="1"/>
+    <col min="9496" max="9496" width="1.6640625" style="36" customWidth="1"/>
+    <col min="9497" max="9497" width="25.6640625" style="36" customWidth="1"/>
+    <col min="9498" max="9498" width="31.33203125" style="36" customWidth="1"/>
+    <col min="9499" max="9708" width="8.83203125" style="36"/>
+    <col min="9709" max="9709" width="1.5" style="36" customWidth="1"/>
+    <col min="9710" max="9710" width="1.33203125" style="36" customWidth="1"/>
+    <col min="9711" max="9711" width="42" style="36" customWidth="1"/>
+    <col min="9712" max="9712" width="5.5" style="36" customWidth="1"/>
+    <col min="9713" max="9714" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="9715" max="9715" width="2.6640625" style="36" customWidth="1"/>
+    <col min="9716" max="9751" width="3.33203125" style="36" customWidth="1"/>
+    <col min="9752" max="9752" width="1.6640625" style="36" customWidth="1"/>
+    <col min="9753" max="9753" width="25.6640625" style="36" customWidth="1"/>
+    <col min="9754" max="9754" width="31.33203125" style="36" customWidth="1"/>
+    <col min="9755" max="9964" width="8.83203125" style="36"/>
+    <col min="9965" max="9965" width="1.5" style="36" customWidth="1"/>
+    <col min="9966" max="9966" width="1.33203125" style="36" customWidth="1"/>
+    <col min="9967" max="9967" width="42" style="36" customWidth="1"/>
+    <col min="9968" max="9968" width="5.5" style="36" customWidth="1"/>
+    <col min="9969" max="9970" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="9971" max="9971" width="2.6640625" style="36" customWidth="1"/>
+    <col min="9972" max="10007" width="3.33203125" style="36" customWidth="1"/>
+    <col min="10008" max="10008" width="1.6640625" style="36" customWidth="1"/>
+    <col min="10009" max="10009" width="25.6640625" style="36" customWidth="1"/>
+    <col min="10010" max="10010" width="31.33203125" style="36" customWidth="1"/>
+    <col min="10011" max="10220" width="8.83203125" style="36"/>
+    <col min="10221" max="10221" width="1.5" style="36" customWidth="1"/>
+    <col min="10222" max="10222" width="1.33203125" style="36" customWidth="1"/>
+    <col min="10223" max="10223" width="42" style="36" customWidth="1"/>
+    <col min="10224" max="10224" width="5.5" style="36" customWidth="1"/>
+    <col min="10225" max="10226" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="10227" max="10227" width="2.6640625" style="36" customWidth="1"/>
+    <col min="10228" max="10263" width="3.33203125" style="36" customWidth="1"/>
+    <col min="10264" max="10264" width="1.6640625" style="36" customWidth="1"/>
+    <col min="10265" max="10265" width="25.6640625" style="36" customWidth="1"/>
+    <col min="10266" max="10266" width="31.33203125" style="36" customWidth="1"/>
+    <col min="10267" max="10476" width="8.83203125" style="36"/>
+    <col min="10477" max="10477" width="1.5" style="36" customWidth="1"/>
+    <col min="10478" max="10478" width="1.33203125" style="36" customWidth="1"/>
+    <col min="10479" max="10479" width="42" style="36" customWidth="1"/>
+    <col min="10480" max="10480" width="5.5" style="36" customWidth="1"/>
+    <col min="10481" max="10482" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="10483" max="10483" width="2.6640625" style="36" customWidth="1"/>
+    <col min="10484" max="10519" width="3.33203125" style="36" customWidth="1"/>
+    <col min="10520" max="10520" width="1.6640625" style="36" customWidth="1"/>
+    <col min="10521" max="10521" width="25.6640625" style="36" customWidth="1"/>
+    <col min="10522" max="10522" width="31.33203125" style="36" customWidth="1"/>
+    <col min="10523" max="10732" width="8.83203125" style="36"/>
+    <col min="10733" max="10733" width="1.5" style="36" customWidth="1"/>
+    <col min="10734" max="10734" width="1.33203125" style="36" customWidth="1"/>
+    <col min="10735" max="10735" width="42" style="36" customWidth="1"/>
+    <col min="10736" max="10736" width="5.5" style="36" customWidth="1"/>
+    <col min="10737" max="10738" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="10739" max="10739" width="2.6640625" style="36" customWidth="1"/>
+    <col min="10740" max="10775" width="3.33203125" style="36" customWidth="1"/>
+    <col min="10776" max="10776" width="1.6640625" style="36" customWidth="1"/>
+    <col min="10777" max="10777" width="25.6640625" style="36" customWidth="1"/>
+    <col min="10778" max="10778" width="31.33203125" style="36" customWidth="1"/>
+    <col min="10779" max="10988" width="8.83203125" style="36"/>
+    <col min="10989" max="10989" width="1.5" style="36" customWidth="1"/>
+    <col min="10990" max="10990" width="1.33203125" style="36" customWidth="1"/>
+    <col min="10991" max="10991" width="42" style="36" customWidth="1"/>
+    <col min="10992" max="10992" width="5.5" style="36" customWidth="1"/>
+    <col min="10993" max="10994" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="10995" max="10995" width="2.6640625" style="36" customWidth="1"/>
+    <col min="10996" max="11031" width="3.33203125" style="36" customWidth="1"/>
+    <col min="11032" max="11032" width="1.6640625" style="36" customWidth="1"/>
+    <col min="11033" max="11033" width="25.6640625" style="36" customWidth="1"/>
+    <col min="11034" max="11034" width="31.33203125" style="36" customWidth="1"/>
+    <col min="11035" max="11244" width="8.83203125" style="36"/>
+    <col min="11245" max="11245" width="1.5" style="36" customWidth="1"/>
+    <col min="11246" max="11246" width="1.33203125" style="36" customWidth="1"/>
+    <col min="11247" max="11247" width="42" style="36" customWidth="1"/>
+    <col min="11248" max="11248" width="5.5" style="36" customWidth="1"/>
+    <col min="11249" max="11250" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="11251" max="11251" width="2.6640625" style="36" customWidth="1"/>
+    <col min="11252" max="11287" width="3.33203125" style="36" customWidth="1"/>
+    <col min="11288" max="11288" width="1.6640625" style="36" customWidth="1"/>
+    <col min="11289" max="11289" width="25.6640625" style="36" customWidth="1"/>
+    <col min="11290" max="11290" width="31.33203125" style="36" customWidth="1"/>
+    <col min="11291" max="11500" width="8.83203125" style="36"/>
+    <col min="11501" max="11501" width="1.5" style="36" customWidth="1"/>
+    <col min="11502" max="11502" width="1.33203125" style="36" customWidth="1"/>
+    <col min="11503" max="11503" width="42" style="36" customWidth="1"/>
+    <col min="11504" max="11504" width="5.5" style="36" customWidth="1"/>
+    <col min="11505" max="11506" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="11507" max="11507" width="2.6640625" style="36" customWidth="1"/>
+    <col min="11508" max="11543" width="3.33203125" style="36" customWidth="1"/>
+    <col min="11544" max="11544" width="1.6640625" style="36" customWidth="1"/>
+    <col min="11545" max="11545" width="25.6640625" style="36" customWidth="1"/>
+    <col min="11546" max="11546" width="31.33203125" style="36" customWidth="1"/>
+    <col min="11547" max="11756" width="8.83203125" style="36"/>
+    <col min="11757" max="11757" width="1.5" style="36" customWidth="1"/>
+    <col min="11758" max="11758" width="1.33203125" style="36" customWidth="1"/>
+    <col min="11759" max="11759" width="42" style="36" customWidth="1"/>
+    <col min="11760" max="11760" width="5.5" style="36" customWidth="1"/>
+    <col min="11761" max="11762" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="11763" max="11763" width="2.6640625" style="36" customWidth="1"/>
+    <col min="11764" max="11799" width="3.33203125" style="36" customWidth="1"/>
+    <col min="11800" max="11800" width="1.6640625" style="36" customWidth="1"/>
+    <col min="11801" max="11801" width="25.6640625" style="36" customWidth="1"/>
+    <col min="11802" max="11802" width="31.33203125" style="36" customWidth="1"/>
+    <col min="11803" max="12012" width="8.83203125" style="36"/>
+    <col min="12013" max="12013" width="1.5" style="36" customWidth="1"/>
+    <col min="12014" max="12014" width="1.33203125" style="36" customWidth="1"/>
+    <col min="12015" max="12015" width="42" style="36" customWidth="1"/>
+    <col min="12016" max="12016" width="5.5" style="36" customWidth="1"/>
+    <col min="12017" max="12018" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="12019" max="12019" width="2.6640625" style="36" customWidth="1"/>
+    <col min="12020" max="12055" width="3.33203125" style="36" customWidth="1"/>
+    <col min="12056" max="12056" width="1.6640625" style="36" customWidth="1"/>
+    <col min="12057" max="12057" width="25.6640625" style="36" customWidth="1"/>
+    <col min="12058" max="12058" width="31.33203125" style="36" customWidth="1"/>
+    <col min="12059" max="12268" width="8.83203125" style="36"/>
+    <col min="12269" max="12269" width="1.5" style="36" customWidth="1"/>
+    <col min="12270" max="12270" width="1.33203125" style="36" customWidth="1"/>
+    <col min="12271" max="12271" width="42" style="36" customWidth="1"/>
+    <col min="12272" max="12272" width="5.5" style="36" customWidth="1"/>
+    <col min="12273" max="12274" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="12275" max="12275" width="2.6640625" style="36" customWidth="1"/>
+    <col min="12276" max="12311" width="3.33203125" style="36" customWidth="1"/>
+    <col min="12312" max="12312" width="1.6640625" style="36" customWidth="1"/>
+    <col min="12313" max="12313" width="25.6640625" style="36" customWidth="1"/>
+    <col min="12314" max="12314" width="31.33203125" style="36" customWidth="1"/>
+    <col min="12315" max="12524" width="8.83203125" style="36"/>
+    <col min="12525" max="12525" width="1.5" style="36" customWidth="1"/>
+    <col min="12526" max="12526" width="1.33203125" style="36" customWidth="1"/>
+    <col min="12527" max="12527" width="42" style="36" customWidth="1"/>
+    <col min="12528" max="12528" width="5.5" style="36" customWidth="1"/>
+    <col min="12529" max="12530" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="12531" max="12531" width="2.6640625" style="36" customWidth="1"/>
+    <col min="12532" max="12567" width="3.33203125" style="36" customWidth="1"/>
+    <col min="12568" max="12568" width="1.6640625" style="36" customWidth="1"/>
+    <col min="12569" max="12569" width="25.6640625" style="36" customWidth="1"/>
+    <col min="12570" max="12570" width="31.33203125" style="36" customWidth="1"/>
+    <col min="12571" max="12780" width="8.83203125" style="36"/>
+    <col min="12781" max="12781" width="1.5" style="36" customWidth="1"/>
+    <col min="12782" max="12782" width="1.33203125" style="36" customWidth="1"/>
+    <col min="12783" max="12783" width="42" style="36" customWidth="1"/>
+    <col min="12784" max="12784" width="5.5" style="36" customWidth="1"/>
+    <col min="12785" max="12786" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="12787" max="12787" width="2.6640625" style="36" customWidth="1"/>
+    <col min="12788" max="12823" width="3.33203125" style="36" customWidth="1"/>
+    <col min="12824" max="12824" width="1.6640625" style="36" customWidth="1"/>
+    <col min="12825" max="12825" width="25.6640625" style="36" customWidth="1"/>
+    <col min="12826" max="12826" width="31.33203125" style="36" customWidth="1"/>
+    <col min="12827" max="13036" width="8.83203125" style="36"/>
+    <col min="13037" max="13037" width="1.5" style="36" customWidth="1"/>
+    <col min="13038" max="13038" width="1.33203125" style="36" customWidth="1"/>
+    <col min="13039" max="13039" width="42" style="36" customWidth="1"/>
+    <col min="13040" max="13040" width="5.5" style="36" customWidth="1"/>
+    <col min="13041" max="13042" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="13043" max="13043" width="2.6640625" style="36" customWidth="1"/>
+    <col min="13044" max="13079" width="3.33203125" style="36" customWidth="1"/>
+    <col min="13080" max="13080" width="1.6640625" style="36" customWidth="1"/>
+    <col min="13081" max="13081" width="25.6640625" style="36" customWidth="1"/>
+    <col min="13082" max="13082" width="31.33203125" style="36" customWidth="1"/>
+    <col min="13083" max="13292" width="8.83203125" style="36"/>
+    <col min="13293" max="13293" width="1.5" style="36" customWidth="1"/>
+    <col min="13294" max="13294" width="1.33203125" style="36" customWidth="1"/>
+    <col min="13295" max="13295" width="42" style="36" customWidth="1"/>
+    <col min="13296" max="13296" width="5.5" style="36" customWidth="1"/>
+    <col min="13297" max="13298" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="13299" max="13299" width="2.6640625" style="36" customWidth="1"/>
+    <col min="13300" max="13335" width="3.33203125" style="36" customWidth="1"/>
+    <col min="13336" max="13336" width="1.6640625" style="36" customWidth="1"/>
+    <col min="13337" max="13337" width="25.6640625" style="36" customWidth="1"/>
+    <col min="13338" max="13338" width="31.33203125" style="36" customWidth="1"/>
+    <col min="13339" max="13548" width="8.83203125" style="36"/>
+    <col min="13549" max="13549" width="1.5" style="36" customWidth="1"/>
+    <col min="13550" max="13550" width="1.33203125" style="36" customWidth="1"/>
+    <col min="13551" max="13551" width="42" style="36" customWidth="1"/>
+    <col min="13552" max="13552" width="5.5" style="36" customWidth="1"/>
+    <col min="13553" max="13554" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="13555" max="13555" width="2.6640625" style="36" customWidth="1"/>
+    <col min="13556" max="13591" width="3.33203125" style="36" customWidth="1"/>
+    <col min="13592" max="13592" width="1.6640625" style="36" customWidth="1"/>
+    <col min="13593" max="13593" width="25.6640625" style="36" customWidth="1"/>
+    <col min="13594" max="13594" width="31.33203125" style="36" customWidth="1"/>
+    <col min="13595" max="13804" width="8.83203125" style="36"/>
+    <col min="13805" max="13805" width="1.5" style="36" customWidth="1"/>
+    <col min="13806" max="13806" width="1.33203125" style="36" customWidth="1"/>
+    <col min="13807" max="13807" width="42" style="36" customWidth="1"/>
+    <col min="13808" max="13808" width="5.5" style="36" customWidth="1"/>
+    <col min="13809" max="13810" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="13811" max="13811" width="2.6640625" style="36" customWidth="1"/>
+    <col min="13812" max="13847" width="3.33203125" style="36" customWidth="1"/>
+    <col min="13848" max="13848" width="1.6640625" style="36" customWidth="1"/>
+    <col min="13849" max="13849" width="25.6640625" style="36" customWidth="1"/>
+    <col min="13850" max="13850" width="31.33203125" style="36" customWidth="1"/>
+    <col min="13851" max="14060" width="8.83203125" style="36"/>
+    <col min="14061" max="14061" width="1.5" style="36" customWidth="1"/>
+    <col min="14062" max="14062" width="1.33203125" style="36" customWidth="1"/>
+    <col min="14063" max="14063" width="42" style="36" customWidth="1"/>
+    <col min="14064" max="14064" width="5.5" style="36" customWidth="1"/>
+    <col min="14065" max="14066" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="14067" max="14067" width="2.6640625" style="36" customWidth="1"/>
+    <col min="14068" max="14103" width="3.33203125" style="36" customWidth="1"/>
+    <col min="14104" max="14104" width="1.6640625" style="36" customWidth="1"/>
+    <col min="14105" max="14105" width="25.6640625" style="36" customWidth="1"/>
+    <col min="14106" max="14106" width="31.33203125" style="36" customWidth="1"/>
+    <col min="14107" max="14316" width="8.83203125" style="36"/>
+    <col min="14317" max="14317" width="1.5" style="36" customWidth="1"/>
+    <col min="14318" max="14318" width="1.33203125" style="36" customWidth="1"/>
+    <col min="14319" max="14319" width="42" style="36" customWidth="1"/>
+    <col min="14320" max="14320" width="5.5" style="36" customWidth="1"/>
+    <col min="14321" max="14322" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="14323" max="14323" width="2.6640625" style="36" customWidth="1"/>
+    <col min="14324" max="14359" width="3.33203125" style="36" customWidth="1"/>
+    <col min="14360" max="14360" width="1.6640625" style="36" customWidth="1"/>
+    <col min="14361" max="14361" width="25.6640625" style="36" customWidth="1"/>
+    <col min="14362" max="14362" width="31.33203125" style="36" customWidth="1"/>
+    <col min="14363" max="14572" width="8.83203125" style="36"/>
+    <col min="14573" max="14573" width="1.5" style="36" customWidth="1"/>
+    <col min="14574" max="14574" width="1.33203125" style="36" customWidth="1"/>
+    <col min="14575" max="14575" width="42" style="36" customWidth="1"/>
+    <col min="14576" max="14576" width="5.5" style="36" customWidth="1"/>
+    <col min="14577" max="14578" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="14579" max="14579" width="2.6640625" style="36" customWidth="1"/>
+    <col min="14580" max="14615" width="3.33203125" style="36" customWidth="1"/>
+    <col min="14616" max="14616" width="1.6640625" style="36" customWidth="1"/>
+    <col min="14617" max="14617" width="25.6640625" style="36" customWidth="1"/>
+    <col min="14618" max="14618" width="31.33203125" style="36" customWidth="1"/>
+    <col min="14619" max="14828" width="8.83203125" style="36"/>
+    <col min="14829" max="14829" width="1.5" style="36" customWidth="1"/>
+    <col min="14830" max="14830" width="1.33203125" style="36" customWidth="1"/>
+    <col min="14831" max="14831" width="42" style="36" customWidth="1"/>
+    <col min="14832" max="14832" width="5.5" style="36" customWidth="1"/>
+    <col min="14833" max="14834" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="14835" max="14835" width="2.6640625" style="36" customWidth="1"/>
+    <col min="14836" max="14871" width="3.33203125" style="36" customWidth="1"/>
+    <col min="14872" max="14872" width="1.6640625" style="36" customWidth="1"/>
+    <col min="14873" max="14873" width="25.6640625" style="36" customWidth="1"/>
+    <col min="14874" max="14874" width="31.33203125" style="36" customWidth="1"/>
+    <col min="14875" max="15084" width="8.83203125" style="36"/>
+    <col min="15085" max="15085" width="1.5" style="36" customWidth="1"/>
+    <col min="15086" max="15086" width="1.33203125" style="36" customWidth="1"/>
+    <col min="15087" max="15087" width="42" style="36" customWidth="1"/>
+    <col min="15088" max="15088" width="5.5" style="36" customWidth="1"/>
+    <col min="15089" max="15090" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="15091" max="15091" width="2.6640625" style="36" customWidth="1"/>
+    <col min="15092" max="15127" width="3.33203125" style="36" customWidth="1"/>
+    <col min="15128" max="15128" width="1.6640625" style="36" customWidth="1"/>
+    <col min="15129" max="15129" width="25.6640625" style="36" customWidth="1"/>
+    <col min="15130" max="15130" width="31.33203125" style="36" customWidth="1"/>
+    <col min="15131" max="15340" width="8.83203125" style="36"/>
+    <col min="15341" max="15341" width="1.5" style="36" customWidth="1"/>
+    <col min="15342" max="15342" width="1.33203125" style="36" customWidth="1"/>
+    <col min="15343" max="15343" width="42" style="36" customWidth="1"/>
+    <col min="15344" max="15344" width="5.5" style="36" customWidth="1"/>
+    <col min="15345" max="15346" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="15347" max="15347" width="2.6640625" style="36" customWidth="1"/>
+    <col min="15348" max="15383" width="3.33203125" style="36" customWidth="1"/>
+    <col min="15384" max="15384" width="1.6640625" style="36" customWidth="1"/>
+    <col min="15385" max="15385" width="25.6640625" style="36" customWidth="1"/>
+    <col min="15386" max="15386" width="31.33203125" style="36" customWidth="1"/>
+    <col min="15387" max="15596" width="8.83203125" style="36"/>
+    <col min="15597" max="15597" width="1.5" style="36" customWidth="1"/>
+    <col min="15598" max="15598" width="1.33203125" style="36" customWidth="1"/>
+    <col min="15599" max="15599" width="42" style="36" customWidth="1"/>
+    <col min="15600" max="15600" width="5.5" style="36" customWidth="1"/>
+    <col min="15601" max="15602" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="15603" max="15603" width="2.6640625" style="36" customWidth="1"/>
+    <col min="15604" max="15639" width="3.33203125" style="36" customWidth="1"/>
+    <col min="15640" max="15640" width="1.6640625" style="36" customWidth="1"/>
+    <col min="15641" max="15641" width="25.6640625" style="36" customWidth="1"/>
+    <col min="15642" max="15642" width="31.33203125" style="36" customWidth="1"/>
+    <col min="15643" max="15852" width="8.83203125" style="36"/>
+    <col min="15853" max="15853" width="1.5" style="36" customWidth="1"/>
+    <col min="15854" max="15854" width="1.33203125" style="36" customWidth="1"/>
+    <col min="15855" max="15855" width="42" style="36" customWidth="1"/>
+    <col min="15856" max="15856" width="5.5" style="36" customWidth="1"/>
+    <col min="15857" max="15858" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="15859" max="15859" width="2.6640625" style="36" customWidth="1"/>
+    <col min="15860" max="15895" width="3.33203125" style="36" customWidth="1"/>
+    <col min="15896" max="15896" width="1.6640625" style="36" customWidth="1"/>
+    <col min="15897" max="15897" width="25.6640625" style="36" customWidth="1"/>
+    <col min="15898" max="15898" width="31.33203125" style="36" customWidth="1"/>
+    <col min="15899" max="16108" width="8.83203125" style="36"/>
+    <col min="16109" max="16109" width="1.5" style="36" customWidth="1"/>
+    <col min="16110" max="16110" width="1.33203125" style="36" customWidth="1"/>
+    <col min="16111" max="16111" width="42" style="36" customWidth="1"/>
+    <col min="16112" max="16112" width="5.5" style="36" customWidth="1"/>
+    <col min="16113" max="16114" width="0" style="36" hidden="1" customWidth="1"/>
+    <col min="16115" max="16115" width="2.6640625" style="36" customWidth="1"/>
+    <col min="16116" max="16151" width="3.33203125" style="36" customWidth="1"/>
+    <col min="16152" max="16152" width="1.6640625" style="36" customWidth="1"/>
+    <col min="16153" max="16153" width="25.6640625" style="36" customWidth="1"/>
+    <col min="16154" max="16154" width="31.33203125" style="36" customWidth="1"/>
+    <col min="16155" max="16384" width="8.83203125" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="70" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" ht="35" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="2:35" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="66" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="2:35" ht="35" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C2" s="36"/>
     </row>
-    <row r="3" spans="2:7" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="53" t="s">
-        <v>49</v>
-      </c>
-      <c r="D3" s="53" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="53" t="s">
-        <v>43</v>
-      </c>
-      <c r="F3" s="53" t="s">
-        <v>44</v>
-      </c>
-      <c r="G3" s="54" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="48" x14ac:dyDescent="0.15">
-      <c r="B4" s="74" t="s">
+    <row r="3" spans="2:35" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B3" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" s="89" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE3" s="36"/>
+      <c r="AF3" s="36"/>
+      <c r="AG3" s="36"/>
+      <c r="AH3" s="36"/>
+      <c r="AI3" s="36"/>
+    </row>
+    <row r="4" spans="2:35" ht="32" x14ac:dyDescent="0.15">
+      <c r="B4" s="67" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4" s="68" t="s">
+        <v>84</v>
+      </c>
+      <c r="D4" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="E4" s="88">
+        <v>42513.552083333336</v>
+      </c>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="36"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="36"/>
+    </row>
+    <row r="5" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B5" s="67" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="88">
+        <v>42524.337500000001</v>
+      </c>
+      <c r="AE5" s="36"/>
+      <c r="AF5" s="36"/>
+      <c r="AG5" s="36"/>
+      <c r="AH5" s="36"/>
+      <c r="AI5" s="36"/>
+    </row>
+    <row r="6" spans="2:35" ht="32" x14ac:dyDescent="0.15">
+      <c r="B6" s="67" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="88">
+        <v>42478.36041666667</v>
+      </c>
+      <c r="AE6" s="36"/>
+      <c r="AF6" s="36"/>
+      <c r="AG6" s="36"/>
+      <c r="AH6" s="36"/>
+      <c r="AI6" s="36"/>
+    </row>
+    <row r="7" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B7" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E7" s="88">
+        <v>42473.386111111111</v>
+      </c>
+      <c r="AE7" s="36"/>
+      <c r="AF7" s="36"/>
+      <c r="AG7" s="36"/>
+      <c r="AH7" s="36"/>
+      <c r="AI7" s="36"/>
+    </row>
+    <row r="8" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B8" s="67" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="68" t="s">
+        <v>89</v>
+      </c>
+      <c r="D8" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="88">
+        <v>42494.717361111114</v>
+      </c>
+      <c r="AE8" s="36"/>
+      <c r="AF8" s="36"/>
+      <c r="AG8" s="36"/>
+      <c r="AH8" s="36"/>
+      <c r="AI8" s="36"/>
+    </row>
+    <row r="9" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B9" s="67" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="68" t="s">
         <v>67</v>
       </c>
-      <c r="C4" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="76" t="s">
+      <c r="D9" s="68" t="s">
         <v>72</v>
       </c>
-      <c r="E4" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="G4" s="76" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="48" x14ac:dyDescent="0.15">
-      <c r="B5" s="71" t="s">
+      <c r="E9" s="88">
+        <v>42522.482638888891</v>
+      </c>
+      <c r="AE9" s="36"/>
+      <c r="AF9" s="36"/>
+      <c r="AG9" s="36"/>
+      <c r="AH9" s="36"/>
+      <c r="AI9" s="36"/>
+    </row>
+    <row r="10" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B10" s="67" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="68" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="88">
+        <v>42523.647222222222</v>
+      </c>
+      <c r="AE10" s="36"/>
+      <c r="AF10" s="36"/>
+      <c r="AG10" s="36"/>
+      <c r="AH10" s="36"/>
+      <c r="AI10" s="36"/>
+    </row>
+    <row r="11" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B11" s="67" t="s">
+        <v>60</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E11" s="88">
+        <v>42503.751388888886</v>
+      </c>
+      <c r="AE11" s="36"/>
+      <c r="AF11" s="36"/>
+      <c r="AG11" s="36"/>
+      <c r="AH11" s="36"/>
+      <c r="AI11" s="36"/>
+    </row>
+    <row r="12" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B12" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="68" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" s="88">
+        <v>42556.534722222219</v>
+      </c>
+      <c r="AE12" s="36"/>
+      <c r="AF12" s="36"/>
+      <c r="AG12" s="36"/>
+      <c r="AH12" s="36"/>
+      <c r="AI12" s="36"/>
+    </row>
+    <row r="13" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+      <c r="B13" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="72" t="s">
-        <v>74</v>
-      </c>
-      <c r="D5" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="96" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="32" x14ac:dyDescent="0.15">
-      <c r="B6" s="74" t="s">
-        <v>75</v>
-      </c>
-      <c r="C6" s="75" t="s">
-        <v>89</v>
-      </c>
-      <c r="D6" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>93</v>
-      </c>
-      <c r="F6" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="G6" s="98" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="48" x14ac:dyDescent="0.15">
-      <c r="B7" s="74" t="s">
-        <v>76</v>
-      </c>
-      <c r="C7" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="D7" s="76" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="F7" s="78" t="s">
-        <v>71</v>
-      </c>
-      <c r="G7" s="76" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="32" x14ac:dyDescent="0.15">
-      <c r="B8" s="71" t="s">
-        <v>77</v>
-      </c>
-      <c r="C8" s="77" t="s">
-        <v>90</v>
-      </c>
-      <c r="D8" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="96" t="s">
-        <v>83</v>
-      </c>
-      <c r="F8" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="G8" s="73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="32" x14ac:dyDescent="0.15">
-      <c r="B9" s="71" t="s">
-        <v>78</v>
-      </c>
-      <c r="C9" s="77" t="s">
-        <v>79</v>
-      </c>
-      <c r="D9" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="96" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" s="73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="32" x14ac:dyDescent="0.15">
-      <c r="B10" s="71" t="s">
-        <v>80</v>
-      </c>
-      <c r="C10" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="96" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" s="96" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="26" x14ac:dyDescent="0.15">
-      <c r="B11" s="71" t="s">
-        <v>82</v>
-      </c>
-      <c r="C11" s="77" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="96" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="96" t="s">
-        <v>93</v>
-      </c>
-      <c r="F11" s="97" t="s">
-        <v>71</v>
-      </c>
-      <c r="G11" s="73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="B12" s="71" t="s">
-        <v>85</v>
-      </c>
-      <c r="C12" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="47" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" s="73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="2:7" ht="16" x14ac:dyDescent="0.15">
-      <c r="B13" s="71" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="72" t="s">
-        <v>87</v>
-      </c>
-      <c r="D13" s="47" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="96" t="s">
-        <v>70</v>
-      </c>
-      <c r="F13" s="48" t="s">
-        <v>71</v>
-      </c>
-      <c r="G13" s="73" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="14" x14ac:dyDescent="0.15">
+      <c r="E13" s="88">
+        <v>42444.615972222222</v>
+      </c>
+      <c r="AE13" s="36"/>
+      <c r="AF13" s="36"/>
+      <c r="AG13" s="36"/>
+      <c r="AH13" s="36"/>
+      <c r="AI13" s="36"/>
+    </row>
+    <row r="14" spans="2:35" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="20"/>
-      <c r="C14" s="55"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="56"/>
-    </row>
-    <row r="15" spans="2:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="B15" s="55"/>
-      <c r="C15" s="55"/>
-      <c r="D15" s="55"/>
-      <c r="E15" s="56"/>
-    </row>
-    <row r="16" spans="2:7" ht="14" x14ac:dyDescent="0.15">
-      <c r="B16" s="55"/>
-      <c r="C16" s="55"/>
-      <c r="D16" s="55"/>
-      <c r="E16" s="56"/>
-    </row>
-    <row r="17" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B17" s="55"/>
-      <c r="C17" s="55"/>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
-    </row>
-    <row r="18" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B18" s="55"/>
-      <c r="C18" s="55"/>
-      <c r="D18" s="55"/>
-      <c r="E18" s="56"/>
-    </row>
-    <row r="19" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B19" s="55"/>
-      <c r="C19" s="55"/>
-      <c r="D19" s="55"/>
-      <c r="E19" s="56"/>
-    </row>
-    <row r="20" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B20" s="55"/>
-      <c r="C20" s="55"/>
-      <c r="D20" s="55"/>
-      <c r="E20" s="56"/>
-    </row>
-    <row r="21" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B21" s="55"/>
-      <c r="C21" s="55"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="56"/>
-    </row>
-    <row r="22" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B22" s="55"/>
-      <c r="C22" s="55"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="56"/>
-    </row>
-    <row r="23" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B23" s="55"/>
-      <c r="C23" s="55"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="56"/>
-    </row>
-    <row r="24" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B24" s="55"/>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="56"/>
-    </row>
-    <row r="25" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B25" s="55"/>
-      <c r="C25" s="55"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="56"/>
-    </row>
-    <row r="26" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B26" s="55"/>
-      <c r="C26" s="55"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="56"/>
-    </row>
-    <row r="27" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B27" s="55"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="52"/>
+    </row>
+    <row r="15" spans="2:35" ht="14" x14ac:dyDescent="0.15">
+      <c r="B15" s="51"/>
+      <c r="C15" s="51"/>
+      <c r="D15" s="52"/>
+    </row>
+    <row r="16" spans="2:35" ht="14" x14ac:dyDescent="0.15">
+      <c r="B16" s="51"/>
+      <c r="C16" s="51"/>
+      <c r="D16" s="52"/>
+    </row>
+    <row r="17" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B17" s="51"/>
+      <c r="C17" s="51"/>
+      <c r="D17" s="52"/>
+    </row>
+    <row r="18" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B18" s="51"/>
+      <c r="C18" s="51"/>
+      <c r="D18" s="52"/>
+    </row>
+    <row r="19" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B19" s="51"/>
+      <c r="C19" s="51"/>
+      <c r="D19" s="52"/>
+    </row>
+    <row r="20" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B20" s="51"/>
+      <c r="C20" s="51"/>
+      <c r="D20" s="52"/>
+    </row>
+    <row r="21" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B21" s="51"/>
+      <c r="C21" s="51"/>
+      <c r="D21" s="52"/>
+    </row>
+    <row r="22" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B22" s="51"/>
+      <c r="C22" s="51"/>
+      <c r="D22" s="52"/>
+    </row>
+    <row r="23" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B23" s="51"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="52"/>
+    </row>
+    <row r="24" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B24" s="51"/>
+      <c r="C24" s="51"/>
+      <c r="D24" s="52"/>
+    </row>
+    <row r="25" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B25" s="51"/>
+      <c r="C25" s="51"/>
+      <c r="D25" s="52"/>
+    </row>
+    <row r="26" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B26" s="51"/>
+      <c r="C26" s="51"/>
+      <c r="D26" s="52"/>
+    </row>
+    <row r="27" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B27" s="51"/>
       <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-    </row>
-    <row r="28" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B28" s="55"/>
-    </row>
-    <row r="29" spans="2:5" ht="14" x14ac:dyDescent="0.15">
-      <c r="B29" s="55"/>
+    </row>
+    <row r="28" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B28" s="51"/>
+    </row>
+    <row r="29" spans="2:4" ht="14" x14ac:dyDescent="0.15">
+      <c r="B29" s="51"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
-  <phoneticPr fontId="30" type="noConversion"/>
+  <phoneticPr fontId="28" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
@@ -7259,10 +7725,10 @@
     <hyperlink ref="B13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
-  <pageSetup paperSize="9" scale="67" fitToHeight="100" orientation="landscape" r:id="rId11"/>
+  <pageSetup paperSize="9" scale="98" fitToHeight="100" orientation="landscape" r:id="rId11"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.1&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId12"/>
   <extLst>

</xml_diff>

<commit_message>
[BG-302]: Updated Residual Anomalies document for BlueLib Android after review
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="28800" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="689" activeTab="2"/>
+    <workbookView xWindow="67200" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="689" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="102">
   <si>
     <t>1.1</t>
   </si>
@@ -358,9 +358,6 @@
     <t>Thijs Winter</t>
   </si>
   <si>
-    <t>Domain leader conenctivity</t>
-  </si>
-  <si>
     <t>Blocker</t>
   </si>
   <si>
@@ -428,6 +425,30 @@
   </si>
   <si>
     <t>[Moonshot] TFS 32433 - Scale pairing issue Nexus [Support only]</t>
+  </si>
+  <si>
+    <t>Conclusion: The build cannot be released to clients due to 1 critical and 8 major  defects.</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>2016-JUL-14</t>
+  </si>
+  <si>
+    <t>Changed severity classification</t>
+  </si>
+  <si>
+    <t>Domain leader connectivity</t>
+  </si>
+  <si>
+    <t>Review comments by Erik Gall</t>
+  </si>
+  <si>
+    <t>0.3</t>
+  </si>
+  <si>
+    <t>2016-JUL-15</t>
   </si>
   <si>
     <r>
@@ -447,7 +468,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> is generated from the defect tracking database. The defet severity is decided in an analysis session where the defect is judged on the occurrence rate, its effect on application stability, possiblity of data loss, ability to recover from the defect and market share of phone on which the defect occurs. See the table below for the explanation of defect severities.
+      <t xml:space="preserve"> is generated from the defect tracking database. The defect severity is decided in an analysis session where the defect is judged on the occurrence rate, its effect on application stability, possibility of data loss, ability to recover from the defect and market share of phone on which the defect occurs. See the table below for the explanation of defect severities.
 The tab "Maturity Grid" gives an overview of the amount of residual anomalies per defect severity. The tab "Anomalies" gives an overview of the anomalous behavior.
 </t>
     </r>
@@ -463,19 +484,7 @@
     </r>
   </si>
   <si>
-    <t>Conclusion: The build cannot be released to clients due to 1 critical and 8 major  defects.</t>
-  </si>
-  <si>
-    <t>0.2</t>
-  </si>
-  <si>
-    <t>2016-JUL-14</t>
-  </si>
-  <si>
-    <t>Changed severity classification</t>
-  </si>
-  <si>
-    <t>Review comments</t>
+    <t>Cosmetic changes</t>
   </si>
 </sst>
 </file>
@@ -750,7 +759,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -796,6 +805,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1030,7 +1045,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="126">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1136,7 +1151,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1186,6 +1200,42 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="22" fontId="35" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1224,24 +1274,18 @@
     <xf numFmtId="0" fontId="20" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="35" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="40" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1251,27 +1295,15 @@
     <xf numFmtId="0" fontId="40" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="38" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="7" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="36" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="38" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -2361,8 +2393,8 @@
   </sheetPr>
   <dimension ref="A1:G17"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="110" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView view="pageLayout" topLeftCell="A5" zoomScale="110" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2380,7 +2412,7 @@
       <c r="A1" t="s">
         <v>44</v>
       </c>
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="62" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="6"/>
@@ -2412,11 +2444,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="B6" s="94"/>
+      <c r="C6" s="94"/>
+      <c r="D6" s="94"/>
+      <c r="E6" s="94"/>
+      <c r="F6" s="94"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2426,10 +2458,10 @@
       <c r="C7" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="59" t="s">
+      <c r="D7" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="E7" s="59" t="s">
+      <c r="E7" s="58" t="s">
         <v>23</v>
       </c>
       <c r="F7" s="22"/>
@@ -2440,7 +2472,7 @@
         <v>68</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>20</v>
@@ -2479,17 +2511,17 @@
       <c r="B12" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="64" t="s">
+      <c r="C12" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="70" t="s">
+      <c r="D12" s="95" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="70"/>
+      <c r="E12" s="95"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="64" t="s">
+      <c r="G12" s="63" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2497,17 +2529,17 @@
       <c r="B13" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="71" t="s">
+      <c r="D13" s="96" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="71"/>
+      <c r="E13" s="96"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="64" t="s">
+      <c r="G13" s="63" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2515,15 +2547,15 @@
       <c r="B14" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="64" t="s">
-        <v>49</v>
-      </c>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
+      <c r="C14" s="63" t="s">
+        <v>98</v>
+      </c>
+      <c r="D14" s="96"/>
+      <c r="E14" s="96"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="30" t="s">
         <v>68</v>
       </c>
     </row>
@@ -2531,7 +2563,7 @@
       <c r="B15" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="64" t="s">
+      <c r="C15" s="63" t="s">
         <v>47</v>
       </c>
       <c r="D15" s="28" t="s">
@@ -2540,10 +2572,10 @@
       <c r="E15" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="F15" s="60" t="s">
+      <c r="F15" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="G15" s="61" t="s">
+      <c r="G15" s="60" t="s">
         <v>27</v>
       </c>
     </row>
@@ -2574,7 +2606,7 @@
   <pageSetup paperSize="9" scale="72" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -2592,7 +2624,7 @@
   </sheetPr>
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A6" zoomScale="99" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A8" zoomScale="99" zoomScaleNormal="80" zoomScalePageLayoutView="80" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -2608,7 +2640,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="50.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="62" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="6"/>
@@ -2643,11 +2675,11 @@
       <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="78" t="s">
+      <c r="D6" s="103" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="79"/>
-      <c r="F6" s="80"/>
+      <c r="E6" s="104"/>
+      <c r="F6" s="105"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
@@ -2656,11 +2688,11 @@
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="81" t="s">
+      <c r="D7" s="106" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="E7" s="106"/>
+      <c r="F7" s="106"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
@@ -2672,16 +2704,16 @@
       <c r="D8" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="55" t="s">
+      <c r="E8" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="62" t="s">
+      <c r="F8" s="61" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="33"/>
-      <c r="C9" s="65" t="s">
+      <c r="C9" s="64" t="s">
         <v>55</v>
       </c>
       <c r="D9" s="18"/>
@@ -2709,69 +2741,69 @@
       <c r="C12" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="82" t="s">
+      <c r="E12" s="107" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="82"/>
+      <c r="F12" s="107"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
-      <c r="D13" s="50" t="s">
+      <c r="D13" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="72" t="s">
+      <c r="E13" s="97" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="73"/>
+      <c r="F13" s="98"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
       <c r="C14" s="31"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="75"/>
+      <c r="E14" s="99"/>
+      <c r="F14" s="100"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
       <c r="C15" s="10"/>
       <c r="D15" s="18"/>
-      <c r="E15" s="57"/>
-      <c r="F15" s="58"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="77"/>
+      <c r="E16" s="101"/>
+      <c r="F16" s="102"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="51"/>
+      <c r="A19" s="50"/>
       <c r="B19" s="3"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="51"/>
+      <c r="A20" s="50"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="51"/>
+      <c r="A21" s="50"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="51"/>
+      <c r="A22" s="50"/>
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="51"/>
+      <c r="A23" s="50"/>
       <c r="B23" s="3"/>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="51"/>
+      <c r="A24" s="50"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="51"/>
+      <c r="A25" s="50"/>
     </row>
     <row r="28" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
@@ -2808,7 +2840,7 @@
   <pageSetup paperSize="9" scale="63" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -2826,8 +2858,8 @@
   </sheetPr>
   <dimension ref="B1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2842,7 +2874,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14" customFormat="1" ht="44" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>45</v>
       </c>
       <c r="C1" s="6"/>
@@ -2925,19 +2957,19 @@
       <c r="N6" s="17"/>
     </row>
     <row r="7" spans="2:14" ht="14" x14ac:dyDescent="0.15">
-      <c r="B7" s="64" t="s">
+      <c r="B7" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="64" t="s">
+      <c r="C7" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="64" t="s">
+      <c r="D7" s="63" t="s">
         <v>51</v>
       </c>
-      <c r="E7" s="64" t="s">
+      <c r="E7" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="F7" s="64" t="s">
+      <c r="F7" s="63" t="s">
         <v>56</v>
       </c>
       <c r="G7" s="17"/>
@@ -2951,19 +2983,19 @@
     </row>
     <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B8" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="C8" s="64" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="64" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="35" t="s">
+      <c r="F8" s="35" t="s">
         <v>97</v>
-      </c>
-      <c r="F8" s="35" t="s">
-        <v>98</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -2974,12 +3006,22 @@
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
     </row>
-    <row r="9" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
-      <c r="F9" s="17"/>
+    <row r="9" spans="2:14" ht="14" x14ac:dyDescent="0.15">
+      <c r="B9" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="35" t="s">
+        <v>97</v>
+      </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
       <c r="I9" s="17"/>
@@ -5546,7 +5588,7 @@
   <pageSetup paperSize="9" scale="91" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -5562,7 +5604,7 @@
   <dimension ref="B1:AK26"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5572,7 +5614,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:37" s="36" customFormat="1" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="63" t="s">
+      <c r="B1" s="62" t="s">
         <v>45</v>
       </c>
       <c r="D1" s="37"/>
@@ -5663,124 +5705,124 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="83" t="s">
-        <v>93</v>
-      </c>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
+      <c r="B4" s="114" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="115"/>
+      <c r="D4" s="115"/>
+      <c r="E4" s="115"/>
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="115"/>
+      <c r="J4" s="115"/>
+      <c r="K4" s="115"/>
+      <c r="L4" s="115"/>
     </row>
     <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="48"/>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="49"/>
-      <c r="J5" s="49"/>
-      <c r="K5" s="49"/>
-      <c r="L5" s="49"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="48"/>
+      <c r="G5" s="48"/>
+      <c r="H5" s="48"/>
+      <c r="I5" s="48"/>
+      <c r="J5" s="48"/>
+      <c r="K5" s="48"/>
+      <c r="L5" s="48"/>
     </row>
     <row r="6" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B6" s="90" t="s">
+      <c r="B6" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="91" t="s">
+      <c r="C6" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="92"/>
-      <c r="E6" s="92"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="92"/>
-      <c r="H6" s="92"/>
-      <c r="I6" s="93"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="118"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="80" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="119" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="120"/>
+      <c r="E7" s="120"/>
+      <c r="F7" s="120"/>
+      <c r="G7" s="120"/>
+      <c r="H7" s="120"/>
+      <c r="I7" s="121"/>
+      <c r="M7" s="53"/>
+      <c r="N7" s="53"/>
+      <c r="O7" s="53"/>
+      <c r="P7" s="53"/>
+      <c r="Q7" s="53"/>
+    </row>
+    <row r="8" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B8" s="73" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="112" t="s">
+      <c r="C8" s="122" t="s">
         <v>75</v>
       </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="114"/>
-      <c r="M7" s="54"/>
-      <c r="N7" s="54"/>
-      <c r="O7" s="54"/>
-      <c r="P7" s="54"/>
-      <c r="Q7" s="54"/>
-    </row>
-    <row r="8" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B8" s="95" t="s">
+      <c r="D8" s="123"/>
+      <c r="E8" s="123"/>
+      <c r="F8" s="123"/>
+      <c r="G8" s="123"/>
+      <c r="H8" s="123"/>
+      <c r="I8" s="124"/>
+      <c r="M8" s="53"/>
+      <c r="N8" s="53"/>
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+    </row>
+    <row r="9" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B9" s="74" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="96" t="s">
+      <c r="C9" s="111" t="s">
         <v>76</v>
       </c>
-      <c r="D8" s="97"/>
-      <c r="E8" s="97"/>
-      <c r="F8" s="97"/>
-      <c r="G8" s="97"/>
-      <c r="H8" s="97"/>
-      <c r="I8" s="98"/>
-      <c r="M8" s="54"/>
-      <c r="N8" s="54"/>
-      <c r="O8" s="54"/>
-      <c r="P8" s="54"/>
-      <c r="Q8" s="54"/>
-    </row>
-    <row r="9" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B9" s="99" t="s">
+      <c r="D9" s="112"/>
+      <c r="E9" s="112"/>
+      <c r="F9" s="112"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="112"/>
+      <c r="I9" s="113"/>
+      <c r="M9" s="53"/>
+      <c r="N9" s="53"/>
+      <c r="O9" s="53"/>
+      <c r="P9" s="53"/>
+      <c r="Q9" s="53"/>
+    </row>
+    <row r="10" spans="2:37" x14ac:dyDescent="0.2">
+      <c r="B10" s="75" t="s">
         <v>72</v>
       </c>
-      <c r="C9" s="100" t="s">
+      <c r="C10" s="76" t="s">
         <v>77</v>
       </c>
-      <c r="D9" s="101"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="101"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-      <c r="I9" s="102"/>
-      <c r="M9" s="54"/>
-      <c r="N9" s="54"/>
-      <c r="O9" s="54"/>
-      <c r="P9" s="54"/>
-      <c r="Q9" s="54"/>
-    </row>
-    <row r="10" spans="2:37" x14ac:dyDescent="0.2">
-      <c r="B10" s="103" t="s">
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="78"/>
+    </row>
+    <row r="11" spans="2:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="79" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="104" t="s">
+      <c r="C11" s="108" t="s">
         <v>78</v>
-      </c>
-      <c r="D10" s="105"/>
-      <c r="E10" s="105"/>
-      <c r="F10" s="105"/>
-      <c r="G10" s="105"/>
-      <c r="H10" s="105"/>
-      <c r="I10" s="106"/>
-    </row>
-    <row r="11" spans="2:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="107" t="s">
-        <v>74</v>
-      </c>
-      <c r="C11" s="108" t="s">
-        <v>79</v>
       </c>
       <c r="D11" s="109"/>
       <c r="E11" s="109"/>
@@ -5790,22 +5832,22 @@
       <c r="I11" s="110"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="C12" s="86"/>
+      <c r="C12" s="68"/>
     </row>
     <row r="13" spans="2:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="C13" s="86"/>
+      <c r="C13" s="68"/>
     </row>
     <row r="14" spans="2:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="C14" s="86"/>
+      <c r="C14" s="68"/>
     </row>
     <row r="15" spans="2:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="C15" s="86"/>
+      <c r="C15" s="68"/>
     </row>
     <row r="16" spans="2:37" ht="18" x14ac:dyDescent="0.2">
-      <c r="C16" s="86"/>
+      <c r="C16" s="68"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="53"/>
+      <c r="B20" s="52"/>
     </row>
     <row r="22" spans="2:12" ht="16" x14ac:dyDescent="0.2">
       <c r="B22" s="42"/>
@@ -5873,7 +5915,7 @@
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -5892,7 +5934,7 @@
   <dimension ref="B1:AJ11"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6604,17 +6646,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="85" t="s">
+      <c r="B3" s="125" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
+      <c r="C3" s="125"/>
+      <c r="D3" s="125"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="39"/>
@@ -6622,58 +6664,58 @@
       <c r="D4" s="39"/>
     </row>
     <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B5" s="87" t="s">
+      <c r="B5" s="81" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="82">
+        <v>0</v>
+      </c>
+      <c r="D5" s="39"/>
+    </row>
+    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B6" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="C5" s="47">
-        <v>0</v>
-      </c>
-      <c r="D5" s="39"/>
-    </row>
-    <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B6" s="87" t="s">
+      <c r="C6" s="84">
+        <v>1</v>
+      </c>
+      <c r="D6" s="39"/>
+    </row>
+    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B7" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="C6" s="47">
-        <v>1</v>
-      </c>
-      <c r="D6" s="39"/>
-    </row>
-    <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B7" s="87" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="47">
+      <c r="C7" s="86">
         <v>8</v>
       </c>
       <c r="D7" s="39"/>
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="87" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="88">
+        <v>1</v>
+      </c>
+      <c r="D8" s="39"/>
+    </row>
+    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="B9" s="89" t="s">
         <v>73</v>
       </c>
-      <c r="C8" s="47">
-        <v>1</v>
-      </c>
-      <c r="D8" s="39"/>
-    </row>
-    <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B9" s="87" t="s">
-        <v>74</v>
-      </c>
-      <c r="C9" s="50">
+      <c r="C9" s="90">
         <v>0</v>
       </c>
       <c r="D9" s="41"/>
     </row>
     <row r="10" spans="2:4" ht="15" x14ac:dyDescent="0.2">
-      <c r="B10" s="94"/>
+      <c r="B10" s="72"/>
       <c r="C10" s="41"/>
       <c r="D10" s="41"/>
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="40" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6688,7 +6730,7 @@
   <pageSetup paperSize="9" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId2"/>
   <extLst>
@@ -6706,8 +6748,8 @@
   </sheetPr>
   <dimension ref="B1:AI29"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D13"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7418,7 +7460,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:35" ht="31.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="66" t="s">
+      <c r="B1" s="65" t="s">
         <v>45</v>
       </c>
     </row>
@@ -7426,17 +7468,17 @@
       <c r="C2" s="36"/>
     </row>
     <row r="3" spans="2:35" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="70" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="70" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="D3" s="70" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="89" t="s">
+      <c r="E3" s="70" t="s">
         <v>82</v>
-      </c>
-      <c r="E3" s="89" t="s">
-        <v>83</v>
       </c>
       <c r="AE3" s="36"/>
       <c r="AF3" s="36"/>
@@ -7445,16 +7487,16 @@
       <c r="AI3" s="36"/>
     </row>
     <row r="4" spans="2:35" ht="32" x14ac:dyDescent="0.15">
-      <c r="B4" s="67" t="s">
+      <c r="B4" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="C4" s="68" t="s">
-        <v>84</v>
-      </c>
-      <c r="D4" s="68" t="s">
-        <v>71</v>
-      </c>
-      <c r="E4" s="88">
+      <c r="C4" s="67" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="91" t="s">
+        <v>70</v>
+      </c>
+      <c r="E4" s="69">
         <v>42513.552083333336</v>
       </c>
       <c r="AE4" s="36"/>
@@ -7464,16 +7506,16 @@
       <c r="AI4" s="36"/>
     </row>
     <row r="5" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B5" s="67" t="s">
+      <c r="B5" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="C5" s="68" t="s">
-        <v>85</v>
-      </c>
-      <c r="D5" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E5" s="88">
+      <c r="C5" s="67" t="s">
+        <v>84</v>
+      </c>
+      <c r="D5" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" s="69">
         <v>42524.337500000001</v>
       </c>
       <c r="AE5" s="36"/>
@@ -7483,16 +7525,16 @@
       <c r="AI5" s="36"/>
     </row>
     <row r="6" spans="2:35" ht="32" x14ac:dyDescent="0.15">
-      <c r="B6" s="67" t="s">
+      <c r="B6" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="C6" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="68" t="s">
-        <v>87</v>
-      </c>
-      <c r="D6" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E6" s="88">
+      <c r="D6" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E6" s="69">
         <v>42478.36041666667</v>
       </c>
       <c r="AE6" s="36"/>
@@ -7502,16 +7544,16 @@
       <c r="AI6" s="36"/>
     </row>
     <row r="7" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B7" s="67" t="s">
+      <c r="B7" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="68" t="s">
+      <c r="C7" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="D7" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E7" s="88">
+      <c r="D7" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E7" s="69">
         <v>42473.386111111111</v>
       </c>
       <c r="AE7" s="36"/>
@@ -7521,16 +7563,16 @@
       <c r="AI7" s="36"/>
     </row>
     <row r="8" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="66" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="C8" s="68" t="s">
-        <v>89</v>
-      </c>
-      <c r="D8" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="88">
+      <c r="D8" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="69">
         <v>42494.717361111114</v>
       </c>
       <c r="AE8" s="36"/>
@@ -7540,16 +7582,16 @@
       <c r="AI8" s="36"/>
     </row>
     <row r="9" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B9" s="67" t="s">
+      <c r="B9" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="67" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="88">
+      <c r="D9" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E9" s="69">
         <v>42522.482638888891</v>
       </c>
       <c r="AE9" s="36"/>
@@ -7559,16 +7601,16 @@
       <c r="AI9" s="36"/>
     </row>
     <row r="10" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B10" s="67" t="s">
+      <c r="B10" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="68" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E10" s="88">
+      <c r="C10" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E10" s="69">
         <v>42523.647222222222</v>
       </c>
       <c r="AE10" s="36"/>
@@ -7578,16 +7620,16 @@
       <c r="AI10" s="36"/>
     </row>
     <row r="11" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="68" t="s">
-        <v>91</v>
-      </c>
-      <c r="D11" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E11" s="88">
+      <c r="C11" s="67" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="69">
         <v>42503.751388888886</v>
       </c>
       <c r="AE11" s="36"/>
@@ -7597,16 +7639,16 @@
       <c r="AI11" s="36"/>
     </row>
     <row r="12" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B12" s="67" t="s">
+      <c r="B12" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="68" t="s">
-        <v>92</v>
-      </c>
-      <c r="D12" s="68" t="s">
-        <v>72</v>
-      </c>
-      <c r="E12" s="88">
+      <c r="C12" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="D12" s="92" t="s">
+        <v>71</v>
+      </c>
+      <c r="E12" s="69">
         <v>42556.534722222219</v>
       </c>
       <c r="AE12" s="36"/>
@@ -7615,17 +7657,17 @@
       <c r="AH12" s="36"/>
       <c r="AI12" s="36"/>
     </row>
-    <row r="13" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B13" s="67" t="s">
+    <row r="13" spans="2:35" ht="32" x14ac:dyDescent="0.15">
+      <c r="B13" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="68" t="s">
+      <c r="C13" s="67" t="s">
         <v>59</v>
       </c>
-      <c r="D13" s="68" t="s">
-        <v>73</v>
-      </c>
-      <c r="E13" s="88">
+      <c r="D13" s="93" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="69">
         <v>42444.615972222222</v>
       </c>
       <c r="AE13" s="36"/>
@@ -7636,78 +7678,78 @@
     </row>
     <row r="14" spans="2:35" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="20"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="52"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="51"/>
     </row>
     <row r="15" spans="2:35" ht="14" x14ac:dyDescent="0.15">
-      <c r="B15" s="51"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="52"/>
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
     </row>
     <row r="16" spans="2:35" ht="14" x14ac:dyDescent="0.15">
-      <c r="B16" s="51"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="52"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
     </row>
     <row r="17" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B17" s="51"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="52"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="50"/>
+      <c r="D17" s="51"/>
     </row>
     <row r="18" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B18" s="51"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="52"/>
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+      <c r="D18" s="51"/>
     </row>
     <row r="19" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B19" s="51"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="52"/>
+      <c r="B19" s="50"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
     </row>
     <row r="20" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B20" s="51"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="52"/>
+      <c r="B20" s="50"/>
+      <c r="C20" s="50"/>
+      <c r="D20" s="51"/>
     </row>
     <row r="21" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B21" s="51"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="52"/>
+      <c r="B21" s="50"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
     </row>
     <row r="22" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B22" s="51"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="52"/>
+      <c r="B22" s="50"/>
+      <c r="C22" s="50"/>
+      <c r="D22" s="51"/>
     </row>
     <row r="23" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B23" s="51"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="52"/>
+      <c r="B23" s="50"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="51"/>
     </row>
     <row r="24" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B24" s="51"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="52"/>
+      <c r="B24" s="50"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
     </row>
     <row r="25" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B25" s="51"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="52"/>
+      <c r="B25" s="50"/>
+      <c r="C25" s="50"/>
+      <c r="D25" s="51"/>
     </row>
     <row r="26" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B26" s="51"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="52"/>
+      <c r="B26" s="50"/>
+      <c r="C26" s="50"/>
+      <c r="D26" s="51"/>
     </row>
     <row r="27" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B27" s="51"/>
+      <c r="B27" s="50"/>
       <c r="C27" s="20"/>
     </row>
     <row r="28" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B28" s="51"/>
+      <c r="B28" s="50"/>
     </row>
     <row r="29" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B29" s="51"/>
+      <c r="B29" s="50"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -7728,7 +7770,7 @@
   <pageSetup paperSize="9" scale="98" fitToHeight="100" orientation="landscape" r:id="rId11"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
-    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.2&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId12"/>
   <extLst>

</xml_diff>

<commit_message>
[BG-302]: Updated Residual Anomalies document for BlueLib Android
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="67200" yWindow="460" windowWidth="38400" windowHeight="23540" tabRatio="689" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="689" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="98">
   <si>
     <t>1.1</t>
   </si>
@@ -322,18 +322,12 @@
     <t>Document creation</t>
   </si>
   <si>
-    <t>BG-208</t>
-  </si>
-  <si>
     <t>BG-22</t>
   </si>
   <si>
     <t>Association with LifeSense BPM can fail unexpectedly on some Android combos</t>
   </si>
   <si>
-    <t>BG-158</t>
-  </si>
-  <si>
     <t>BG-241</t>
   </si>
   <si>
@@ -400,9 +394,6 @@
     <t>Created</t>
   </si>
   <si>
-    <t>[Android] Random Crash observed while syncing in samsung android device</t>
-  </si>
-  <si>
     <t>Bug 30721:Moonshine pairing fails</t>
   </si>
   <si>
@@ -421,13 +412,7 @@
     <t>Bug 30096:[Android] Sync error observed in dashboard screen.</t>
   </si>
   <si>
-    <t>[Moonshine] [Bug#656] Moonshine pairing issues with Android phones</t>
-  </si>
-  <si>
     <t>[Moonshot] TFS 32433 - Scale pairing issue Nexus [Support only]</t>
-  </si>
-  <si>
-    <t>Conclusion: The build cannot be released to clients due to 1 critical and 8 major  defects.</t>
   </si>
   <si>
     <t>0.2</t>
@@ -485,6 +470,9 @@
   </si>
   <si>
     <t>Cosmetic changes</t>
+  </si>
+  <si>
+    <t>Conclusion: The build cannot be released to clients due to 7 major  defects.</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1033,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="126">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1227,9 +1215,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="35" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2444,11 +2429,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="94"/>
-      <c r="C6" s="94"/>
-      <c r="D6" s="94"/>
-      <c r="E6" s="94"/>
-      <c r="F6" s="94"/>
+      <c r="B6" s="93"/>
+      <c r="C6" s="93"/>
+      <c r="D6" s="93"/>
+      <c r="E6" s="93"/>
+      <c r="F6" s="93"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2469,10 +2454,10 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>20</v>
@@ -2514,10 +2499,10 @@
       <c r="C12" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="95" t="s">
+      <c r="D12" s="94" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="95"/>
+      <c r="E12" s="94"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
@@ -2532,10 +2517,10 @@
       <c r="C13" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="96" t="s">
+      <c r="D13" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="96"/>
+      <c r="E13" s="95"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
@@ -2548,15 +2533,15 @@
         <v>14</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>98</v>
-      </c>
-      <c r="D14" s="96"/>
-      <c r="E14" s="96"/>
+        <v>93</v>
+      </c>
+      <c r="D14" s="95"/>
+      <c r="E14" s="95"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2675,11 +2660,11 @@
       <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="103" t="s">
+      <c r="D6" s="102" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="104"/>
-      <c r="F6" s="105"/>
+      <c r="E6" s="103"/>
+      <c r="F6" s="104"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
@@ -2688,11 +2673,11 @@
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="106" t="s">
+      <c r="D7" s="105" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="106"/>
-      <c r="F7" s="106"/>
+      <c r="E7" s="105"/>
+      <c r="F7" s="105"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
@@ -2744,27 +2729,27 @@
       <c r="D12" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="107" t="s">
+      <c r="E12" s="106" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="107"/>
+      <c r="F12" s="106"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
       <c r="D13" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="97" t="s">
+      <c r="E13" s="96" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="98"/>
+      <c r="F13" s="97"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
       <c r="C14" s="31"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="99"/>
-      <c r="F14" s="100"/>
+      <c r="E14" s="98"/>
+      <c r="F14" s="99"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
@@ -2777,8 +2762,8 @@
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="102"/>
+      <c r="E16" s="100"/>
+      <c r="F16" s="101"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
@@ -2859,7 +2844,7 @@
   <dimension ref="B1:N179"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="B9" sqref="B9:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2983,19 +2968,19 @@
     </row>
     <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B8" s="35" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C8" s="63" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D8" s="63" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -3008,19 +2993,19 @@
     </row>
     <row r="9" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="35" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C9" s="63" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D9" s="63" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -5705,19 +5690,19 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="114" t="s">
-        <v>100</v>
-      </c>
-      <c r="C4" s="115"/>
-      <c r="D4" s="115"/>
-      <c r="E4" s="115"/>
-      <c r="F4" s="115"/>
-      <c r="G4" s="115"/>
-      <c r="H4" s="115"/>
-      <c r="I4" s="115"/>
-      <c r="J4" s="115"/>
-      <c r="K4" s="115"/>
-      <c r="L4" s="115"/>
+      <c r="B4" s="113" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="114"/>
+      <c r="D4" s="114"/>
+      <c r="E4" s="114"/>
+      <c r="F4" s="114"/>
+      <c r="G4" s="114"/>
+      <c r="H4" s="114"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="114"/>
+      <c r="K4" s="114"/>
+      <c r="L4" s="114"/>
     </row>
     <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
@@ -5736,29 +5721,29 @@
       <c r="B6" s="71" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="116" t="s">
+      <c r="C6" s="115" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="117"/>
-      <c r="E6" s="117"/>
-      <c r="F6" s="117"/>
-      <c r="G6" s="117"/>
-      <c r="H6" s="117"/>
-      <c r="I6" s="118"/>
+      <c r="D6" s="116"/>
+      <c r="E6" s="116"/>
+      <c r="F6" s="116"/>
+      <c r="G6" s="116"/>
+      <c r="H6" s="116"/>
+      <c r="I6" s="117"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B7" s="80" t="s">
-        <v>69</v>
-      </c>
-      <c r="C7" s="119" t="s">
-        <v>74</v>
-      </c>
-      <c r="D7" s="120"/>
-      <c r="E7" s="120"/>
-      <c r="F7" s="120"/>
-      <c r="G7" s="120"/>
-      <c r="H7" s="120"/>
-      <c r="I7" s="121"/>
+        <v>67</v>
+      </c>
+      <c r="C7" s="118" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="119"/>
+      <c r="E7" s="119"/>
+      <c r="F7" s="119"/>
+      <c r="G7" s="119"/>
+      <c r="H7" s="119"/>
+      <c r="I7" s="120"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
       <c r="O7" s="53"/>
@@ -5767,17 +5752,17 @@
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B8" s="73" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" s="122" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="123"/>
-      <c r="G8" s="123"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="124"/>
+        <v>68</v>
+      </c>
+      <c r="C8" s="121" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="122"/>
+      <c r="E8" s="122"/>
+      <c r="F8" s="122"/>
+      <c r="G8" s="122"/>
+      <c r="H8" s="122"/>
+      <c r="I8" s="123"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
       <c r="O8" s="53"/>
@@ -5786,17 +5771,17 @@
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B9" s="74" t="s">
-        <v>71</v>
-      </c>
-      <c r="C9" s="111" t="s">
-        <v>76</v>
-      </c>
-      <c r="D9" s="112"/>
-      <c r="E9" s="112"/>
-      <c r="F9" s="112"/>
-      <c r="G9" s="112"/>
-      <c r="H9" s="112"/>
-      <c r="I9" s="113"/>
+        <v>69</v>
+      </c>
+      <c r="C9" s="110" t="s">
+        <v>74</v>
+      </c>
+      <c r="D9" s="111"/>
+      <c r="E9" s="111"/>
+      <c r="F9" s="111"/>
+      <c r="G9" s="111"/>
+      <c r="H9" s="111"/>
+      <c r="I9" s="112"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
       <c r="O9" s="53"/>
@@ -5805,10 +5790,10 @@
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B10" s="75" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C10" s="76" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D10" s="77"/>
       <c r="E10" s="77"/>
@@ -5819,17 +5804,17 @@
     </row>
     <row r="11" spans="2:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="79" t="s">
-        <v>73</v>
-      </c>
-      <c r="C11" s="108" t="s">
-        <v>78</v>
-      </c>
-      <c r="D11" s="109"/>
-      <c r="E11" s="109"/>
-      <c r="F11" s="109"/>
-      <c r="G11" s="109"/>
-      <c r="H11" s="109"/>
-      <c r="I11" s="110"/>
+        <v>71</v>
+      </c>
+      <c r="C11" s="107" t="s">
+        <v>76</v>
+      </c>
+      <c r="D11" s="108"/>
+      <c r="E11" s="108"/>
+      <c r="F11" s="108"/>
+      <c r="G11" s="108"/>
+      <c r="H11" s="108"/>
+      <c r="I11" s="109"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
       <c r="C12" s="68"/>
@@ -5934,7 +5919,7 @@
   <dimension ref="B1:AJ11"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6652,11 +6637,11 @@
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="125" t="s">
+      <c r="B3" s="124" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="39"/>
@@ -6665,7 +6650,7 @@
     </row>
     <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="81" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C5" s="82">
         <v>0</v>
@@ -6674,7 +6659,7 @@
     </row>
     <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="83" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" s="84">
         <v>1</v>
@@ -6683,7 +6668,7 @@
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="85" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C7" s="86">
         <v>8</v>
@@ -6692,7 +6677,7 @@
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="87" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C8" s="88">
         <v>1</v>
@@ -6701,7 +6686,7 @@
     </row>
     <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="89" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C9" s="90">
         <v>0</v>
@@ -6715,7 +6700,7 @@
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="40" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6746,10 +6731,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AI29"/>
+  <dimension ref="B1:AI27"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7469,16 +7454,16 @@
     </row>
     <row r="3" spans="2:35" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="70" t="s">
+        <v>78</v>
+      </c>
+      <c r="D3" s="70" t="s">
         <v>79</v>
       </c>
-      <c r="C3" s="70" t="s">
+      <c r="E3" s="70" t="s">
         <v>80</v>
-      </c>
-      <c r="D3" s="70" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="70" t="s">
-        <v>82</v>
       </c>
       <c r="AE3" s="36"/>
       <c r="AF3" s="36"/>
@@ -7486,18 +7471,18 @@
       <c r="AH3" s="36"/>
       <c r="AI3" s="36"/>
     </row>
-    <row r="4" spans="2:35" ht="32" x14ac:dyDescent="0.15">
+    <row r="4" spans="2:35" ht="16" x14ac:dyDescent="0.15">
       <c r="B4" s="66" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C4" s="67" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D4" s="91" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E4" s="69">
-        <v>42513.552083333336</v>
+        <v>42524.337500000001</v>
       </c>
       <c r="AE4" s="36"/>
       <c r="AF4" s="36"/>
@@ -7505,18 +7490,18 @@
       <c r="AH4" s="36"/>
       <c r="AI4" s="36"/>
     </row>
-    <row r="5" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+    <row r="5" spans="2:35" ht="32" x14ac:dyDescent="0.15">
       <c r="B5" s="66" t="s">
-        <v>64</v>
+        <v>82</v>
       </c>
       <c r="C5" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="D5" s="92" t="s">
-        <v>71</v>
+        <v>83</v>
+      </c>
+      <c r="D5" s="91" t="s">
+        <v>69</v>
       </c>
       <c r="E5" s="69">
-        <v>42524.337500000001</v>
+        <v>42478.36041666667</v>
       </c>
       <c r="AE5" s="36"/>
       <c r="AF5" s="36"/>
@@ -7524,18 +7509,18 @@
       <c r="AH5" s="36"/>
       <c r="AI5" s="36"/>
     </row>
-    <row r="6" spans="2:35" ht="32" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:35" ht="16" x14ac:dyDescent="0.15">
       <c r="B6" s="66" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C6" s="67" t="s">
-        <v>86</v>
-      </c>
-      <c r="D6" s="92" t="s">
-        <v>71</v>
+        <v>61</v>
+      </c>
+      <c r="D6" s="91" t="s">
+        <v>69</v>
       </c>
       <c r="E6" s="69">
-        <v>42478.36041666667</v>
+        <v>42473.386111111111</v>
       </c>
       <c r="AE6" s="36"/>
       <c r="AF6" s="36"/>
@@ -7545,16 +7530,16 @@
     </row>
     <row r="7" spans="2:35" ht="16" x14ac:dyDescent="0.15">
       <c r="B7" s="66" t="s">
-        <v>62</v>
+        <v>84</v>
       </c>
       <c r="C7" s="67" t="s">
-        <v>63</v>
-      </c>
-      <c r="D7" s="92" t="s">
-        <v>71</v>
+        <v>85</v>
+      </c>
+      <c r="D7" s="91" t="s">
+        <v>69</v>
       </c>
       <c r="E7" s="69">
-        <v>42473.386111111111</v>
+        <v>42494.717361111114</v>
       </c>
       <c r="AE7" s="36"/>
       <c r="AF7" s="36"/>
@@ -7564,16 +7549,16 @@
     </row>
     <row r="8" spans="2:35" ht="16" x14ac:dyDescent="0.15">
       <c r="B8" s="66" t="s">
-        <v>87</v>
+        <v>64</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>88</v>
-      </c>
-      <c r="D8" s="92" t="s">
-        <v>71</v>
+        <v>65</v>
+      </c>
+      <c r="D8" s="91" t="s">
+        <v>69</v>
       </c>
       <c r="E8" s="69">
-        <v>42494.717361111114</v>
+        <v>42522.482638888891</v>
       </c>
       <c r="AE8" s="36"/>
       <c r="AF8" s="36"/>
@@ -7583,16 +7568,16 @@
     </row>
     <row r="9" spans="2:35" ht="16" x14ac:dyDescent="0.15">
       <c r="B9" s="66" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="92" t="s">
-        <v>71</v>
+        <v>86</v>
+      </c>
+      <c r="D9" s="91" t="s">
+        <v>69</v>
       </c>
       <c r="E9" s="69">
-        <v>42522.482638888891</v>
+        <v>42523.647222222222</v>
       </c>
       <c r="AE9" s="36"/>
       <c r="AF9" s="36"/>
@@ -7602,16 +7587,16 @@
     </row>
     <row r="10" spans="2:35" ht="16" x14ac:dyDescent="0.15">
       <c r="B10" s="66" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>89</v>
-      </c>
-      <c r="D10" s="92" t="s">
-        <v>71</v>
+        <v>87</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>69</v>
       </c>
       <c r="E10" s="69">
-        <v>42523.647222222222</v>
+        <v>42556.534722222219</v>
       </c>
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
@@ -7619,18 +7604,18 @@
       <c r="AH10" s="36"/>
       <c r="AI10" s="36"/>
     </row>
-    <row r="11" spans="2:35" ht="16" x14ac:dyDescent="0.15">
+    <row r="11" spans="2:35" ht="32" x14ac:dyDescent="0.15">
       <c r="B11" s="66" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="D11" s="92" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E11" s="69">
-        <v>42503.751388888886</v>
+        <v>42444.615972222222</v>
       </c>
       <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
@@ -7638,38 +7623,20 @@
       <c r="AH11" s="36"/>
       <c r="AI11" s="36"/>
     </row>
-    <row r="12" spans="2:35" ht="16" x14ac:dyDescent="0.15">
-      <c r="B12" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="67" t="s">
-        <v>91</v>
-      </c>
-      <c r="D12" s="92" t="s">
-        <v>71</v>
-      </c>
-      <c r="E12" s="69">
-        <v>42556.534722222219</v>
-      </c>
+    <row r="12" spans="2:35" ht="14" x14ac:dyDescent="0.15">
+      <c r="B12" s="20"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="51"/>
       <c r="AE12" s="36"/>
       <c r="AF12" s="36"/>
       <c r="AG12" s="36"/>
       <c r="AH12" s="36"/>
       <c r="AI12" s="36"/>
     </row>
-    <row r="13" spans="2:35" ht="32" x14ac:dyDescent="0.15">
-      <c r="B13" s="66" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="67" t="s">
-        <v>59</v>
-      </c>
-      <c r="D13" s="93" t="s">
-        <v>72</v>
-      </c>
-      <c r="E13" s="69">
-        <v>42444.615972222222</v>
-      </c>
+    <row r="13" spans="2:35" ht="14" x14ac:dyDescent="0.15">
+      <c r="B13" s="50"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="51"/>
       <c r="AE13" s="36"/>
       <c r="AF13" s="36"/>
       <c r="AG13" s="36"/>
@@ -7677,7 +7644,7 @@
       <c r="AI13" s="36"/>
     </row>
     <row r="14" spans="2:35" ht="14" x14ac:dyDescent="0.15">
-      <c r="B14" s="20"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="50"/>
       <c r="D14" s="51"/>
     </row>
@@ -7733,23 +7700,13 @@
     </row>
     <row r="25" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B25" s="50"/>
-      <c r="C25" s="50"/>
-      <c r="D25" s="51"/>
+      <c r="C25" s="20"/>
     </row>
     <row r="26" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B26" s="50"/>
-      <c r="C26" s="50"/>
-      <c r="D26" s="51"/>
     </row>
     <row r="27" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B27" s="50"/>
-      <c r="C27" s="20"/>
-    </row>
-    <row r="28" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B28" s="50"/>
-    </row>
-    <row r="29" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B29" s="50"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
@@ -7763,16 +7720,14 @@
     <hyperlink ref="B9" r:id="rId6"/>
     <hyperlink ref="B10" r:id="rId7"/>
     <hyperlink ref="B11" r:id="rId8"/>
-    <hyperlink ref="B12" r:id="rId9"/>
-    <hyperlink ref="B13" r:id="rId10"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
-  <pageSetup paperSize="9" scale="98" fitToHeight="100" orientation="landscape" r:id="rId11"/>
+  <pageSetup paperSize="9" scale="98" fitToHeight="100" orientation="landscape" r:id="rId9"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
     <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId12"/>
+  <drawing r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Minor changes to the Residual Anomalies document
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="689" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="689" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -427,9 +427,6 @@
     <t>Domain leader connectivity</t>
   </si>
   <si>
-    <t>Review comments by Erik Gall</t>
-  </si>
-  <si>
     <t>0.3</t>
   </si>
   <si>
@@ -473,6 +470,9 @@
   </si>
   <si>
     <t>Conclusion: The build cannot be released to clients due to 7 major  defects.</t>
+  </si>
+  <si>
+    <t>Review comments by Erik Gaal</t>
   </si>
 </sst>
 </file>
@@ -2533,7 +2533,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D14" s="95"/>
       <c r="E14" s="95"/>
@@ -2844,7 +2844,7 @@
   <dimension ref="B1:N179"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:F9"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2980,7 +2980,7 @@
         <v>90</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -2993,19 +2993,19 @@
     </row>
     <row r="9" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="63" t="s">
         <v>93</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>94</v>
       </c>
       <c r="D9" s="63" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -5691,7 +5691,7 @@
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="113" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C4" s="114"/>
       <c r="D4" s="114"/>
@@ -6700,7 +6700,7 @@
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="40" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6743,7 +6743,7 @@
     <col min="2" max="2" width="7.1640625" style="37" customWidth="1"/>
     <col min="3" max="3" width="68.5" style="37" customWidth="1"/>
     <col min="4" max="4" width="8" style="38" customWidth="1"/>
-    <col min="5" max="5" width="14.5" style="38" customWidth="1"/>
+    <col min="5" max="5" width="17.5" style="38" customWidth="1"/>
     <col min="6" max="6" width="17.33203125" style="38" customWidth="1"/>
     <col min="7" max="25" width="3.33203125" style="38" customWidth="1"/>
     <col min="26" max="26" width="10" style="38" customWidth="1"/>
@@ -7722,7 +7722,7 @@
     <hyperlink ref="B11" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
-  <pageSetup paperSize="9" scale="98" fitToHeight="100" orientation="landscape" r:id="rId9"/>
+  <pageSetup paperSize="9" scale="96" fitToHeight="100" orientation="landscape" r:id="rId9"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
     <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>

</xml_diff>

<commit_message>
[Release-2.0.1]: Updated residual anomalies document
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="689" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="689" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -328,9 +328,6 @@
     <t>Crash , associating when bluetooth turned off</t>
   </si>
   <si>
-    <t>Crash during association</t>
-  </si>
-  <si>
     <t>Thijs Winter</t>
   </si>
   <si>
@@ -455,18 +452,9 @@
     <t>BL-88</t>
   </si>
   <si>
-    <t>BL-238</t>
-  </si>
-  <si>
     <t>BL-22</t>
   </si>
   <si>
-    <t>BL-385</t>
-  </si>
-  <si>
-    <t>NPE when disconnecting BtGatt</t>
-  </si>
-  <si>
     <t>BL-386</t>
   </si>
   <si>
@@ -474,6 +462,18 @@
   </si>
   <si>
     <t>Conclusion: The build cannot be released to clients due to 3 major  defects.</t>
+  </si>
+  <si>
+    <t>BL-390</t>
+  </si>
+  <si>
+    <t>NPE when calling readRssi()</t>
+  </si>
+  <si>
+    <t>BL-392</t>
+  </si>
+  <si>
+    <t>BlueLib doesn't build on a clean development environment</t>
   </si>
 </sst>
 </file>
@@ -804,7 +804,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -1024,6 +1024,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1202,6 +1217,30 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="34" fillId="0" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1269,30 +1308,6 @@
     <xf numFmtId="0" fontId="38" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="1" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2434,11 +2449,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="87"/>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2459,10 +2474,10 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>20</v>
@@ -2504,10 +2519,10 @@
       <c r="C12" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="88" t="s">
+      <c r="D12" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="88"/>
+      <c r="E12" s="96"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
@@ -2522,10 +2537,10 @@
       <c r="C13" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="89"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
@@ -2538,15 +2553,15 @@
         <v>14</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>79</v>
-      </c>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
+        <v>78</v>
+      </c>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2665,11 +2680,11 @@
       <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="96" t="s">
+      <c r="D6" s="104" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="97"/>
-      <c r="F6" s="98"/>
+      <c r="E6" s="105"/>
+      <c r="F6" s="106"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
@@ -2678,11 +2693,11 @@
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="99" t="s">
+      <c r="D7" s="107" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="99"/>
-      <c r="F7" s="99"/>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
@@ -2734,27 +2749,27 @@
       <c r="D12" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="100" t="s">
+      <c r="E12" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="100"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
       <c r="D13" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="90" t="s">
+      <c r="E13" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="91"/>
+      <c r="F13" s="99"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
       <c r="C14" s="31"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="93"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="101"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
@@ -2767,8 +2782,8 @@
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="94"/>
-      <c r="F16" s="95"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="103"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
@@ -2848,7 +2863,7 @@
   </sheetPr>
   <dimension ref="B1:N179"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A9" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2973,19 +2988,19 @@
     </row>
     <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B8" s="35" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="63" t="s">
         <v>75</v>
-      </c>
-      <c r="C8" s="63" t="s">
-        <v>76</v>
       </c>
       <c r="D8" s="63" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -2998,19 +3013,19 @@
     </row>
     <row r="9" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="35" t="s">
+        <v>78</v>
+      </c>
+      <c r="C9" s="63" t="s">
         <v>79</v>
-      </c>
-      <c r="C9" s="63" t="s">
-        <v>80</v>
       </c>
       <c r="D9" s="63" t="s">
         <v>51</v>
       </c>
       <c r="E9" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="35" t="s">
         <v>82</v>
-      </c>
-      <c r="F9" s="35" t="s">
-        <v>83</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -3023,19 +3038,19 @@
     </row>
     <row r="10" spans="2:14" ht="56" x14ac:dyDescent="0.15">
       <c r="B10" s="35" t="s">
+        <v>83</v>
+      </c>
+      <c r="C10" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="D10" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="E10" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>86</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>87</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -5585,7 +5600,7 @@
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <phoneticPr fontId="28" type="noConversion"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
-  <pageSetup paperSize="9" fitToHeight="100" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="91" fitToHeight="100" orientation="landscape" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
     <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
@@ -5603,7 +5618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:AK26"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A4" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+    <sheetView view="pageLayout" topLeftCell="A2" zoomScale="150" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -5705,19 +5720,19 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="107" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="108"/>
-      <c r="J4" s="108"/>
-      <c r="K4" s="108"/>
-      <c r="L4" s="108"/>
+      <c r="B4" s="115" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
     </row>
     <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
@@ -5736,29 +5751,29 @@
       <c r="B6" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="109" t="s">
+      <c r="C6" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="110"/>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="111"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="119"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B7" s="76" t="s">
-        <v>61</v>
-      </c>
-      <c r="C7" s="112" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" s="113"/>
-      <c r="E7" s="113"/>
-      <c r="F7" s="113"/>
-      <c r="G7" s="113"/>
-      <c r="H7" s="113"/>
-      <c r="I7" s="114"/>
+        <v>60</v>
+      </c>
+      <c r="C7" s="120" t="s">
+        <v>65</v>
+      </c>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="122"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
       <c r="O7" s="53"/>
@@ -5767,17 +5782,17 @@
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B8" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="115" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="116"/>
-      <c r="E8" s="116"/>
-      <c r="F8" s="116"/>
-      <c r="G8" s="116"/>
-      <c r="H8" s="116"/>
-      <c r="I8" s="117"/>
+        <v>61</v>
+      </c>
+      <c r="C8" s="123" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" s="124"/>
+      <c r="E8" s="124"/>
+      <c r="F8" s="124"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="125"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
       <c r="O8" s="53"/>
@@ -5786,17 +5801,17 @@
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B9" s="70" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" s="104" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" s="105"/>
-      <c r="E9" s="105"/>
-      <c r="F9" s="105"/>
-      <c r="G9" s="105"/>
-      <c r="H9" s="105"/>
-      <c r="I9" s="106"/>
+        <v>62</v>
+      </c>
+      <c r="C9" s="112" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="114"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
       <c r="O9" s="53"/>
@@ -5805,10 +5820,10 @@
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B10" s="71" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D10" s="73"/>
       <c r="E10" s="73"/>
@@ -5819,17 +5834,17 @@
     </row>
     <row r="11" spans="2:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="75" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="101" t="s">
-        <v>70</v>
-      </c>
-      <c r="D11" s="102"/>
-      <c r="E11" s="102"/>
-      <c r="F11" s="102"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="102"/>
-      <c r="I11" s="103"/>
+        <v>64</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="111"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
       <c r="C12" s="66"/>
@@ -6652,11 +6667,11 @@
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="118" t="s">
+      <c r="B3" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="118"/>
-      <c r="D3" s="118"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="39"/>
@@ -6665,7 +6680,7 @@
     </row>
     <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="77" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="78">
         <v>0</v>
@@ -6674,7 +6689,7 @@
     </row>
     <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="80">
         <v>0</v>
@@ -6683,7 +6698,7 @@
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="81" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C7" s="82">
         <v>3</v>
@@ -6692,7 +6707,7 @@
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="83" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C8" s="84">
         <v>3</v>
@@ -6701,7 +6716,7 @@
     </row>
     <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="85" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C9" s="86">
         <v>0</v>
@@ -6715,7 +6730,7 @@
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="40" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6749,7 +6764,7 @@
   <dimension ref="B1:AH27"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7467,14 +7482,14 @@
       <c r="C2" s="36"/>
     </row>
     <row r="3" spans="2:34" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="121" t="s">
+      <c r="B3" s="89" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="89" t="s">
         <v>71</v>
       </c>
-      <c r="C3" s="121" t="s">
+      <c r="D3" s="89" t="s">
         <v>72</v>
-      </c>
-      <c r="D3" s="121" t="s">
-        <v>73</v>
       </c>
       <c r="AD3" s="36"/>
       <c r="AE3" s="36"/>
@@ -7483,14 +7498,14 @@
       <c r="AH3" s="36"/>
     </row>
     <row r="4" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B4" s="122" t="s">
-        <v>90</v>
-      </c>
-      <c r="C4" s="123" t="s">
+      <c r="B4" s="91" t="s">
+        <v>89</v>
+      </c>
+      <c r="C4" s="92" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="125" t="s">
-        <v>63</v>
+      <c r="D4" s="93" t="s">
+        <v>62</v>
       </c>
       <c r="AD4" s="36"/>
       <c r="AE4" s="36"/>
@@ -7499,14 +7514,14 @@
       <c r="AH4" s="36"/>
     </row>
     <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B5" s="122" t="s">
-        <v>91</v>
-      </c>
-      <c r="C5" s="123" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="125" t="s">
-        <v>63</v>
+      <c r="B5" s="91" t="s">
+        <v>94</v>
+      </c>
+      <c r="C5" s="92" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="93" t="s">
+        <v>62</v>
       </c>
       <c r="AD5" s="36"/>
       <c r="AE5" s="36"/>
@@ -7515,14 +7530,14 @@
       <c r="AH5" s="36"/>
     </row>
     <row r="6" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B6" s="122" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="123" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="125" t="s">
-        <v>63</v>
+      <c r="B6" s="91" t="s">
+        <v>96</v>
+      </c>
+      <c r="C6" s="92" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="93" t="s">
+        <v>62</v>
       </c>
       <c r="AD6" s="36"/>
       <c r="AE6" s="36"/>
@@ -7531,14 +7546,14 @@
       <c r="AH6" s="36"/>
     </row>
     <row r="7" spans="2:34" ht="32" x14ac:dyDescent="0.15">
-      <c r="B7" s="122" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="123" t="s">
+      <c r="B7" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="92" t="s">
         <v>57</v>
       </c>
-      <c r="D7" s="126" t="s">
-        <v>64</v>
+      <c r="D7" s="94" t="s">
+        <v>63</v>
       </c>
       <c r="AD7" s="36"/>
       <c r="AE7" s="36"/>
@@ -7547,14 +7562,14 @@
       <c r="AH7" s="36"/>
     </row>
     <row r="8" spans="2:34" ht="32" x14ac:dyDescent="0.15">
-      <c r="B8" s="122" t="s">
-        <v>89</v>
-      </c>
-      <c r="C8" s="123" t="s">
-        <v>74</v>
-      </c>
-      <c r="D8" s="126" t="s">
-        <v>64</v>
+      <c r="B8" s="91" t="s">
+        <v>88</v>
+      </c>
+      <c r="C8" s="92" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="94" t="s">
+        <v>63</v>
       </c>
       <c r="AD8" s="36"/>
       <c r="AE8" s="36"/>
@@ -7563,14 +7578,14 @@
       <c r="AH8" s="36"/>
     </row>
     <row r="9" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B9" s="122" t="s">
-        <v>95</v>
-      </c>
-      <c r="C9" s="123" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="126" t="s">
-        <v>64</v>
+      <c r="B9" s="91" t="s">
+        <v>91</v>
+      </c>
+      <c r="C9" s="92" t="s">
+        <v>92</v>
+      </c>
+      <c r="D9" s="94" t="s">
+        <v>63</v>
       </c>
       <c r="AD9" s="36"/>
       <c r="AE9" s="36"/>
@@ -7579,9 +7594,9 @@
       <c r="AH9" s="36"/>
     </row>
     <row r="10" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B10" s="119"/>
-      <c r="C10" s="120"/>
-      <c r="D10" s="124"/>
+      <c r="B10" s="87"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="90"/>
       <c r="AD10" s="36"/>
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
@@ -7589,9 +7604,9 @@
       <c r="AH10" s="36"/>
     </row>
     <row r="11" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B11" s="119"/>
-      <c r="C11" s="120"/>
-      <c r="D11" s="124"/>
+      <c r="B11" s="87"/>
+      <c r="C11" s="88"/>
+      <c r="D11" s="90"/>
       <c r="AD11" s="36"/>
       <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>

</xml_diff>

<commit_message>
Updated residual anomalies document for version 2.0.2
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310193817/Development/Git/Android-ShineLib/Documents/External/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310216383/Philips/android-shinelib/Documents/External/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="689" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22520" tabRatio="689" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -56,6 +56,9 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -64,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="107">
   <si>
     <t>1.1</t>
   </si>
@@ -474,6 +477,33 @@
   </si>
   <si>
     <t>BlueLib doesn't build on a clean development environment</t>
+  </si>
+  <si>
+    <t>BL-395</t>
+  </si>
+  <si>
+    <t>IndexOutOfBoundsException in BlueLib</t>
+  </si>
+  <si>
+    <t>BL-396</t>
+  </si>
+  <si>
+    <t>NullPointerException in BlueLib using example App</t>
+  </si>
+  <si>
+    <t>0.5</t>
+  </si>
+  <si>
+    <t>2016-SEP-21</t>
+  </si>
+  <si>
+    <t>Peter Fortuin</t>
+  </si>
+  <si>
+    <t>2.0.2 Release</t>
+  </si>
+  <si>
+    <t>Anomalies updated</t>
   </si>
 </sst>
 </file>
@@ -804,7 +834,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1039,6 +1069,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1047,7 +1105,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="128">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1217,17 +1275,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="36" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="34" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="39" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="34" fillId="0" borderId="17" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1239,6 +1288,11 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="19" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1309,6 +1363,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -2399,7 +2454,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="110" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2553,7 +2608,7 @@
         <v>14</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="D14" s="97"/>
       <c r="E14" s="97"/>
@@ -2863,8 +2918,8 @@
   </sheetPr>
   <dimension ref="B1:N179"/>
   <sheetViews>
-    <sheetView view="pageLayout" topLeftCell="A9" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3062,11 +3117,21 @@
       <c r="N10" s="17"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
-      <c r="F11" s="17"/>
+      <c r="B11" s="127" t="s">
+        <v>102</v>
+      </c>
+      <c r="C11" s="127" t="s">
+        <v>103</v>
+      </c>
+      <c r="D11" s="127" t="s">
+        <v>104</v>
+      </c>
+      <c r="E11" s="127" t="s">
+        <v>106</v>
+      </c>
+      <c r="F11" s="127" t="s">
+        <v>105</v>
+      </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
       <c r="I11" s="17"/>
@@ -5949,7 +6014,7 @@
   <dimension ref="B1:AJ11"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6701,7 +6766,7 @@
         <v>62</v>
       </c>
       <c r="C7" s="82">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D7" s="39"/>
     </row>
@@ -6710,7 +6775,7 @@
         <v>63</v>
       </c>
       <c r="C8" s="84">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D8" s="39"/>
     </row>
@@ -6763,8 +6828,8 @@
   </sheetPr>
   <dimension ref="B1:AH27"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7482,13 +7547,13 @@
       <c r="C2" s="36"/>
     </row>
     <row r="3" spans="2:34" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="89" t="s">
+      <c r="B3" s="87" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="89" t="s">
+      <c r="C3" s="87" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="89" t="s">
+      <c r="D3" s="87" t="s">
         <v>72</v>
       </c>
       <c r="AD3" s="36"/>
@@ -7498,13 +7563,13 @@
       <c r="AH3" s="36"/>
     </row>
     <row r="4" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B4" s="91" t="s">
+      <c r="B4" s="88" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="92" t="s">
+      <c r="C4" s="89" t="s">
         <v>58</v>
       </c>
-      <c r="D4" s="93" t="s">
+      <c r="D4" s="90" t="s">
         <v>62</v>
       </c>
       <c r="AD4" s="36"/>
@@ -7514,13 +7579,13 @@
       <c r="AH4" s="36"/>
     </row>
     <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B5" s="91" t="s">
+      <c r="B5" s="88" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="92" t="s">
+      <c r="C5" s="89" t="s">
         <v>95</v>
       </c>
-      <c r="D5" s="93" t="s">
+      <c r="D5" s="90" t="s">
         <v>62</v>
       </c>
       <c r="AD5" s="36"/>
@@ -7530,13 +7595,13 @@
       <c r="AH5" s="36"/>
     </row>
     <row r="6" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B6" s="91" t="s">
+      <c r="B6" s="88" t="s">
         <v>96</v>
       </c>
-      <c r="C6" s="92" t="s">
+      <c r="C6" s="89" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="93" t="s">
+      <c r="D6" s="90" t="s">
         <v>62</v>
       </c>
       <c r="AD6" s="36"/>
@@ -7545,15 +7610,15 @@
       <c r="AG6" s="36"/>
       <c r="AH6" s="36"/>
     </row>
-    <row r="7" spans="2:34" ht="32" x14ac:dyDescent="0.15">
-      <c r="B7" s="91" t="s">
-        <v>90</v>
-      </c>
-      <c r="C7" s="92" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7" s="94" t="s">
-        <v>63</v>
+    <row r="7" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+      <c r="B7" s="92" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="D7" s="90" t="s">
+        <v>62</v>
       </c>
       <c r="AD7" s="36"/>
       <c r="AE7" s="36"/>
@@ -7562,13 +7627,13 @@
       <c r="AH7" s="36"/>
     </row>
     <row r="8" spans="2:34" ht="32" x14ac:dyDescent="0.15">
-      <c r="B8" s="91" t="s">
-        <v>88</v>
-      </c>
-      <c r="C8" s="92" t="s">
-        <v>73</v>
-      </c>
-      <c r="D8" s="94" t="s">
+      <c r="B8" s="88" t="s">
+        <v>90</v>
+      </c>
+      <c r="C8" s="89" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="91" t="s">
         <v>63</v>
       </c>
       <c r="AD8" s="36"/>
@@ -7577,14 +7642,14 @@
       <c r="AG8" s="36"/>
       <c r="AH8" s="36"/>
     </row>
-    <row r="9" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B9" s="91" t="s">
-        <v>91</v>
-      </c>
-      <c r="C9" s="92" t="s">
-        <v>92</v>
-      </c>
-      <c r="D9" s="94" t="s">
+    <row r="9" spans="2:34" ht="32" x14ac:dyDescent="0.15">
+      <c r="B9" s="88" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="89" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="91" t="s">
         <v>63</v>
       </c>
       <c r="AD9" s="36"/>
@@ -7594,19 +7659,31 @@
       <c r="AH9" s="36"/>
     </row>
     <row r="10" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B10" s="87"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="90"/>
+      <c r="B10" s="88" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" s="89" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" s="91" t="s">
+        <v>63</v>
+      </c>
       <c r="AD10" s="36"/>
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
       <c r="AG10" s="36"/>
       <c r="AH10" s="36"/>
     </row>
-    <row r="11" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B11" s="87"/>
-      <c r="C11" s="88"/>
-      <c r="D11" s="90"/>
+    <row r="11" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+      <c r="B11" s="93" t="s">
+        <v>100</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="D11" s="91" t="s">
+        <v>63</v>
+      </c>
       <c r="AD11" s="36"/>
       <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
@@ -7705,17 +7782,19 @@
     <hyperlink ref="B4" r:id="rId1"/>
     <hyperlink ref="B5" r:id="rId2"/>
     <hyperlink ref="B6" r:id="rId3"/>
-    <hyperlink ref="B7" r:id="rId4"/>
-    <hyperlink ref="B8" r:id="rId5"/>
-    <hyperlink ref="B9" r:id="rId6"/>
+    <hyperlink ref="B8" r:id="rId4"/>
+    <hyperlink ref="B9" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId6"/>
+    <hyperlink ref="B7" r:id="rId7"/>
+    <hyperlink ref="B11" r:id="rId8"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
-  <pageSetup paperSize="9" fitToHeight="100" orientation="landscape" r:id="rId7"/>
+  <pageSetup paperSize="9" fitToHeight="100" orientation="landscape" r:id="rId9"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
     <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId8"/>
+  <drawing r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
[Release 2.0.3]: Updated residual anomalies document
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26709"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310216383/Philips/android-shinelib/Documents/External/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310193817/Development/Git/android-shinelib/Documents/External/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22520" tabRatio="689" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="689" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -56,9 +56,6 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -67,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
   <si>
     <t>1.1</t>
   </si>
@@ -504,6 +501,18 @@
   </si>
   <si>
     <t>Anomalies updated</t>
+  </si>
+  <si>
+    <t>0.6</t>
+  </si>
+  <si>
+    <t>2016-SEP-27</t>
+  </si>
+  <si>
+    <t>2.0.3 Release</t>
+  </si>
+  <si>
+    <t>No changes needed.</t>
   </si>
 </sst>
 </file>
@@ -1295,6 +1304,7 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1363,7 +1373,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
@@ -2504,11 +2513,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="95"/>
-      <c r="C6" s="95"/>
-      <c r="D6" s="95"/>
-      <c r="E6" s="95"/>
-      <c r="F6" s="95"/>
+      <c r="B6" s="96"/>
+      <c r="C6" s="96"/>
+      <c r="D6" s="96"/>
+      <c r="E6" s="96"/>
+      <c r="F6" s="96"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2574,10 +2583,10 @@
       <c r="C12" s="63" t="s">
         <v>48</v>
       </c>
-      <c r="D12" s="96" t="s">
+      <c r="D12" s="97" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="96"/>
+      <c r="E12" s="97"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
@@ -2592,10 +2601,10 @@
       <c r="C13" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="97" t="s">
+      <c r="D13" s="98" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="97"/>
+      <c r="E13" s="98"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
@@ -2610,8 +2619,8 @@
       <c r="C14" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="D14" s="97"/>
-      <c r="E14" s="97"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="98"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
@@ -2735,11 +2744,11 @@
       <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="104" t="s">
+      <c r="D6" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="105"/>
-      <c r="F6" s="106"/>
+      <c r="E6" s="106"/>
+      <c r="F6" s="107"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
@@ -2748,11 +2757,11 @@
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="107" t="s">
+      <c r="D7" s="108" t="s">
         <v>53</v>
       </c>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
+      <c r="E7" s="108"/>
+      <c r="F7" s="108"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
@@ -2804,27 +2813,27 @@
       <c r="D12" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="108" t="s">
+      <c r="E12" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="108"/>
+      <c r="F12" s="109"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
       <c r="D13" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="98" t="s">
+      <c r="E13" s="99" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="99"/>
+      <c r="F13" s="100"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
       <c r="C14" s="31"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="100"/>
-      <c r="F14" s="101"/>
+      <c r="E14" s="101"/>
+      <c r="F14" s="102"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
@@ -2837,8 +2846,8 @@
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="102"/>
-      <c r="F16" s="103"/>
+      <c r="E16" s="103"/>
+      <c r="F16" s="104"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
@@ -2919,7 +2928,7 @@
   <dimension ref="B1:N179"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3117,19 +3126,19 @@
       <c r="N10" s="17"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B11" s="127" t="s">
+      <c r="B11" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="C11" s="127" t="s">
+      <c r="C11" s="95" t="s">
         <v>103</v>
       </c>
-      <c r="D11" s="127" t="s">
+      <c r="D11" s="95" t="s">
         <v>104</v>
       </c>
-      <c r="E11" s="127" t="s">
+      <c r="E11" s="95" t="s">
         <v>106</v>
       </c>
-      <c r="F11" s="127" t="s">
+      <c r="F11" s="95" t="s">
         <v>105</v>
       </c>
       <c r="G11" s="17"/>
@@ -3142,11 +3151,21 @@
       <c r="N11" s="17"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="17"/>
+      <c r="B12" s="95" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12" s="95" t="s">
+        <v>108</v>
+      </c>
+      <c r="D12" s="95" t="s">
+        <v>51</v>
+      </c>
+      <c r="E12" s="95" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="95" t="s">
+        <v>109</v>
+      </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
       <c r="I12" s="17"/>
@@ -5785,19 +5804,19 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="115" t="s">
+      <c r="B4" s="116" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="116"/>
-      <c r="D4" s="116"/>
-      <c r="E4" s="116"/>
-      <c r="F4" s="116"/>
-      <c r="G4" s="116"/>
-      <c r="H4" s="116"/>
-      <c r="I4" s="116"/>
-      <c r="J4" s="116"/>
-      <c r="K4" s="116"/>
-      <c r="L4" s="116"/>
+      <c r="C4" s="117"/>
+      <c r="D4" s="117"/>
+      <c r="E4" s="117"/>
+      <c r="F4" s="117"/>
+      <c r="G4" s="117"/>
+      <c r="H4" s="117"/>
+      <c r="I4" s="117"/>
+      <c r="J4" s="117"/>
+      <c r="K4" s="117"/>
+      <c r="L4" s="117"/>
     </row>
     <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
@@ -5816,29 +5835,29 @@
       <c r="B6" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="117" t="s">
+      <c r="C6" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="118"/>
-      <c r="E6" s="118"/>
-      <c r="F6" s="118"/>
-      <c r="G6" s="118"/>
-      <c r="H6" s="118"/>
-      <c r="I6" s="119"/>
+      <c r="D6" s="119"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="119"/>
+      <c r="G6" s="119"/>
+      <c r="H6" s="119"/>
+      <c r="I6" s="120"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B7" s="76" t="s">
         <v>60</v>
       </c>
-      <c r="C7" s="120" t="s">
+      <c r="C7" s="121" t="s">
         <v>65</v>
       </c>
-      <c r="D7" s="121"/>
-      <c r="E7" s="121"/>
-      <c r="F7" s="121"/>
-      <c r="G7" s="121"/>
-      <c r="H7" s="121"/>
-      <c r="I7" s="122"/>
+      <c r="D7" s="122"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="122"/>
+      <c r="G7" s="122"/>
+      <c r="H7" s="122"/>
+      <c r="I7" s="123"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
       <c r="O7" s="53"/>
@@ -5849,15 +5868,15 @@
       <c r="B8" s="69" t="s">
         <v>61</v>
       </c>
-      <c r="C8" s="123" t="s">
+      <c r="C8" s="124" t="s">
         <v>66</v>
       </c>
-      <c r="D8" s="124"/>
-      <c r="E8" s="124"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="124"/>
-      <c r="H8" s="124"/>
-      <c r="I8" s="125"/>
+      <c r="D8" s="125"/>
+      <c r="E8" s="125"/>
+      <c r="F8" s="125"/>
+      <c r="G8" s="125"/>
+      <c r="H8" s="125"/>
+      <c r="I8" s="126"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
       <c r="O8" s="53"/>
@@ -5868,15 +5887,15 @@
       <c r="B9" s="70" t="s">
         <v>62</v>
       </c>
-      <c r="C9" s="112" t="s">
+      <c r="C9" s="113" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="113"/>
-      <c r="E9" s="113"/>
-      <c r="F9" s="113"/>
-      <c r="G9" s="113"/>
-      <c r="H9" s="113"/>
-      <c r="I9" s="114"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="114"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="114"/>
+      <c r="H9" s="114"/>
+      <c r="I9" s="115"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
       <c r="O9" s="53"/>
@@ -5901,15 +5920,15 @@
       <c r="B11" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="C11" s="109" t="s">
+      <c r="C11" s="110" t="s">
         <v>69</v>
       </c>
-      <c r="D11" s="110"/>
-      <c r="E11" s="110"/>
-      <c r="F11" s="110"/>
-      <c r="G11" s="110"/>
-      <c r="H11" s="110"/>
-      <c r="I11" s="111"/>
+      <c r="D11" s="111"/>
+      <c r="E11" s="111"/>
+      <c r="F11" s="111"/>
+      <c r="G11" s="111"/>
+      <c r="H11" s="111"/>
+      <c r="I11" s="112"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
       <c r="C12" s="66"/>
@@ -6732,11 +6751,11 @@
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="126" t="s">
+      <c r="B3" s="127" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="126"/>
-      <c r="D3" s="126"/>
+      <c r="C3" s="127"/>
+      <c r="D3" s="127"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="39"/>

</xml_diff>

<commit_message>
updated residual anomalies document after formal review session for 2.0.3 release
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26709"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27715"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310193817/Development/Git/android-shinelib/Documents/External/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/310088528p/dev/android-shinelib/Documents/External/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16000" tabRatio="689" activeTab="2"/>
+    <workbookView xWindow="-2260" yWindow="-19500" windowWidth="28800" windowHeight="15940" tabRatio="689" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -43,7 +43,7 @@
     <definedName name="ListYN" localSheetId="5">#REF!</definedName>
     <definedName name="ListYN" localSheetId="4">#REF!</definedName>
     <definedName name="ListYN">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">Anomalies!$A$1:$F$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">Anomalies!$A$1:$F$35</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Document Introduction'!$A$1:$G$26</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="3">Introduction!$A$1:$M$20</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="4">'Maturity Grid'!$A$1:$E$23</definedName>
@@ -56,6 +56,9 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -64,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="111">
   <si>
     <t>1.1</t>
   </si>
@@ -242,9 +245,6 @@
     <t>2016-JUL-11</t>
   </si>
   <si>
-    <t>draft</t>
-  </si>
-  <si>
     <t>NatKuz-20160711-01V01</t>
   </si>
   <si>
@@ -325,9 +325,6 @@
     <t>Association with LifeSense BPM can fail unexpectedly on some Android combos</t>
   </si>
   <si>
-    <t>Crash , associating when bluetooth turned off</t>
-  </si>
-  <si>
     <t>Thijs Winter</t>
   </si>
   <si>
@@ -449,9 +446,6 @@
     <t>BL-95</t>
   </si>
   <si>
-    <t>BL-88</t>
-  </si>
-  <si>
     <t>BL-22</t>
   </si>
   <si>
@@ -461,21 +455,12 @@
     <t>Reconnect fails with Nexus 5, 4.4.2</t>
   </si>
   <si>
-    <t>Conclusion: The build cannot be released to clients due to 3 major  defects.</t>
-  </si>
-  <si>
     <t>BL-390</t>
   </si>
   <si>
     <t>NPE when calling readRssi()</t>
   </si>
   <si>
-    <t>BL-392</t>
-  </si>
-  <si>
-    <t>BlueLib doesn't build on a clean development environment</t>
-  </si>
-  <si>
     <t>BL-395</t>
   </si>
   <si>
@@ -513,13 +498,49 @@
   </si>
   <si>
     <t>No changes needed.</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Conclusion: The build </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t>can</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> be released.</t>
+    </r>
+  </si>
+  <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>2016-DEC-20</t>
+  </si>
+  <si>
+    <t>Bas Flaton</t>
+  </si>
+  <si>
+    <t>Updated to correctly reflect 2.0.3 release anomalies after review</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="41" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -785,6 +806,11 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1293,9 +1319,6 @@
     <xf numFmtId="0" fontId="35" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="35" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1372,6 +1395,9 @@
     <xf numFmtId="0" fontId="38" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -2463,7 +2489,7 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="110" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -2513,11 +2539,11 @@
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="79.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="96"/>
-      <c r="C6" s="96"/>
-      <c r="D6" s="96"/>
-      <c r="E6" s="96"/>
-      <c r="F6" s="96"/>
+      <c r="B6" s="95"/>
+      <c r="C6" s="95"/>
+      <c r="D6" s="95"/>
+      <c r="E6" s="95"/>
+      <c r="F6" s="95"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
@@ -2538,10 +2564,10 @@
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C8" s="35" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D8" s="29" t="s">
         <v>20</v>
@@ -2581,17 +2607,17 @@
         <v>12</v>
       </c>
       <c r="C12" s="63" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="97" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="96" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="97"/>
+      <c r="E12" s="96"/>
       <c r="F12" s="28" t="s">
         <v>16</v>
       </c>
       <c r="G12" s="63" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2601,15 +2627,15 @@
       <c r="C13" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="98" t="s">
+      <c r="D13" s="97" t="s">
         <v>45</v>
       </c>
-      <c r="E13" s="98"/>
+      <c r="E13" s="97"/>
       <c r="F13" s="28" t="s">
         <v>17</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2617,15 +2643,15 @@
         <v>14</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>102</v>
-      </c>
-      <c r="D14" s="98"/>
-      <c r="E14" s="98"/>
+        <v>105</v>
+      </c>
+      <c r="D14" s="97"/>
+      <c r="E14" s="97"/>
       <c r="F14" s="28" t="s">
         <v>18</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2633,7 +2659,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="63" t="s">
-        <v>47</v>
+        <v>107</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>35</v>
@@ -2744,11 +2770,11 @@
       <c r="C6" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="105" t="s">
-        <v>52</v>
-      </c>
-      <c r="E6" s="106"/>
-      <c r="F6" s="107"/>
+      <c r="D6" s="104" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="105"/>
+      <c r="F6" s="106"/>
     </row>
     <row r="7" spans="2:6" ht="48.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="31" t="s">
@@ -2757,11 +2783,11 @@
       <c r="C7" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="108" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" s="108"/>
-      <c r="F7" s="108"/>
+      <c r="D7" s="107" t="s">
+        <v>52</v>
+      </c>
+      <c r="E7" s="107"/>
+      <c r="F7" s="107"/>
     </row>
     <row r="8" spans="2:6" ht="36" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="32" t="s">
@@ -2771,7 +2797,7 @@
         <v>5</v>
       </c>
       <c r="D8" s="16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="54" t="s">
         <v>6</v>
@@ -2783,7 +2809,7 @@
     <row r="9" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="33"/>
       <c r="C9" s="64" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
@@ -2813,27 +2839,27 @@
       <c r="D12" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="109" t="s">
+      <c r="E12" s="108" t="s">
         <v>9</v>
       </c>
-      <c r="F12" s="109"/>
+      <c r="F12" s="108"/>
     </row>
     <row r="13" spans="2:6" ht="57.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B13" s="32"/>
       <c r="D13" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="99" t="s">
+      <c r="E13" s="98" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="100"/>
+      <c r="F13" s="99"/>
     </row>
     <row r="14" spans="2:6" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="33"/>
       <c r="C14" s="31"/>
       <c r="D14" s="18"/>
-      <c r="E14" s="101"/>
-      <c r="F14" s="102"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="101"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B15" s="19"/>
@@ -2846,8 +2872,8 @@
       <c r="B16" s="19"/>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
-      <c r="E16" s="103"/>
-      <c r="F16" s="104"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="103"/>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="50"/>
@@ -2928,7 +2954,7 @@
   <dimension ref="B1:N179"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3027,19 +3053,19 @@
     </row>
     <row r="7" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B7" s="63" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="63" t="s">
         <v>46</v>
       </c>
       <c r="D7" s="63" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E7" s="63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F7" s="63" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G7" s="17"/>
       <c r="H7" s="17"/>
@@ -3052,19 +3078,19 @@
     </row>
     <row r="8" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B8" s="35" t="s">
+        <v>72</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="63" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="E8" s="35" t="s">
-        <v>76</v>
-      </c>
       <c r="F8" s="35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G8" s="17"/>
       <c r="H8" s="17"/>
@@ -3077,19 +3103,19 @@
     </row>
     <row r="9" spans="2:14" ht="14" x14ac:dyDescent="0.15">
       <c r="B9" s="35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C9" s="63" t="s">
+        <v>77</v>
+      </c>
+      <c r="D9" s="63" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="63" t="s">
-        <v>51</v>
-      </c>
-      <c r="E9" s="35" t="s">
-        <v>81</v>
-      </c>
       <c r="F9" s="35" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -3100,21 +3126,21 @@
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
     </row>
-    <row r="10" spans="2:14" ht="56" x14ac:dyDescent="0.15">
+    <row r="10" spans="2:14" ht="42" x14ac:dyDescent="0.15">
       <c r="B10" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>82</v>
+      </c>
+      <c r="D10" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="E10" s="35" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" s="35" t="s">
         <v>84</v>
-      </c>
-      <c r="D10" s="63" t="s">
-        <v>85</v>
-      </c>
-      <c r="E10" s="35" t="s">
-        <v>87</v>
-      </c>
-      <c r="F10" s="35" t="s">
-        <v>86</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -3126,20 +3152,20 @@
       <c r="N10" s="17"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B11" s="95" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="95" t="s">
-        <v>103</v>
-      </c>
-      <c r="D11" s="95" t="s">
-        <v>104</v>
-      </c>
-      <c r="E11" s="95" t="s">
-        <v>106</v>
-      </c>
-      <c r="F11" s="95" t="s">
-        <v>105</v>
+      <c r="B11" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="C11" s="94" t="s">
+        <v>97</v>
+      </c>
+      <c r="D11" s="94" t="s">
+        <v>98</v>
+      </c>
+      <c r="E11" s="94" t="s">
+        <v>100</v>
+      </c>
+      <c r="F11" s="94" t="s">
+        <v>99</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -3151,20 +3177,20 @@
       <c r="N11" s="17"/>
     </row>
     <row r="12" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B12" s="95" t="s">
-        <v>107</v>
-      </c>
-      <c r="C12" s="95" t="s">
-        <v>108</v>
-      </c>
-      <c r="D12" s="95" t="s">
-        <v>51</v>
-      </c>
-      <c r="E12" s="95" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" s="95" t="s">
-        <v>109</v>
+      <c r="B12" s="94" t="s">
+        <v>101</v>
+      </c>
+      <c r="C12" s="94" t="s">
+        <v>102</v>
+      </c>
+      <c r="D12" s="94" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="94" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="94" t="s">
+        <v>103</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -3175,12 +3201,22 @@
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
     </row>
-    <row r="13" spans="2:14" x14ac:dyDescent="0.15">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
-      <c r="F13" s="17"/>
+    <row r="13" spans="2:14" ht="26" x14ac:dyDescent="0.15">
+      <c r="B13" s="94" t="s">
+        <v>105</v>
+      </c>
+      <c r="C13" s="94" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="94" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="127" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="94" t="s">
+        <v>103</v>
+      </c>
       <c r="G13" s="17"/>
       <c r="H13" s="17"/>
       <c r="I13" s="17"/>
@@ -5804,19 +5840,19 @@
       <c r="L3" s="5"/>
     </row>
     <row r="4" spans="2:37" ht="120.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="116" t="s">
-        <v>80</v>
-      </c>
-      <c r="C4" s="117"/>
-      <c r="D4" s="117"/>
-      <c r="E4" s="117"/>
-      <c r="F4" s="117"/>
-      <c r="G4" s="117"/>
-      <c r="H4" s="117"/>
-      <c r="I4" s="117"/>
-      <c r="J4" s="117"/>
-      <c r="K4" s="117"/>
-      <c r="L4" s="117"/>
+      <c r="B4" s="115" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="116"/>
+      <c r="D4" s="116"/>
+      <c r="E4" s="116"/>
+      <c r="F4" s="116"/>
+      <c r="G4" s="116"/>
+      <c r="H4" s="116"/>
+      <c r="I4" s="116"/>
+      <c r="J4" s="116"/>
+      <c r="K4" s="116"/>
+      <c r="L4" s="116"/>
     </row>
     <row r="5" spans="2:37" ht="18.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="47"/>
@@ -5835,29 +5871,29 @@
       <c r="B6" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="C6" s="118" t="s">
+      <c r="C6" s="117" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119"/>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119"/>
-      <c r="I6" s="120"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="118"/>
+      <c r="F6" s="118"/>
+      <c r="G6" s="118"/>
+      <c r="H6" s="118"/>
+      <c r="I6" s="119"/>
     </row>
     <row r="7" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B7" s="76" t="s">
-        <v>60</v>
-      </c>
-      <c r="C7" s="121" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" s="122"/>
-      <c r="E7" s="122"/>
-      <c r="F7" s="122"/>
-      <c r="G7" s="122"/>
-      <c r="H7" s="122"/>
-      <c r="I7" s="123"/>
+        <v>58</v>
+      </c>
+      <c r="C7" s="120" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="121"/>
+      <c r="E7" s="121"/>
+      <c r="F7" s="121"/>
+      <c r="G7" s="121"/>
+      <c r="H7" s="121"/>
+      <c r="I7" s="122"/>
       <c r="M7" s="53"/>
       <c r="N7" s="53"/>
       <c r="O7" s="53"/>
@@ -5866,17 +5902,17 @@
     </row>
     <row r="8" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B8" s="69" t="s">
-        <v>61</v>
-      </c>
-      <c r="C8" s="124" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" s="125"/>
-      <c r="E8" s="125"/>
-      <c r="F8" s="125"/>
-      <c r="G8" s="125"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="126"/>
+        <v>59</v>
+      </c>
+      <c r="C8" s="123" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="124"/>
+      <c r="E8" s="124"/>
+      <c r="F8" s="124"/>
+      <c r="G8" s="124"/>
+      <c r="H8" s="124"/>
+      <c r="I8" s="125"/>
       <c r="M8" s="53"/>
       <c r="N8" s="53"/>
       <c r="O8" s="53"/>
@@ -5885,17 +5921,17 @@
     </row>
     <row r="9" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B9" s="70" t="s">
-        <v>62</v>
-      </c>
-      <c r="C9" s="113" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="114"/>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="115"/>
+        <v>60</v>
+      </c>
+      <c r="C9" s="112" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="113"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="113"/>
+      <c r="G9" s="113"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="114"/>
       <c r="M9" s="53"/>
       <c r="N9" s="53"/>
       <c r="O9" s="53"/>
@@ -5904,10 +5940,10 @@
     </row>
     <row r="10" spans="2:37" x14ac:dyDescent="0.2">
       <c r="B10" s="71" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D10" s="73"/>
       <c r="E10" s="73"/>
@@ -5918,17 +5954,17 @@
     </row>
     <row r="11" spans="2:37" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="75" t="s">
-        <v>64</v>
-      </c>
-      <c r="C11" s="110" t="s">
-        <v>69</v>
-      </c>
-      <c r="D11" s="111"/>
-      <c r="E11" s="111"/>
-      <c r="F11" s="111"/>
-      <c r="G11" s="111"/>
-      <c r="H11" s="111"/>
-      <c r="I11" s="112"/>
+        <v>62</v>
+      </c>
+      <c r="C11" s="109" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="110"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="110"/>
+      <c r="G11" s="110"/>
+      <c r="H11" s="110"/>
+      <c r="I11" s="111"/>
     </row>
     <row r="12" spans="2:37" ht="18" x14ac:dyDescent="0.2">
       <c r="C12" s="66"/>
@@ -6030,10 +6066,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AJ11"/>
+  <dimension ref="B1:D11"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6042,13 +6078,12 @@
     <col min="2" max="2" width="31.5" style="37" customWidth="1"/>
     <col min="3" max="3" width="6.1640625" style="37" customWidth="1"/>
     <col min="4" max="4" width="47.33203125" style="38" customWidth="1"/>
-    <col min="5" max="5" width="17.33203125" style="38" customWidth="1"/>
-    <col min="6" max="6" width="31.33203125" style="38" customWidth="1"/>
-    <col min="7" max="7" width="17.33203125" style="38" customWidth="1"/>
-    <col min="8" max="26" width="3.33203125" style="38" customWidth="1"/>
-    <col min="27" max="27" width="10" style="38" customWidth="1"/>
-    <col min="28" max="36" width="8.83203125" style="38"/>
-    <col min="37" max="237" width="8.83203125" style="36"/>
+    <col min="5" max="5" width="17.33203125" style="36" customWidth="1"/>
+    <col min="6" max="6" width="31.33203125" style="36" customWidth="1"/>
+    <col min="7" max="7" width="17.33203125" style="36" customWidth="1"/>
+    <col min="8" max="26" width="3.33203125" style="36" customWidth="1"/>
+    <col min="27" max="27" width="10" style="36" customWidth="1"/>
+    <col min="28" max="237" width="8.83203125" style="36"/>
     <col min="238" max="238" width="1.5" style="36" customWidth="1"/>
     <col min="239" max="239" width="1.33203125" style="36" customWidth="1"/>
     <col min="240" max="240" width="42" style="36" customWidth="1"/>
@@ -6751,11 +6786,11 @@
     </row>
     <row r="2" spans="2:4" ht="30.5" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="3" spans="2:4" ht="13.25" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="127" t="s">
+      <c r="B3" s="126" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="127"/>
-      <c r="D3" s="127"/>
+      <c r="C3" s="126"/>
+      <c r="D3" s="126"/>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B4" s="39"/>
@@ -6764,7 +6799,7 @@
     </row>
     <row r="5" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="77" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C5" s="78">
         <v>0</v>
@@ -6773,7 +6808,7 @@
     </row>
     <row r="6" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B6" s="79" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C6" s="80">
         <v>0</v>
@@ -6782,25 +6817,25 @@
     </row>
     <row r="7" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B7" s="81" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C7" s="82">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D7" s="39"/>
     </row>
     <row r="8" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="83" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C8" s="84">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D8" s="39"/>
     </row>
     <row r="9" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B9" s="85" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C9" s="86">
         <v>0</v>
@@ -6814,7 +6849,7 @@
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="40" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6845,10 +6880,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:AH27"/>
+  <dimension ref="B1:AH25"/>
   <sheetViews>
     <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7567,13 +7602,13 @@
     </row>
     <row r="3" spans="2:34" ht="39.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="87" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="87" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="87" t="s">
         <v>70</v>
-      </c>
-      <c r="C3" s="87" t="s">
-        <v>71</v>
-      </c>
-      <c r="D3" s="87" t="s">
-        <v>72</v>
       </c>
       <c r="AD3" s="36"/>
       <c r="AE3" s="36"/>
@@ -7583,13 +7618,13 @@
     </row>
     <row r="4" spans="2:34" ht="16" x14ac:dyDescent="0.15">
       <c r="B4" s="88" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C4" s="89" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="D4" s="90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD4" s="36"/>
       <c r="AE4" s="36"/>
@@ -7597,15 +7632,15 @@
       <c r="AG4" s="36"/>
       <c r="AH4" s="36"/>
     </row>
-    <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B5" s="88" t="s">
-        <v>94</v>
+    <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+      <c r="B5" s="91" t="s">
+        <v>92</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D5" s="90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD5" s="36"/>
       <c r="AE5" s="36"/>
@@ -7613,15 +7648,15 @@
       <c r="AG5" s="36"/>
       <c r="AH5" s="36"/>
     </row>
-    <row r="6" spans="2:34" ht="16" x14ac:dyDescent="0.15">
+    <row r="6" spans="2:34" ht="32" x14ac:dyDescent="0.15">
       <c r="B6" s="88" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C6" s="89" t="s">
-        <v>97</v>
+        <v>56</v>
       </c>
       <c r="D6" s="90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD6" s="36"/>
       <c r="AE6" s="36"/>
@@ -7629,15 +7664,15 @@
       <c r="AG6" s="36"/>
       <c r="AH6" s="36"/>
     </row>
-    <row r="7" spans="2:34" ht="16" x14ac:dyDescent="0.2">
-      <c r="B7" s="92" t="s">
-        <v>98</v>
+    <row r="7" spans="2:34" ht="32" x14ac:dyDescent="0.15">
+      <c r="B7" s="88" t="s">
+        <v>86</v>
       </c>
       <c r="C7" s="89" t="s">
-        <v>99</v>
+        <v>71</v>
       </c>
       <c r="D7" s="90" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AD7" s="36"/>
       <c r="AE7" s="36"/>
@@ -7645,15 +7680,15 @@
       <c r="AG7" s="36"/>
       <c r="AH7" s="36"/>
     </row>
-    <row r="8" spans="2:34" ht="32" x14ac:dyDescent="0.15">
+    <row r="8" spans="2:34" ht="16" x14ac:dyDescent="0.15">
       <c r="B8" s="88" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C8" s="89" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8" s="91" t="s">
-        <v>63</v>
+        <v>89</v>
+      </c>
+      <c r="D8" s="90" t="s">
+        <v>61</v>
       </c>
       <c r="AD8" s="36"/>
       <c r="AE8" s="36"/>
@@ -7661,15 +7696,15 @@
       <c r="AG8" s="36"/>
       <c r="AH8" s="36"/>
     </row>
-    <row r="9" spans="2:34" ht="32" x14ac:dyDescent="0.15">
-      <c r="B9" s="88" t="s">
-        <v>88</v>
-      </c>
-      <c r="C9" s="89" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="91" t="s">
-        <v>63</v>
+    <row r="9" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+      <c r="B9" s="92" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="D9" s="90" t="s">
+        <v>61</v>
       </c>
       <c r="AD9" s="36"/>
       <c r="AE9" s="36"/>
@@ -7677,32 +7712,20 @@
       <c r="AG9" s="36"/>
       <c r="AH9" s="36"/>
     </row>
-    <row r="10" spans="2:34" ht="16" x14ac:dyDescent="0.15">
-      <c r="B10" s="88" t="s">
-        <v>91</v>
-      </c>
-      <c r="C10" s="89" t="s">
-        <v>92</v>
-      </c>
-      <c r="D10" s="91" t="s">
-        <v>63</v>
-      </c>
+    <row r="10" spans="2:34" ht="14" x14ac:dyDescent="0.15">
+      <c r="B10" s="20"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="51"/>
       <c r="AD10" s="36"/>
       <c r="AE10" s="36"/>
       <c r="AF10" s="36"/>
       <c r="AG10" s="36"/>
       <c r="AH10" s="36"/>
     </row>
-    <row r="11" spans="2:34" ht="16" x14ac:dyDescent="0.2">
-      <c r="B11" s="93" t="s">
-        <v>100</v>
-      </c>
-      <c r="C11" s="94" t="s">
-        <v>101</v>
-      </c>
-      <c r="D11" s="91" t="s">
-        <v>63</v>
-      </c>
+    <row r="11" spans="2:34" ht="14" x14ac:dyDescent="0.15">
+      <c r="B11" s="50"/>
+      <c r="C11" s="50"/>
+      <c r="D11" s="51"/>
       <c r="AD11" s="36"/>
       <c r="AE11" s="36"/>
       <c r="AF11" s="36"/>
@@ -7710,24 +7733,14 @@
       <c r="AH11" s="36"/>
     </row>
     <row r="12" spans="2:34" ht="14" x14ac:dyDescent="0.15">
-      <c r="B12" s="20"/>
+      <c r="B12" s="50"/>
       <c r="C12" s="50"/>
       <c r="D12" s="51"/>
-      <c r="AD12" s="36"/>
-      <c r="AE12" s="36"/>
-      <c r="AF12" s="36"/>
-      <c r="AG12" s="36"/>
-      <c r="AH12" s="36"/>
     </row>
     <row r="13" spans="2:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B13" s="50"/>
       <c r="C13" s="50"/>
       <c r="D13" s="51"/>
-      <c r="AD13" s="36"/>
-      <c r="AE13" s="36"/>
-      <c r="AF13" s="36"/>
-      <c r="AG13" s="36"/>
-      <c r="AH13" s="36"/>
     </row>
     <row r="14" spans="2:34" ht="14" x14ac:dyDescent="0.15">
       <c r="B14" s="50"/>
@@ -7776,44 +7789,32 @@
     </row>
     <row r="23" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B23" s="50"/>
-      <c r="C23" s="50"/>
-      <c r="D23" s="51"/>
+      <c r="C23" s="20"/>
     </row>
     <row r="24" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B24" s="50"/>
-      <c r="C24" s="50"/>
-      <c r="D24" s="51"/>
     </row>
     <row r="25" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B25" s="50"/>
-      <c r="C25" s="20"/>
-    </row>
-    <row r="26" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B26" s="50"/>
-    </row>
-    <row r="27" spans="2:4" ht="14" x14ac:dyDescent="0.15">
-      <c r="B27" s="50"/>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0"/>
   <phoneticPr fontId="28" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1"/>
-    <hyperlink ref="B5" r:id="rId2"/>
-    <hyperlink ref="B6" r:id="rId3"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
     <hyperlink ref="B8" r:id="rId4"/>
-    <hyperlink ref="B9" r:id="rId5"/>
-    <hyperlink ref="B10" r:id="rId6"/>
-    <hyperlink ref="B7" r:id="rId7"/>
-    <hyperlink ref="B11" r:id="rId8"/>
+    <hyperlink ref="B5" r:id="rId5"/>
+    <hyperlink ref="B9" r:id="rId6"/>
   </hyperlinks>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.74803149606299202" bottom="1.2480314960000001" header="0.31496062992126" footer="0.31496063000000002"/>
-  <pageSetup paperSize="9" fitToHeight="100" orientation="landscape" r:id="rId9"/>
+  <pageSetup paperSize="9" fitToHeight="100" orientation="landscape" r:id="rId7"/>
   <headerFooter>
     <oddHeader>&amp;L&amp;"-,Bold"&amp;24CDPP</oddHeader>
     <oddFooter>&amp;L&amp;12&amp;F_x000D_Version 0.3&amp;CInternal Use Only&amp;R&amp;P/&amp;N</oddFooter>
   </headerFooter>
-  <drawing r:id="rId10"/>
+  <drawing r:id="rId8"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="1" OnePage="0" WScale="100"/>

</xml_diff>

<commit_message>
Removed iOS stories from Residual Anomalies document
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" tabRatio="689" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" tabRatio="689" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="127">
   <si>
     <t>1.1</t>
   </si>
@@ -512,12 +512,6 @@
     <t>[Android] Future timestamp is displayed during thermometer reading sync</t>
   </si>
   <si>
-    <t>DE14605</t>
-  </si>
-  <si>
-    <t>Bug 32982: [iOS] The "BT not on" error message does not appear when you try to sync Moonshine with BT off</t>
-  </si>
-  <si>
     <t>DE14608</t>
   </si>
   <si>
@@ -558,12 +552,6 @@
   </si>
   <si>
     <t>[Android] Reconnect fails with Nexus 5, 4.4.2</t>
-  </si>
-  <si>
-    <t>DE14619</t>
-  </si>
-  <si>
-    <t>[iOS] The bluetooth on/off update is not triggered</t>
   </si>
   <si>
     <t>DE14620</t>
@@ -2669,7 +2657,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D13" s="98" t="s">
         <v>44</v>
@@ -3002,7 +2990,7 @@
   </sheetPr>
   <dimension ref="B1:N179"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
+    <sheetView view="pageLayout" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3278,7 +3266,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="87" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D14" s="87" t="s">
         <v>82</v>
@@ -3287,7 +3275,7 @@
         <v>84</v>
       </c>
       <c r="F14" s="87" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -6939,8 +6927,8 @@
   </sheetPr>
   <dimension ref="B1:AH25"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7705,7 +7693,7 @@
       <c r="AG5" s="35"/>
       <c r="AH5" s="35"/>
     </row>
-    <row r="6" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="91" t="s">
         <v>103</v>
       </c>
@@ -7754,7 +7742,7 @@
       <c r="C9" s="92" t="s">
         <v>110</v>
       </c>
-      <c r="D9" s="94"/>
+      <c r="D9" s="93"/>
       <c r="AD9" s="35"/>
       <c r="AE9" s="35"/>
       <c r="AF9" s="35"/>
@@ -7798,7 +7786,7 @@
       </c>
       <c r="D12" s="93"/>
     </row>
-    <row r="13" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B13" s="91" t="s">
         <v>117</v>
       </c>
@@ -7814,9 +7802,11 @@
       <c r="C14" s="92" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="93"/>
-    </row>
-    <row r="15" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+      <c r="D14" s="95" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B15" s="91" t="s">
         <v>121</v>
       </c>
@@ -7825,34 +7815,14 @@
       </c>
       <c r="D15" s="93"/>
     </row>
-    <row r="16" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B16" s="91" t="s">
         <v>123</v>
       </c>
       <c r="C16" s="92" t="s">
         <v>124</v>
       </c>
-      <c r="D16" s="95" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="B17" s="91" t="s">
-        <v>125</v>
-      </c>
-      <c r="C17" s="92" t="s">
-        <v>126</v>
-      </c>
-      <c r="D17" s="93"/>
-    </row>
-    <row r="18" spans="2:4" ht="32" x14ac:dyDescent="0.2">
-      <c r="B18" s="91" t="s">
-        <v>127</v>
-      </c>
-      <c r="C18" s="92" t="s">
-        <v>128</v>
-      </c>
-      <c r="D18" s="93"/>
+      <c r="D16" s="93"/>
     </row>
     <row r="19" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="49"/>

</xml_diff>

<commit_message>
Update to Residual Anomalies document (discussed with Joost)
</commit_message>
<xml_diff>
--- a/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
+++ b/Documents/External/Residual_Anomalies_BlueLib_Android_NatKuz-20160711-01V01.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" tabRatio="689" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="22440" tabRatio="689" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Title Page" sheetId="3" r:id="rId1"/>
@@ -67,7 +67,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="125">
   <si>
     <t>1.1</t>
   </si>
@@ -455,8 +455,110 @@
     <t>1.0</t>
   </si>
   <si>
+    <t>approved</t>
+  </si>
+  <si>
+    <t>2016-DEC-20</t>
+  </si>
+  <si>
+    <t>Bas Flaton</t>
+  </si>
+  <si>
+    <t>Updated to correctly reflect 2.0.3 release anomalies after review</t>
+  </si>
+  <si>
+    <t>https://bitbucket.atlas.philips.com/projects/EHSHN/repos/android-shinelib/browse/Documents/External/</t>
+  </si>
+  <si>
+    <t>Ernest Anglès Isern</t>
+  </si>
+  <si>
+    <t>Lead Architect Connectivity / Chief Product Owner</t>
+  </si>
+  <si>
+    <t>For internal use</t>
+  </si>
+  <si>
+    <t>DE13270</t>
+  </si>
+  <si>
+    <t>[Android] Thermometer Pairing issues Android N</t>
+  </si>
+  <si>
+    <t>DE14608</t>
+  </si>
+  <si>
+    <t>[Android] BlueLib doesn't build on a clean development environment</t>
+  </si>
+  <si>
+    <t>DE14613</t>
+  </si>
+  <si>
+    <t>Bug 43674: [Android] Crash observed when syncing continously</t>
+  </si>
+  <si>
+    <t>DE14614</t>
+  </si>
+  <si>
+    <t>[Android] DiCommChannel is not resilient against leading garbage</t>
+  </si>
+  <si>
+    <t>DE14615</t>
+  </si>
+  <si>
+    <t>[Android] NullPointerException in BlueLib using example App</t>
+  </si>
+  <si>
+    <t>DE14616</t>
+  </si>
+  <si>
+    <t>[Android] IndexOutOfBoundsException</t>
+  </si>
+  <si>
+    <t>DE14617</t>
+  </si>
+  <si>
+    <t>[Android] NPE when calling readRssi()</t>
+  </si>
+  <si>
+    <t>DE14618</t>
+  </si>
+  <si>
+    <t>[Android] Reconnect fails with Nexus 5, 4.4.2</t>
+  </si>
+  <si>
+    <t>DE14620</t>
+  </si>
+  <si>
+    <t>[Android] SHNDeviceImpl should actively disconnect when not all expected services are discovered</t>
+  </si>
+  <si>
+    <t>DE14677</t>
+  </si>
+  <si>
+    <t>[Android] App crashes on launch of the application</t>
+  </si>
+  <si>
+    <t>DE15010</t>
+  </si>
+  <si>
+    <t>TFS-49782 [Android] App Crashes on launch after the app upgrade</t>
+  </si>
+  <si>
+    <t>DE15038</t>
+  </si>
+  <si>
+    <t>[Android] TFS-40215:After Unpairing Moonshine and Pairing it back to same User is failing.</t>
+  </si>
+  <si>
+    <t>2017-FEB-28</t>
+  </si>
+  <si>
+    <t>2.3.2 Release</t>
+  </si>
+  <si>
     <r>
-      <t xml:space="preserve">Conclusion: The build </t>
+      <t xml:space="preserve">Conclusion: There are 2 major issues. Both are waiting for external input. The build </t>
     </r>
     <r>
       <rPr>
@@ -474,114 +576,6 @@
       </rPr>
       <t xml:space="preserve"> be released.</t>
     </r>
-  </si>
-  <si>
-    <t>approved</t>
-  </si>
-  <si>
-    <t>2016-DEC-20</t>
-  </si>
-  <si>
-    <t>Bas Flaton</t>
-  </si>
-  <si>
-    <t>Updated to correctly reflect 2.0.3 release anomalies after review</t>
-  </si>
-  <si>
-    <t>https://bitbucket.atlas.philips.com/projects/EHSHN/repos/android-shinelib/browse/Documents/External/</t>
-  </si>
-  <si>
-    <t>Ernest Anglès Isern</t>
-  </si>
-  <si>
-    <t>Lead Architect Connectivity / Chief Product Owner</t>
-  </si>
-  <si>
-    <t>For internal use</t>
-  </si>
-  <si>
-    <t>DE13270</t>
-  </si>
-  <si>
-    <t>[Android] Thermometer Pairing issues Android N</t>
-  </si>
-  <si>
-    <t>DE14423</t>
-  </si>
-  <si>
-    <t>[Android] Future timestamp is displayed during thermometer reading sync</t>
-  </si>
-  <si>
-    <t>DE14608</t>
-  </si>
-  <si>
-    <t>[Android] BlueLib doesn't build on a clean development environment</t>
-  </si>
-  <si>
-    <t>DE14613</t>
-  </si>
-  <si>
-    <t>Bug 43674: [Android] Crash observed when syncing continously</t>
-  </si>
-  <si>
-    <t>DE14614</t>
-  </si>
-  <si>
-    <t>[Android] DiCommChannel is not resilient against leading garbage</t>
-  </si>
-  <si>
-    <t>DE14615</t>
-  </si>
-  <si>
-    <t>[Android] NullPointerException in BlueLib using example App</t>
-  </si>
-  <si>
-    <t>DE14616</t>
-  </si>
-  <si>
-    <t>[Android] IndexOutOfBoundsException</t>
-  </si>
-  <si>
-    <t>DE14617</t>
-  </si>
-  <si>
-    <t>[Android] NPE when calling readRssi()</t>
-  </si>
-  <si>
-    <t>DE14618</t>
-  </si>
-  <si>
-    <t>[Android] Reconnect fails with Nexus 5, 4.4.2</t>
-  </si>
-  <si>
-    <t>DE14620</t>
-  </si>
-  <si>
-    <t>[Android] SHNDeviceImpl should actively disconnect when not all expected services are discovered</t>
-  </si>
-  <si>
-    <t>DE14677</t>
-  </si>
-  <si>
-    <t>[Android] App crashes on launch of the application</t>
-  </si>
-  <si>
-    <t>DE15010</t>
-  </si>
-  <si>
-    <t>TFS-49782 [Android] App Crashes on launch after the app upgrade</t>
-  </si>
-  <si>
-    <t>DE15038</t>
-  </si>
-  <si>
-    <t>[Android] TFS-40215:After Unpairing Moonshine and Pairing it back to same User is failing.</t>
-  </si>
-  <si>
-    <t>2017-FEB-28</t>
-  </si>
-  <si>
-    <t>2.3.2 Release</t>
   </si>
 </sst>
 </file>
@@ -2596,16 +2590,16 @@
     </row>
     <row r="8" spans="1:7" ht="48" x14ac:dyDescent="0.2">
       <c r="B8" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="34" t="s">
         <v>96</v>
-      </c>
-      <c r="C8" s="34" t="s">
-        <v>97</v>
       </c>
       <c r="D8" s="90" t="s">
         <v>20</v>
       </c>
       <c r="E8" s="89" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F8" s="22"/>
       <c r="G8" s="23"/>
@@ -2649,7 +2643,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="62" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2657,7 +2651,7 @@
         <v>13</v>
       </c>
       <c r="C13" s="62" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D13" s="98" t="s">
         <v>44</v>
@@ -2683,7 +2677,7 @@
         <v>18</v>
       </c>
       <c r="G14" s="29" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2691,7 +2685,7 @@
         <v>15</v>
       </c>
       <c r="C15" s="62" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>34</v>
@@ -3241,13 +3235,13 @@
         <v>89</v>
       </c>
       <c r="C13" s="87" t="s">
+        <v>91</v>
+      </c>
+      <c r="D13" s="87" t="s">
         <v>92</v>
       </c>
-      <c r="D13" s="87" t="s">
+      <c r="E13" s="88" t="s">
         <v>93</v>
-      </c>
-      <c r="E13" s="88" t="s">
-        <v>94</v>
       </c>
       <c r="F13" s="87" t="s">
         <v>87</v>
@@ -3266,7 +3260,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="87" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D14" s="87" t="s">
         <v>82</v>
@@ -3275,7 +3269,7 @@
         <v>84</v>
       </c>
       <c r="F14" s="87" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G14" s="17"/>
       <c r="H14" s="17"/>
@@ -6113,8 +6107,8 @@
   </sheetPr>
   <dimension ref="B1:D11"/>
   <sheetViews>
-    <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScaleSheetLayoutView="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -6865,7 +6859,7 @@
         <v>56</v>
       </c>
       <c r="C7" s="81">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D7" s="38"/>
     </row>
@@ -6894,7 +6888,7 @@
     </row>
     <row r="11" spans="2:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B11" s="39" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="C11"/>
       <c r="D11"/>
@@ -6927,8 +6921,8 @@
   </sheetPr>
   <dimension ref="B1:AH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView view="pageLayout" zoomScale="140" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -7663,10 +7657,10 @@
     </row>
     <row r="4" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B4" s="91" t="s">
+        <v>98</v>
+      </c>
+      <c r="C4" s="92" t="s">
         <v>99</v>
-      </c>
-      <c r="C4" s="92" t="s">
-        <v>100</v>
       </c>
       <c r="D4" s="95" t="s">
         <v>56</v>
@@ -7679,14 +7673,12 @@
     </row>
     <row r="5" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B5" s="91" t="s">
+        <v>100</v>
+      </c>
+      <c r="C5" s="92" t="s">
         <v>101</v>
       </c>
-      <c r="C5" s="92" t="s">
-        <v>102</v>
-      </c>
-      <c r="D5" s="95" t="s">
-        <v>56</v>
-      </c>
+      <c r="D5" s="94"/>
       <c r="AD5" s="35"/>
       <c r="AE5" s="35"/>
       <c r="AF5" s="35"/>
@@ -7695,10 +7687,10 @@
     </row>
     <row r="6" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B6" s="91" t="s">
+        <v>102</v>
+      </c>
+      <c r="C6" s="92" t="s">
         <v>103</v>
-      </c>
-      <c r="C6" s="92" t="s">
-        <v>104</v>
       </c>
       <c r="D6" s="94"/>
       <c r="AD6" s="35"/>
@@ -7709,10 +7701,10 @@
     </row>
     <row r="7" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B7" s="91" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="92" t="s">
         <v>105</v>
-      </c>
-      <c r="C7" s="92" t="s">
-        <v>106</v>
       </c>
       <c r="D7" s="94"/>
       <c r="AD7" s="35"/>
@@ -7723,12 +7715,12 @@
     </row>
     <row r="8" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B8" s="91" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="92" t="s">
         <v>107</v>
       </c>
-      <c r="C8" s="92" t="s">
-        <v>108</v>
-      </c>
-      <c r="D8" s="94"/>
+      <c r="D8" s="93"/>
       <c r="AD8" s="35"/>
       <c r="AE8" s="35"/>
       <c r="AF8" s="35"/>
@@ -7737,10 +7729,10 @@
     </row>
     <row r="9" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B9" s="91" t="s">
+        <v>108</v>
+      </c>
+      <c r="C9" s="92" t="s">
         <v>109</v>
-      </c>
-      <c r="C9" s="92" t="s">
-        <v>110</v>
       </c>
       <c r="D9" s="93"/>
       <c r="AD9" s="35"/>
@@ -7751,10 +7743,10 @@
     </row>
     <row r="10" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B10" s="91" t="s">
+        <v>110</v>
+      </c>
+      <c r="C10" s="92" t="s">
         <v>111</v>
-      </c>
-      <c r="C10" s="92" t="s">
-        <v>112</v>
       </c>
       <c r="D10" s="93"/>
       <c r="AD10" s="35"/>
@@ -7765,10 +7757,10 @@
     </row>
     <row r="11" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B11" s="91" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="92" t="s">
         <v>113</v>
-      </c>
-      <c r="C11" s="92" t="s">
-        <v>114</v>
       </c>
       <c r="D11" s="93"/>
       <c r="AD11" s="35"/>
@@ -7777,52 +7769,43 @@
       <c r="AG11" s="35"/>
       <c r="AH11" s="35"/>
     </row>
-    <row r="12" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:34" ht="32" x14ac:dyDescent="0.2">
       <c r="B12" s="91" t="s">
+        <v>114</v>
+      </c>
+      <c r="C12" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="C12" s="92" t="s">
+      <c r="D12" s="93"/>
+    </row>
+    <row r="13" spans="2:34" ht="16" x14ac:dyDescent="0.2">
+      <c r="B13" s="91" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="93"/>
-    </row>
-    <row r="13" spans="2:34" ht="32" x14ac:dyDescent="0.2">
-      <c r="B13" s="91" t="s">
+      <c r="C13" s="92" t="s">
         <v>117</v>
       </c>
-      <c r="C13" s="92" t="s">
-        <v>118</v>
-      </c>
-      <c r="D13" s="93"/>
+      <c r="D13" s="95" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="2:34" ht="16" x14ac:dyDescent="0.2">
       <c r="B14" s="91" t="s">
+        <v>118</v>
+      </c>
+      <c r="C14" s="92" t="s">
         <v>119</v>
       </c>
-      <c r="C14" s="92" t="s">
+      <c r="D14" s="93"/>
+    </row>
+    <row r="15" spans="2:34" ht="32" x14ac:dyDescent="0.2">
+      <c r="B15" s="91" t="s">
         <v>120</v>
       </c>
-      <c r="D14" s="95" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="2:34" ht="16" x14ac:dyDescent="0.2">
-      <c r="B15" s="91" t="s">
+      <c r="C15" s="92" t="s">
         <v>121</v>
       </c>
-      <c r="C15" s="92" t="s">
-        <v>122</v>
-      </c>
       <c r="D15" s="93"/>
-    </row>
-    <row r="16" spans="2:34" ht="32" x14ac:dyDescent="0.2">
-      <c r="B16" s="91" t="s">
-        <v>123</v>
-      </c>
-      <c r="C16" s="92" t="s">
-        <v>124</v>
-      </c>
-      <c r="D16" s="93"/>
     </row>
     <row r="19" spans="2:4" ht="14" x14ac:dyDescent="0.15">
       <c r="B19" s="49"/>

</xml_diff>